<commit_message>
Updated to average price
</commit_message>
<xml_diff>
--- a/data/case study data.xlsx
+++ b/data/case study data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10708"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fernaag/Library/CloudStorage/Box-Box/MIT/generalization/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C4F584D-5EA0-1848-A3FD-774D76359D94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF6AFD7E-4A30-6941-9A38-D7BF791A9CC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{9C1DBEC5-9C42-494B-AEAA-1D89B674AD0D}"/>
   </bookViews>
@@ -1764,7 +1764,7 @@
   <dimension ref="A1:AK74"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="R39" sqref="R39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4950,8 +4950,8 @@
         <v>5.6010000000000001E-3</v>
       </c>
       <c r="Q38" s="18"/>
-      <c r="R38" s="6">
-        <v>1.1629945427094399</v>
+      <c r="R38" s="49">
+        <v>5.5303602419031304</v>
       </c>
       <c r="S38" s="6" t="s">
         <v>34</v>
@@ -5038,7 +5038,7 @@
       </c>
       <c r="Q39" s="20"/>
       <c r="R39" s="8">
-        <v>0.54876084489486399</v>
+        <v>2.37751350500784</v>
       </c>
       <c r="S39" s="8" t="s">
         <v>34</v>
@@ -5126,7 +5126,7 @@
       </c>
       <c r="Q40" s="18"/>
       <c r="R40" s="49">
-        <v>1.1629945427094399</v>
+        <v>0.98090753516626605</v>
       </c>
       <c r="S40" s="6" t="s">
         <v>34</v>
@@ -5212,7 +5212,7 @@
         <v>0.119309</v>
       </c>
       <c r="R41" s="49">
-        <v>0.54876084489486399</v>
+        <v>0.34055052130256103</v>
       </c>
       <c r="S41" s="8" t="s">
         <v>34</v>
@@ -7093,7 +7093,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7180,7 +7180,7 @@
         <v>70</v>
       </c>
       <c r="D5" s="5">
-        <v>2096.3778424944198</v>
+        <v>1991.2932632688505</v>
       </c>
       <c r="E5" s="5">
         <v>76.145567</v>
@@ -7198,7 +7198,7 @@
         <v>78.5</v>
       </c>
       <c r="D6" s="5">
-        <v>2375.8771057128938</v>
+        <v>2130.5714445568283</v>
       </c>
       <c r="E6" s="5">
         <v>85.971186000000003</v>
@@ -7216,7 +7216,7 @@
         <v>90</v>
       </c>
       <c r="D7" s="5">
-        <v>3256.0443542480489</v>
+        <v>2576.0997674851205</v>
       </c>
       <c r="E7" s="5">
         <v>96.04539299999999</v>
@@ -7234,7 +7234,7 @@
         <v>80</v>
       </c>
       <c r="D8" s="5">
-        <v>4287.9830078124996</v>
+        <v>3306.6348225911474</v>
       </c>
       <c r="E8" s="5">
         <v>105.140455</v>
@@ -7252,7 +7252,7 @@
         <v>86.6</v>
       </c>
       <c r="D9" s="5">
-        <v>6010.4877522786455</v>
+        <v>4518.171704779732</v>
       </c>
       <c r="E9" s="5">
         <v>121.12909199999999</v>
@@ -7270,7 +7270,7 @@
         <v>112.8</v>
       </c>
       <c r="D10" s="5">
-        <v>6046.8367309570312</v>
+        <v>5448.4358303493918</v>
       </c>
       <c r="E10" s="5">
         <v>125.57747800000001</v>
@@ -7288,7 +7288,7 @@
         <v>95</v>
       </c>
       <c r="D11" s="5">
-        <v>5452.4385986328125</v>
+        <v>5836.5876939561631</v>
       </c>
       <c r="E11" s="5">
         <v>99.382306999999997</v>
@@ -7306,7 +7306,7 @@
         <v>125</v>
       </c>
       <c r="D12" s="5">
-        <v>4979.4941030649043</v>
+        <v>5492.9231442182499</v>
       </c>
       <c r="E12" s="5">
         <v>143.25536400000001</v>
@@ -7324,7 +7324,7 @@
         <v>122.429</v>
       </c>
       <c r="D13" s="5">
-        <v>4948.2326096754823</v>
+        <v>5126.7217704577333</v>
       </c>
       <c r="E13" s="5">
         <v>177.108566</v>
@@ -7342,7 +7342,7 @@
         <v>150.1086</v>
       </c>
       <c r="D14" s="5">
-        <v>5233.7805350167409</v>
+        <v>5053.8357492523764</v>
       </c>
       <c r="E14" s="5">
         <v>183.31275300000004</v>
@@ -7360,7 +7360,7 @@
         <v>159.69</v>
       </c>
       <c r="D15" s="5">
-        <v>5540.7611607142853</v>
+        <v>5240.9247684688362</v>
       </c>
       <c r="E15" s="5">
         <v>172.04403400000001</v>
@@ -7378,7 +7378,7 @@
         <v>165</v>
       </c>
       <c r="D16" s="5">
-        <v>5611.9737025669647</v>
+        <v>5462.1717994326636</v>
       </c>
       <c r="E16" s="5">
         <v>186.019372</v>
@@ -7396,7 +7396,7 @@
         <v>194</v>
       </c>
       <c r="D17" s="5">
-        <v>6032.6183919270834</v>
+        <v>5728.4510850694451</v>
       </c>
       <c r="E17" s="5">
         <v>201.32204200000001</v>
@@ -7414,7 +7414,7 @@
         <v>195.35410000000002</v>
       </c>
       <c r="D18" s="5">
-        <v>10903.384212239584</v>
+        <v>7515.9921022445442</v>
       </c>
       <c r="E18" s="5">
         <v>246.11897900000002</v>
@@ -7432,7 +7432,7 @@
         <v>211.32310000000004</v>
       </c>
       <c r="D19" s="5">
-        <v>14657.141308593749</v>
+        <v>10531.047970920139</v>
       </c>
       <c r="E19" s="5">
         <v>312.55251800000002</v>
@@ -7450,7 +7450,7 @@
         <v>253.37480000000002</v>
       </c>
       <c r="D20" s="5">
-        <v>15786.893098958333</v>
+        <v>13782.472873263891</v>
       </c>
       <c r="E20" s="5">
         <v>361.04267200000004</v>
@@ -7468,7 +7468,7 @@
         <v>298.08800000000002</v>
       </c>
       <c r="D21" s="5">
-        <v>11120.835754394531</v>
+        <v>13854.956720648872</v>
       </c>
       <c r="E21" s="5">
         <v>439.40106200000008</v>

</xml_diff>

<commit_message>
added new column in 'Au' sheet
added new column in 'Au' sheet for gold commodity price adjusted for inflation
</commit_message>
<xml_diff>
--- a/data/case study data.xlsx
+++ b/data/case study data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michelenaorourke/Documents/GitHub/generalization/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FE7A14E-7784-A44D-9855-EE845BF733A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD5EE754-DD6D-BB4A-9521-5F38DB899503}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4040" yWindow="460" windowWidth="19680" windowHeight="16580" activeTab="3" xr2:uid="{9C1DBEC5-9C42-494B-AEAA-1D89B674AD0D}"/>
+    <workbookView xWindow="5100" yWindow="460" windowWidth="19680" windowHeight="16580" activeTab="3" xr2:uid="{9C1DBEC5-9C42-494B-AEAA-1D89B674AD0D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="17" r:id="rId1"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="357">
   <si>
     <t>Al</t>
   </si>
@@ -1151,6 +1151,9 @@
   </si>
   <si>
     <t>C:\Users\ryter\Dropbox (MIT)\Group Research Folder_Olivetti\Displacement\00 Simulation\05 Data Compile\Metalor and other, iron ore and precious metals, daily.xls   // oil price adjusted for 2002-2018 // assumed 2001 48 dollar decrease // assumed 2019 had 18% increase based on Macrotrends Hundred Year Price Chart</t>
+  </si>
+  <si>
+    <t>Primary commodity price old</t>
   </si>
 </sst>
 </file>
@@ -1161,7 +1164,7 @@
     <numFmt numFmtId="164" formatCode="\Te"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1230,6 +1233,13 @@
       <name val="Courier New"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1273,7 +1283,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1345,6 +1355,7 @@
     </xf>
     <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -8396,10 +8407,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63DF787E-9CE6-4767-AADB-C0D49F24A7F3}">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8408,12 +8419,12 @@
     <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>190</v>
       </c>
       <c r="C1" t="s">
-        <v>194</v>
+        <v>356</v>
       </c>
       <c r="D1" t="s">
         <v>197</v>
@@ -8427,8 +8438,11 @@
       <c r="G1" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="M1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>182</v>
       </c>
@@ -8442,8 +8456,9 @@
         <v>209</v>
       </c>
       <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="M2" s="43"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2001</v>
       </c>
@@ -8458,8 +8473,11 @@
       <c r="D3">
         <v>2.56</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="M3">
+        <v>384.62169599999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2002</v>
       </c>
@@ -8473,8 +8491,11 @@
       <c r="D4">
         <v>2.5499999999999998</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="M4" s="43">
+        <v>432.68009999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2003</v>
       </c>
@@ -8487,8 +8508,11 @@
       <c r="D5">
         <v>2.54</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="M5" s="43">
+        <v>496.37599999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2004</v>
       </c>
@@ -8501,8 +8525,11 @@
       <c r="D6">
         <v>2.42</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="M6" s="43">
+        <v>543.46299999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2005</v>
       </c>
@@ -8515,8 +8542,11 @@
       <c r="D7">
         <v>2.48</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="M7" s="43">
+        <v>571.63080000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2006</v>
       </c>
@@ -8529,8 +8559,11 @@
       <c r="D8">
         <v>2.37</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="M8" s="43">
+        <v>752.69680000000005</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2007</v>
       </c>
@@ -8543,8 +8576,11 @@
       <c r="D9">
         <v>2.35</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="M9" s="43">
+        <v>842.58109999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="19" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2008</v>
       </c>
@@ -8558,8 +8594,11 @@
         <v>2.2799999999999998</v>
       </c>
       <c r="H10" s="41"/>
-    </row>
-    <row r="11" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="M10" s="43">
+        <v>1017.696</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="19" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2009</v>
       </c>
@@ -8573,8 +8612,11 @@
         <v>2.46</v>
       </c>
       <c r="H11" s="41"/>
-    </row>
-    <row r="12" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="M11" s="43">
+        <v>1136.8019999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="19" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2010</v>
       </c>
@@ -8588,8 +8630,11 @@
         <v>2.7545000000000002</v>
       </c>
       <c r="H12" s="41"/>
-    </row>
-    <row r="13" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="M12" s="43">
+        <v>1410.712</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="19" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2011</v>
       </c>
@@ -8603,8 +8648,11 @@
         <v>2.8769</v>
       </c>
       <c r="H13" s="41"/>
-    </row>
-    <row r="14" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="M13" s="43">
+        <v>1755.4659999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="19" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2012</v>
       </c>
@@ -8618,8 +8666,11 @@
         <v>2.9571999999999998</v>
       </c>
       <c r="H14" s="41"/>
-    </row>
-    <row r="15" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="M14" s="43">
+        <v>1824.9770000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="19" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2013</v>
       </c>
@@ -8633,8 +8684,11 @@
         <v>3.1667999999999998</v>
       </c>
       <c r="H15" s="41"/>
-    </row>
-    <row r="16" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="M15" s="43">
+        <v>1520.327</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="19" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2014</v>
       </c>
@@ -8648,8 +8702,11 @@
         <v>3.2705000000000002</v>
       </c>
       <c r="H16" s="41"/>
-    </row>
-    <row r="17" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="M16" s="43">
+        <v>1343.3530000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="19" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2015</v>
       </c>
@@ -8663,8 +8720,11 @@
         <v>3.3662999999999998</v>
       </c>
       <c r="H17" s="41"/>
-    </row>
-    <row r="18" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="M17" s="43">
+        <v>1227.7149999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="19" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2016</v>
       </c>
@@ -8678,8 +8738,11 @@
         <v>3.5173000000000001</v>
       </c>
       <c r="H18" s="41"/>
-    </row>
-    <row r="19" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="M18" s="43">
+        <v>1307.6379999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="19" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2017</v>
       </c>
@@ -8693,8 +8756,11 @@
         <v>3.5678000000000001</v>
       </c>
       <c r="H19" s="41"/>
-    </row>
-    <row r="20" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="M19" s="43">
+        <v>1288.577</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="19" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2018</v>
       </c>
@@ -8708,8 +8774,11 @@
         <v>3.6536</v>
       </c>
       <c r="H20" s="41"/>
-    </row>
-    <row r="21" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="M20" s="43">
+        <v>1272.7950000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="19" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2019</v>
       </c>
@@ -8723,17 +8792,21 @@
         <v>3.5962000000000001</v>
       </c>
       <c r="H21" s="41"/>
-    </row>
-    <row r="22" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="M21">
+        <f>M20+(M20*0.18)</f>
+        <v>1501.8981000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="19" x14ac:dyDescent="0.25">
       <c r="H22" s="41"/>
     </row>
-    <row r="23" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="19" x14ac:dyDescent="0.25">
       <c r="H23" s="41"/>
     </row>
-    <row r="24" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="19" x14ac:dyDescent="0.25">
       <c r="H24" s="41"/>
     </row>
-    <row r="25" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" ht="19" x14ac:dyDescent="0.25">
       <c r="H25" s="41"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed the au sheet
put the inflation adjusted gold data back in column c because it was giving me issues
</commit_message>
<xml_diff>
--- a/data/case study data.xlsx
+++ b/data/case study data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michelenaorourke/Documents/GitHub/generalization/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD5EE754-DD6D-BB4A-9521-5F38DB899503}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{353480AF-E267-5649-ADCC-853251F113B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5100" yWindow="460" windowWidth="19680" windowHeight="16580" activeTab="3" xr2:uid="{9C1DBEC5-9C42-494B-AEAA-1D89B674AD0D}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15860" activeTab="3" xr2:uid="{9C1DBEC5-9C42-494B-AEAA-1D89B674AD0D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="17" r:id="rId1"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="358">
   <si>
     <t>Al</t>
   </si>
@@ -1154,6 +1154,9 @@
   </si>
   <si>
     <t>Primary commodity price old</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Primary commodity price </t>
   </si>
 </sst>
 </file>
@@ -1283,7 +1286,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1354,7 +1357,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
@@ -8407,10 +8409,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63DF787E-9CE6-4767-AADB-C0D49F24A7F3}">
-  <dimension ref="A1:M25"/>
+  <dimension ref="A1:Q25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8419,12 +8421,12 @@
     <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>190</v>
       </c>
       <c r="C1" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="D1" t="s">
         <v>197</v>
@@ -8441,8 +8443,11 @@
       <c r="M1" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="Q1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>182</v>
       </c>
@@ -8456,9 +8461,12 @@
         <v>209</v>
       </c>
       <c r="F2" s="1"/>
-      <c r="M2" s="43"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M2" s="42"/>
+      <c r="Q2" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2001</v>
       </c>
@@ -8466,9 +8474,8 @@
         <f>B4*D3/D4</f>
         <v>2.6211738386810759</v>
       </c>
-      <c r="C3" s="42">
-        <f>(C4-48*35274)</f>
-        <v>11873993.704704</v>
+      <c r="C3">
+        <v>384.62169599999999</v>
       </c>
       <c r="D3">
         <v>2.56</v>
@@ -8476,8 +8483,11 @@
       <c r="M3">
         <v>384.62169599999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="Q3">
+        <v>11873993.704704</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2002</v>
       </c>
@@ -8486,16 +8496,19 @@
         <v>2.6109348783737278</v>
       </c>
       <c r="C4" s="42">
-        <v>13567145.704704</v>
+        <v>432.68009999999998</v>
       </c>
       <c r="D4">
         <v>2.5499999999999998</v>
       </c>
-      <c r="M4" s="43">
+      <c r="M4" s="42">
         <v>432.68009999999998</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="Q4">
+        <v>13567145.704704</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2003</v>
       </c>
@@ -8503,16 +8516,19 @@
         <v>2.6006959180663798</v>
       </c>
       <c r="C5" s="42">
-        <v>15252034.346915999</v>
+        <v>496.37599999999998</v>
       </c>
       <c r="D5">
         <v>2.54</v>
       </c>
-      <c r="M5" s="43">
+      <c r="M5" s="42">
         <v>496.37599999999998</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="Q5">
+        <v>15252034.346915999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2004</v>
       </c>
@@ -8520,16 +8536,19 @@
         <v>3.0508626846620399</v>
       </c>
       <c r="C6" s="42">
-        <v>15749019.786006</v>
+        <v>543.46299999999997</v>
       </c>
       <c r="D6">
         <v>2.42</v>
       </c>
-      <c r="M6" s="43">
+      <c r="M6" s="42">
         <v>543.46299999999997</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="Q6">
+        <v>15749019.786006</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2005</v>
       </c>
@@ -8537,16 +8556,19 @@
         <v>3.1113771591266901</v>
       </c>
       <c r="C7" s="42">
-        <v>15122391.179784</v>
+        <v>571.63080000000002</v>
       </c>
       <c r="D7">
         <v>2.48</v>
       </c>
-      <c r="M7" s="43">
+      <c r="M7" s="42">
         <v>571.63080000000002</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="Q7">
+        <v>15122391.179784</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2006</v>
       </c>
@@ -8554,16 +8576,19 @@
         <v>3.09207937561865</v>
       </c>
       <c r="C8" s="42">
-        <v>20608702.998528</v>
+        <v>752.69680000000005</v>
       </c>
       <c r="D8">
         <v>2.37</v>
       </c>
-      <c r="M8" s="43">
+      <c r="M8" s="42">
         <v>752.69680000000005</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="Q8">
+        <v>20608702.998528</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2007</v>
       </c>
@@ -8571,16 +8596,19 @@
         <v>3.1150351404490899</v>
       </c>
       <c r="C9" s="42">
-        <v>23289317.400419999</v>
+        <v>842.58109999999999</v>
       </c>
       <c r="D9">
         <v>2.35</v>
       </c>
-      <c r="M9" s="43">
+      <c r="M9" s="42">
         <v>842.58109999999999</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" ht="19" x14ac:dyDescent="0.25">
+      <c r="Q9">
+        <v>23289317.400419999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2008</v>
       </c>
@@ -8588,17 +8616,20 @@
         <v>3.7342289806146298</v>
       </c>
       <c r="C10" s="42">
-        <v>26830921.217274003</v>
+        <v>1017.696</v>
       </c>
       <c r="D10">
         <v>2.2799999999999998</v>
       </c>
       <c r="H10" s="41"/>
-      <c r="M10" s="43">
+      <c r="M10" s="42">
         <v>1017.696</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" ht="19" x14ac:dyDescent="0.25">
+      <c r="Q10">
+        <v>26830921.217274003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2009</v>
       </c>
@@ -8606,17 +8637,20 @@
         <v>3.6116350854505699</v>
       </c>
       <c r="C11" s="42">
-        <v>35094737.355630003</v>
+        <v>1136.8019999999999</v>
       </c>
       <c r="D11">
         <v>2.46</v>
       </c>
       <c r="H11" s="41"/>
-      <c r="M11" s="43">
+      <c r="M11" s="42">
         <v>1136.8019999999999</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" ht="19" x14ac:dyDescent="0.25">
+      <c r="Q11">
+        <v>35094737.355630003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2010</v>
       </c>
@@ -8624,17 +8658,20 @@
         <v>4.1711999999999998</v>
       </c>
       <c r="C12" s="42">
-        <v>42975239.260650001</v>
+        <v>1410.712</v>
       </c>
       <c r="D12">
         <v>2.7545000000000002</v>
       </c>
       <c r="H12" s="41"/>
-      <c r="M12" s="43">
+      <c r="M12" s="42">
         <v>1410.712</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" ht="19" x14ac:dyDescent="0.25">
+      <c r="Q12">
+        <v>42975239.260650001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2011</v>
       </c>
@@ -8642,17 +8679,20 @@
         <v>4.7247000000000003</v>
       </c>
       <c r="C13" s="42">
-        <v>53778977.547102004</v>
+        <v>1755.4659999999999</v>
       </c>
       <c r="D13">
         <v>2.8769</v>
       </c>
       <c r="H13" s="41"/>
-      <c r="M13" s="43">
+      <c r="M13" s="42">
         <v>1755.4659999999999</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" ht="19" x14ac:dyDescent="0.25">
+      <c r="Q13">
+        <v>53778977.547102004</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2012</v>
       </c>
@@ -8660,17 +8700,20 @@
         <v>4.6726999999999999</v>
       </c>
       <c r="C14" s="42">
-        <v>56518569.477336004</v>
+        <v>1824.9770000000001</v>
       </c>
       <c r="D14">
         <v>2.9571999999999998</v>
       </c>
       <c r="H14" s="41"/>
-      <c r="M14" s="43">
+      <c r="M14" s="42">
         <v>1824.9770000000001</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" ht="19" x14ac:dyDescent="0.25">
+      <c r="Q14">
+        <v>56518569.477336004</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2013</v>
       </c>
@@ -8678,17 +8721,20 @@
         <v>4.5137</v>
       </c>
       <c r="C15" s="42">
-        <v>45537007.619892001</v>
+        <v>1520.327</v>
       </c>
       <c r="D15">
         <v>3.1667999999999998</v>
       </c>
       <c r="H15" s="41"/>
-      <c r="M15" s="43">
+      <c r="M15" s="42">
         <v>1520.327</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" ht="19" x14ac:dyDescent="0.25">
+      <c r="Q15">
+        <v>45537007.619892001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2014</v>
       </c>
@@ -8696,17 +8742,20 @@
         <v>4.4260999999999999</v>
       </c>
       <c r="C16" s="42">
-        <v>39909789.610542007</v>
+        <v>1343.3530000000001</v>
       </c>
       <c r="D16">
         <v>3.2705000000000002</v>
       </c>
       <c r="H16" s="41"/>
-      <c r="M16" s="43">
+      <c r="M16" s="42">
         <v>1343.3530000000001</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" ht="19" x14ac:dyDescent="0.25">
+      <c r="Q16">
+        <v>39909789.610542007</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2015</v>
       </c>
@@ -8714,17 +8763,20 @@
         <v>4.3685</v>
       </c>
       <c r="C17" s="42">
-        <v>40209714.238356002</v>
+        <v>1227.7149999999999</v>
       </c>
       <c r="D17">
         <v>3.3662999999999998</v>
       </c>
       <c r="H17" s="41"/>
-      <c r="M17" s="43">
+      <c r="M17" s="42">
         <v>1227.7149999999999</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" ht="19" x14ac:dyDescent="0.25">
+      <c r="Q17">
+        <v>40209714.238356002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2016</v>
       </c>
@@ -8732,17 +8784,20 @@
         <v>4.3914</v>
       </c>
       <c r="C18" s="42">
-        <v>43624963.306727998</v>
+        <v>1307.6379999999999</v>
       </c>
       <c r="D18">
         <v>3.5173000000000001</v>
       </c>
       <c r="H18" s="41"/>
-      <c r="M18" s="43">
+      <c r="M18" s="42">
         <v>1307.6379999999999</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" ht="19" x14ac:dyDescent="0.25">
+      <c r="Q18">
+        <v>43624963.306727998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2017</v>
       </c>
@@ -8750,17 +8805,20 @@
         <v>4.2782999999999998</v>
       </c>
       <c r="C19" s="42">
-        <v>42306183.016679995</v>
+        <v>1288.577</v>
       </c>
       <c r="D19">
         <v>3.5678000000000001</v>
       </c>
       <c r="H19" s="41"/>
-      <c r="M19" s="43">
+      <c r="M19" s="42">
         <v>1288.577</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" ht="19" x14ac:dyDescent="0.25">
+      <c r="Q19">
+        <v>42306183.016679995</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2018</v>
       </c>
@@ -8768,25 +8826,29 @@
         <v>4.4542999999999999</v>
       </c>
       <c r="C20" s="42">
-        <v>40434691.598711997</v>
+        <v>1272.7950000000001</v>
       </c>
       <c r="D20">
         <v>3.6536</v>
       </c>
       <c r="H20" s="41"/>
-      <c r="M20" s="43">
+      <c r="M20" s="42">
         <v>1272.7950000000001</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" ht="19" x14ac:dyDescent="0.25">
+      <c r="Q20">
+        <v>40434691.598711997</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2019</v>
       </c>
       <c r="B21">
         <v>4.3593999999999999</v>
       </c>
-      <c r="C21" s="42">
-        <v>47712936.086480156</v>
+      <c r="C21">
+        <f>C20+(C20*0.18)</f>
+        <v>1501.8981000000001</v>
       </c>
       <c r="D21">
         <v>3.5962000000000001</v>
@@ -8796,17 +8858,20 @@
         <f>M20+(M20*0.18)</f>
         <v>1501.8981000000001</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" ht="19" x14ac:dyDescent="0.25">
+      <c r="Q21">
+        <v>47712936.086480156</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="H22" s="41"/>
     </row>
-    <row r="23" spans="1:13" ht="19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="H23" s="41"/>
     </row>
-    <row r="24" spans="1:13" ht="19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="H24" s="41"/>
     </row>
-    <row r="25" spans="1:13" ht="19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="H25" s="41"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dollars per oz to dollars per ton
</commit_message>
<xml_diff>
--- a/data/case study data.xlsx
+++ b/data/case study data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michelenaorourke/Documents/GitHub/generalization/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E07B0BEB-B33E-F644-8F6C-195F13CCC193}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9661CA26-5B3F-3D4C-96E9-7E1F02622925}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15860" activeTab="3" xr2:uid="{9C1DBEC5-9C42-494B-AEAA-1D89B674AD0D}"/>
   </bookViews>
@@ -8409,7 +8409,7 @@
   <dimension ref="A1:Q25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8472,7 +8472,8 @@
         <v>2.6211738386810759</v>
       </c>
       <c r="C3">
-        <v>384.62169599999999</v>
+        <f>M3*35273</f>
+        <v>13566761.083007999</v>
       </c>
       <c r="D3">
         <v>2.56</v>
@@ -8492,8 +8493,9 @@
         <f>B5*D4/D5</f>
         <v>2.6109348783737278</v>
       </c>
-      <c r="C4" s="42">
-        <v>432.68009999999998</v>
+      <c r="C4">
+        <f t="shared" ref="C4:C21" si="0">M4*35273</f>
+        <v>15261925.167299999</v>
       </c>
       <c r="D4">
         <v>2.5499999999999998</v>
@@ -8512,8 +8514,9 @@
       <c r="B5">
         <v>2.6006959180663798</v>
       </c>
-      <c r="C5" s="42">
-        <v>496.37599999999998</v>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>17508670.647999998</v>
       </c>
       <c r="D5">
         <v>2.54</v>
@@ -8532,8 +8535,9 @@
       <c r="B6">
         <v>3.0508626846620399</v>
       </c>
-      <c r="C6" s="42">
-        <v>543.46299999999997</v>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>19169570.399</v>
       </c>
       <c r="D6">
         <v>2.42</v>
@@ -8552,8 +8556,9 @@
       <c r="B7">
         <v>3.1113771591266901</v>
       </c>
-      <c r="C7" s="42">
-        <v>571.63080000000002</v>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>20163133.2084</v>
       </c>
       <c r="D7">
         <v>2.48</v>
@@ -8572,8 +8577,9 @@
       <c r="B8">
         <v>3.09207937561865</v>
       </c>
-      <c r="C8" s="42">
-        <v>752.69680000000005</v>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>26549874.226400003</v>
       </c>
       <c r="D8">
         <v>2.37</v>
@@ -8592,8 +8598,9 @@
       <c r="B9">
         <v>3.1150351404490899</v>
       </c>
-      <c r="C9" s="42">
-        <v>842.58109999999999</v>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>29720363.140299998</v>
       </c>
       <c r="D9">
         <v>2.35</v>
@@ -8612,8 +8619,9 @@
       <c r="B10">
         <v>3.7342289806146298</v>
       </c>
-      <c r="C10" s="42">
-        <v>1017.696</v>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>35897191.008000001</v>
       </c>
       <c r="D10">
         <v>2.2799999999999998</v>
@@ -8633,8 +8641,9 @@
       <c r="B11">
         <v>3.6116350854505699</v>
       </c>
-      <c r="C11" s="42">
-        <v>1136.8019999999999</v>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>40098416.945999995</v>
       </c>
       <c r="D11">
         <v>2.46</v>
@@ -8654,8 +8663,9 @@
       <c r="B12">
         <v>4.1711999999999998</v>
       </c>
-      <c r="C12" s="42">
-        <v>1410.712</v>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>49760044.376000002</v>
       </c>
       <c r="D12">
         <v>2.7545000000000002</v>
@@ -8675,8 +8685,9 @@
       <c r="B13">
         <v>4.7247000000000003</v>
       </c>
-      <c r="C13" s="42">
-        <v>1755.4659999999999</v>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>61920552.217999995</v>
       </c>
       <c r="D13">
         <v>2.8769</v>
@@ -8696,8 +8707,9 @@
       <c r="B14">
         <v>4.6726999999999999</v>
       </c>
-      <c r="C14" s="42">
-        <v>1824.9770000000001</v>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>64372413.721000001</v>
       </c>
       <c r="D14">
         <v>2.9571999999999998</v>
@@ -8717,8 +8729,9 @@
       <c r="B15">
         <v>4.5137</v>
       </c>
-      <c r="C15" s="42">
-        <v>1520.327</v>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>53626494.270999998</v>
       </c>
       <c r="D15">
         <v>3.1667999999999998</v>
@@ -8738,8 +8751,9 @@
       <c r="B16">
         <v>4.4260999999999999</v>
       </c>
-      <c r="C16" s="42">
-        <v>1343.3530000000001</v>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>47384090.369000003</v>
       </c>
       <c r="D16">
         <v>3.2705000000000002</v>
@@ -8759,8 +8773,9 @@
       <c r="B17">
         <v>4.3685</v>
       </c>
-      <c r="C17" s="42">
-        <v>1227.7149999999999</v>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>43305191.195</v>
       </c>
       <c r="D17">
         <v>3.3662999999999998</v>
@@ -8780,8 +8795,9 @@
       <c r="B18">
         <v>4.3914</v>
       </c>
-      <c r="C18" s="42">
-        <v>1307.6379999999999</v>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>46124315.173999995</v>
       </c>
       <c r="D18">
         <v>3.5173000000000001</v>
@@ -8801,8 +8817,9 @@
       <c r="B19">
         <v>4.2782999999999998</v>
       </c>
-      <c r="C19" s="42">
-        <v>1288.577</v>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>45451976.520999998</v>
       </c>
       <c r="D19">
         <v>3.5678000000000001</v>
@@ -8822,8 +8839,9 @@
       <c r="B20">
         <v>4.4542999999999999</v>
       </c>
-      <c r="C20" s="42">
-        <v>1272.7950000000001</v>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>44895298.035000004</v>
       </c>
       <c r="D20">
         <v>3.6536</v>
@@ -8844,8 +8862,8 @@
         <v>4.3593999999999999</v>
       </c>
       <c r="C21">
-        <f>C20+(C20*0.18)</f>
-        <v>1501.8981000000001</v>
+        <f t="shared" si="0"/>
+        <v>52976451.681300007</v>
       </c>
       <c r="D21">
         <v>3.5962000000000001</v>

</xml_diff>

<commit_message>
Modified demand class so that it takes my model inputs for the case of Li. Also added demand files if interesting for other materials
</commit_message>
<xml_diff>
--- a/data/case study data.xlsx
+++ b/data/case study data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10708"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fernaag/Library/CloudStorage/Box-Box/MIT/generalization/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF6AFD7E-4A30-6941-9A38-D7BF791A9CC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C9536BE-3C16-C849-A55B-3BF010956E1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{9C1DBEC5-9C42-494B-AEAA-1D89B674AD0D}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="15" xr2:uid="{9C1DBEC5-9C42-494B-AEAA-1D89B674AD0D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="17" r:id="rId1"/>
@@ -1763,7 +1763,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AAEEA05-303F-4351-9872-7B8EAAB6CD92}">
   <dimension ref="A1:AK74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="R39" sqref="R39"/>
     </sheetView>
   </sheetViews>
@@ -7092,8 +7092,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAEAF772-8B76-4702-B768-A08EDD9553AC}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7180,7 +7180,7 @@
         <v>70</v>
       </c>
       <c r="D5" s="5">
-        <v>1991.2932632688505</v>
+        <v>2096.3778424944198</v>
       </c>
       <c r="E5" s="5">
         <v>76.145567</v>
@@ -7198,7 +7198,7 @@
         <v>78.5</v>
       </c>
       <c r="D6" s="5">
-        <v>2130.5714445568283</v>
+        <v>2375.8771057128938</v>
       </c>
       <c r="E6" s="5">
         <v>85.971186000000003</v>
@@ -7216,7 +7216,7 @@
         <v>90</v>
       </c>
       <c r="D7" s="5">
-        <v>2576.0997674851205</v>
+        <v>3256.0443542480489</v>
       </c>
       <c r="E7" s="5">
         <v>96.04539299999999</v>
@@ -7234,7 +7234,7 @@
         <v>80</v>
       </c>
       <c r="D8" s="5">
-        <v>3306.6348225911474</v>
+        <v>4287.9830078124996</v>
       </c>
       <c r="E8" s="5">
         <v>105.140455</v>
@@ -7252,7 +7252,7 @@
         <v>86.6</v>
       </c>
       <c r="D9" s="5">
-        <v>4518.171704779732</v>
+        <v>6010.4877522786455</v>
       </c>
       <c r="E9" s="5">
         <v>121.12909199999999</v>
@@ -7270,7 +7270,7 @@
         <v>112.8</v>
       </c>
       <c r="D10" s="5">
-        <v>5448.4358303493918</v>
+        <v>6046.8367309570312</v>
       </c>
       <c r="E10" s="5">
         <v>125.57747800000001</v>
@@ -7288,7 +7288,7 @@
         <v>95</v>
       </c>
       <c r="D11" s="5">
-        <v>5836.5876939561631</v>
+        <v>5452.4385986328125</v>
       </c>
       <c r="E11" s="5">
         <v>99.382306999999997</v>
@@ -7306,7 +7306,7 @@
         <v>125</v>
       </c>
       <c r="D12" s="5">
-        <v>5492.9231442182499</v>
+        <v>4979.4941030649043</v>
       </c>
       <c r="E12" s="5">
         <v>143.25536400000001</v>
@@ -7324,7 +7324,7 @@
         <v>122.429</v>
       </c>
       <c r="D13" s="5">
-        <v>5126.7217704577333</v>
+        <v>4948.2326096754823</v>
       </c>
       <c r="E13" s="5">
         <v>177.108566</v>
@@ -7342,7 +7342,7 @@
         <v>150.1086</v>
       </c>
       <c r="D14" s="5">
-        <v>5053.8357492523764</v>
+        <v>5233.7805350167409</v>
       </c>
       <c r="E14" s="5">
         <v>183.31275300000004</v>
@@ -7360,7 +7360,7 @@
         <v>159.69</v>
       </c>
       <c r="D15" s="5">
-        <v>5240.9247684688362</v>
+        <v>5540.7611607142853</v>
       </c>
       <c r="E15" s="5">
         <v>172.04403400000001</v>
@@ -7378,7 +7378,7 @@
         <v>165</v>
       </c>
       <c r="D16" s="5">
-        <v>5462.1717994326636</v>
+        <v>5611.9737025669647</v>
       </c>
       <c r="E16" s="5">
         <v>186.019372</v>
@@ -7396,7 +7396,7 @@
         <v>194</v>
       </c>
       <c r="D17" s="5">
-        <v>5728.4510850694451</v>
+        <v>6032.6183919270834</v>
       </c>
       <c r="E17" s="5">
         <v>201.32204200000001</v>
@@ -7414,7 +7414,7 @@
         <v>195.35410000000002</v>
       </c>
       <c r="D18" s="5">
-        <v>7515.9921022445442</v>
+        <v>10903.384212239584</v>
       </c>
       <c r="E18" s="5">
         <v>246.11897900000002</v>
@@ -7432,7 +7432,7 @@
         <v>211.32310000000004</v>
       </c>
       <c r="D19" s="5">
-        <v>10531.047970920139</v>
+        <v>14657.141308593749</v>
       </c>
       <c r="E19" s="5">
         <v>312.55251800000002</v>
@@ -7450,7 +7450,7 @@
         <v>253.37480000000002</v>
       </c>
       <c r="D20" s="5">
-        <v>13782.472873263891</v>
+        <v>15786.893098958333</v>
       </c>
       <c r="E20" s="5">
         <v>361.04267200000004</v>
@@ -7468,7 +7468,7 @@
         <v>298.08800000000002</v>
       </c>
       <c r="D21" s="5">
-        <v>13854.956720648872</v>
+        <v>11120.835754394531</v>
       </c>
       <c r="E21" s="5">
         <v>439.40106200000008</v>

</xml_diff>

<commit_message>
Updated case study data and other excel
as the title says. Resolved (I think) the conflict between Luca and my most recent commits
</commit_message>
<xml_diff>
--- a/data/case study data.xlsx
+++ b/data/case study data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnryter/Dropbox (MIT)/John MIT/Research/generalizationOutside/generalization/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77C1C112-8609-8940-B412-01A9C7918C57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77355F4E-6450-4B46-864E-7949541317E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15860" activeTab="3" xr2:uid="{9C1DBEC5-9C42-494B-AEAA-1D89B674AD0D}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15860" activeTab="1" xr2:uid="{9C1DBEC5-9C42-494B-AEAA-1D89B674AD0D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="17" r:id="rId1"/>
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="361">
   <si>
     <t>Al</t>
   </si>
@@ -540,9 +540,6 @@
     <t>Sn, self</t>
   </si>
   <si>
-    <t>Based on 400t production in 1900 from this paper (https://www.sciencedirect.com/science/article/pii/0301420782900253) and 4870 t production in 2019 below</t>
-  </si>
-  <si>
     <t>World Gold Council https://www.gold.org/goldhub/data/gold-production-by-country</t>
   </si>
   <si>
@@ -585,9 +582,6 @@
     <t>Our model, mod.demand_sectors.groupby(level=1,axis=1).sum().loc[2019]/mod.demand_sectors.sum(axis=1).loc[2019]</t>
   </si>
   <si>
-    <t>Our model, (np.log(mod.minemod.ml.loc[2019]['Head grade (%)']).var())</t>
-  </si>
-  <si>
     <t>Our model, (np.log(mod.minemod.ml.loc[2019]['Production (Mt)']*1000).var())</t>
   </si>
   <si>
@@ -717,9 +711,6 @@
     <t>World gold council for 2010-2019: https://www.gold.org/goldhub/data/gold-demand-by-country, remainder from USGS minerals yearbooks</t>
   </si>
   <si>
-    <t>World gold council for 2010-2019: https://www.gold.org/goldhub/data/gold-demand-by-country, Seeking Alpha 2003-2009: https://seekingalpha.com/article/1461891-is-it-time-to-buy-gold. Assumed 2001-2002 followed the same trend as primary supply</t>
-  </si>
-  <si>
     <t>Assuming no recycling</t>
   </si>
   <si>
@@ -1156,6 +1147,27 @@
   </si>
   <si>
     <t>Primary commodity price old</t>
+  </si>
+  <si>
+    <t>World gold council for 2010-2019: https://www.gold.org/goldhub/data/gold-demand-by-country, remainder using the BCG Recycled Content plot (exhibit 2, https://www.gold.org/goldhub/research/ups-and-downs-gold-recycling) to calculate total and secondary production from primary supply</t>
+  </si>
+  <si>
+    <t>World gold council for 2010-2019: https://www.gold.org/goldhub/data/gold-demand-by-country, Seeking Alpha 2003-2009: https://seekingalpha.com/article/1461891-is-it-time-to-buy-gold. Assumed 2001-2002 followed the same trend as primary supply. 2006-2015 validated by https://www.spdrgoldshares.com/media/GLD/file/GDT_Q1_2016.pdf (this one is on google scholar as Gold Demand Trends, Street 2016), table 10 in https://www.spdrgoldshares.com/media/GLD/file/GDT_Q1_2010.pdf, table 9 in https://www.spdrgoldshares.com/media/GLD/file/GDT_Q1_2012.pdf; for early years, taking the largest value I can find since it appears from price changes that demand exceeds supply</t>
+  </si>
+  <si>
+    <t>Actual demand</t>
+  </si>
+  <si>
+    <t>Other one is doing 5-yr rolling mean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Based on 400t production in 1900 from this paper (https://www.sciencedirect.com/science/article/pii/0301420782900253) and 4870 t production in 2019 below (0.021225); took the mean of that and the value using 2001-2019 demand in the Au sheet (0.01344), giving </t>
+  </si>
+  <si>
+    <t>Our model, (np.log(mod.minemod.ml.loc[2019]['Head grade (%)']).var()) = 0.0177, trying with higher value due to no opening happening</t>
+  </si>
+  <si>
+    <t>CHECK THAT ALL THESE ARE USING STD DEV NOT VARIANCE</t>
   </si>
 </sst>
 </file>
@@ -1166,7 +1178,7 @@
     <numFmt numFmtId="164" formatCode="\Te"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1242,6 +1254,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Var(--jp-code-font-family)"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1285,7 +1302,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1357,6 +1374,7 @@
     </xf>
     <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -1712,16 +1730,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AAEEA05-303F-4351-9872-7B8EAAB6CD92}">
   <dimension ref="A1:AK74"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="47.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" s="38" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:37" s="38" customFormat="1" ht="34" customHeight="1">
       <c r="A1" s="38" t="s">
         <v>96</v>
       </c>
@@ -1771,7 +1789,7 @@
         <v>94</v>
       </c>
       <c r="Q1" s="39" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="R1" s="38" t="s">
         <v>95</v>
@@ -1831,10 +1849,10 @@
         <v>109</v>
       </c>
       <c r="AK1" s="38" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="2" spans="1:37" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="2" spans="1:37" ht="14.5" customHeight="1">
       <c r="A2" s="6" t="s">
         <v>9</v>
       </c>
@@ -1903,7 +1921,7 @@
       <c r="AJ2" s="7"/>
       <c r="AK2" s="7"/>
     </row>
-    <row r="3" spans="1:37" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:37" ht="14.5" customHeight="1">
       <c r="A3" s="8" t="s">
         <v>17</v>
       </c>
@@ -1922,7 +1940,7 @@
         <v>97.8</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="I3" s="8">
         <v>2.4049999999999998</v>
@@ -1961,7 +1979,7 @@
         <v>18</v>
       </c>
       <c r="U3" s="9" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="V3" s="9" t="s">
         <v>134</v>
@@ -1970,37 +1988,37 @@
       <c r="X3" s="9"/>
       <c r="Y3" s="9"/>
       <c r="Z3" s="21" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="AA3" s="9" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="AB3" s="21" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="AC3" s="9"/>
       <c r="AD3" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="AE3" s="21" t="s">
+        <v>216</v>
+      </c>
+      <c r="AF3" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="AG3" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="AE3" s="21" t="s">
+      <c r="AH3" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="AF3" s="9" t="s">
+      <c r="AI3" s="9" t="s">
         <v>220</v>
-      </c>
-      <c r="AG3" s="9" t="s">
-        <v>221</v>
-      </c>
-      <c r="AH3" s="9" t="s">
-        <v>222</v>
-      </c>
-      <c r="AI3" s="9" t="s">
-        <v>223</v>
       </c>
       <c r="AJ3" s="9"/>
       <c r="AK3" s="9"/>
     </row>
-    <row r="4" spans="1:37" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:37" ht="14.5" customHeight="1">
       <c r="A4" s="6" t="s">
         <v>19</v>
       </c>
@@ -2010,11 +2028,11 @@
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="H4" s="6"/>
       <c r="I4" s="6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J4" s="6">
         <v>2.5399999999999999E-2</v>
@@ -2053,7 +2071,7 @@
       <c r="AJ4" s="7"/>
       <c r="AK4" s="7"/>
     </row>
-    <row r="5" spans="1:37" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:37" ht="14.5" customHeight="1">
       <c r="A5" s="8" t="s">
         <v>22</v>
       </c>
@@ -2064,7 +2082,7 @@
         <v>3.3765999999999997E-2</v>
       </c>
       <c r="D5" s="8">
-        <v>2.1225000000000001E-2</v>
+        <v>1.7332E-2</v>
       </c>
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
@@ -2109,46 +2127,46 @@
         <v>21</v>
       </c>
       <c r="U5" s="9" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="V5" s="9" t="s">
         <v>133</v>
       </c>
       <c r="W5" s="9" t="s">
-        <v>151</v>
+        <v>358</v>
       </c>
       <c r="X5" s="9"/>
       <c r="Y5" s="9"/>
       <c r="Z5" s="9" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="AA5" s="21" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="AB5" s="9" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="AC5" s="9"/>
       <c r="AD5" s="9" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="AE5" s="9" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="AF5" s="9"/>
       <c r="AG5" s="9" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="AH5" s="9" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="AI5" s="9" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="AJ5" s="9"/>
       <c r="AK5" s="9"/>
     </row>
-    <row r="6" spans="1:37" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:37" ht="14.5" customHeight="1">
       <c r="A6" s="6" t="s">
         <v>25</v>
       </c>
@@ -2202,48 +2220,48 @@
       </c>
       <c r="T6" s="7"/>
       <c r="U6" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="V6" s="7" t="s">
         <v>132</v>
       </c>
       <c r="W6" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="X6" s="7"/>
       <c r="Y6" s="7"/>
       <c r="Z6" s="7" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="AA6" s="7" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="AB6" s="7" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="AC6" s="7" t="s">
         <v>78</v>
       </c>
       <c r="AD6" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="AE6" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="AF6" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="AG6" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="AE6" s="7" t="s">
+      <c r="AH6" s="7" t="s">
         <v>237</v>
-      </c>
-      <c r="AF6" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="AG6" s="7" t="s">
-        <v>239</v>
-      </c>
-      <c r="AH6" s="7" t="s">
-        <v>240</v>
       </c>
       <c r="AI6" s="7"/>
       <c r="AJ6" s="7"/>
       <c r="AK6" s="7"/>
     </row>
-    <row r="7" spans="1:37" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:37" ht="14.5" customHeight="1">
       <c r="A7" s="8" t="s">
         <v>26</v>
       </c>
@@ -2299,7 +2317,7 @@
       </c>
       <c r="T7" s="9"/>
       <c r="U7" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="V7" s="9" t="s">
         <v>132</v>
@@ -2310,41 +2328,41 @@
       <c r="X7" s="9"/>
       <c r="Y7" s="9"/>
       <c r="Z7" s="9" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="AA7" s="9" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="AB7" s="9" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="AC7" s="9" t="s">
         <v>78</v>
       </c>
       <c r="AD7" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="AE7" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="AF7" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="AG7" s="9" t="s">
         <v>244</v>
       </c>
-      <c r="AE7" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="AF7" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="AG7" s="9" t="s">
-        <v>247</v>
-      </c>
       <c r="AH7" s="9" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="AI7" s="9" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="AJ7" s="9"/>
       <c r="AK7" s="9" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="8" spans="1:37" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="8" spans="1:37" ht="14.5" customHeight="1">
       <c r="A8" s="6" t="s">
         <v>27</v>
       </c>
@@ -2400,7 +2418,7 @@
       </c>
       <c r="T8" s="7"/>
       <c r="U8" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="V8" s="7" t="s">
         <v>132</v>
@@ -2411,37 +2429,37 @@
       <c r="X8" s="7"/>
       <c r="Y8" s="7"/>
       <c r="Z8" s="7" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="AA8" s="7" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="AB8" s="7" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="AC8" s="7" t="s">
         <v>78</v>
       </c>
       <c r="AD8" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="AE8" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="AF8" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="AG8" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="AH8" s="7" t="s">
         <v>252</v>
-      </c>
-      <c r="AE8" s="7" t="s">
-        <v>253</v>
-      </c>
-      <c r="AF8" s="7" t="s">
-        <v>254</v>
-      </c>
-      <c r="AG8" s="7" t="s">
-        <v>252</v>
-      </c>
-      <c r="AH8" s="7" t="s">
-        <v>255</v>
       </c>
       <c r="AI8" s="7"/>
       <c r="AJ8" s="7"/>
       <c r="AK8" s="7"/>
     </row>
-    <row r="9" spans="1:37" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:37" ht="14.5" customHeight="1">
       <c r="A9" s="8" t="s">
         <v>28</v>
       </c>
@@ -2497,7 +2515,7 @@
       </c>
       <c r="T9" s="9"/>
       <c r="U9" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="V9" s="9" t="s">
         <v>132</v>
@@ -2508,37 +2526,37 @@
       <c r="X9" s="9"/>
       <c r="Y9" s="9"/>
       <c r="Z9" s="9" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="AA9" s="9" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="AB9" s="9" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="AC9" s="9" t="s">
         <v>78</v>
       </c>
       <c r="AD9" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="AE9" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="AF9" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="AG9" s="9" t="s">
         <v>259</v>
       </c>
-      <c r="AE9" s="9" t="s">
+      <c r="AH9" s="9" t="s">
         <v>260</v>
-      </c>
-      <c r="AF9" s="9" t="s">
-        <v>261</v>
-      </c>
-      <c r="AG9" s="9" t="s">
-        <v>262</v>
-      </c>
-      <c r="AH9" s="9" t="s">
-        <v>263</v>
       </c>
       <c r="AI9" s="9"/>
       <c r="AJ9" s="9"/>
       <c r="AK9" s="9"/>
     </row>
-    <row r="10" spans="1:37" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:37" ht="14.5" customHeight="1">
       <c r="A10" s="6" t="s">
         <v>29</v>
       </c>
@@ -2597,7 +2615,7 @@
       </c>
       <c r="T10" s="7"/>
       <c r="U10" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="V10" s="7" t="s">
         <v>132</v>
@@ -2608,35 +2626,35 @@
       <c r="X10" s="7"/>
       <c r="Y10" s="7"/>
       <c r="Z10" s="7" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="AA10" s="7" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="AB10" s="7" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="AC10" s="7" t="s">
         <v>78</v>
       </c>
       <c r="AD10" s="7" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="AE10" s="7" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="AF10" s="7" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="AG10" s="7"/>
       <c r="AH10" s="7" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="AI10" s="7"/>
       <c r="AJ10" s="7"/>
       <c r="AK10" s="7"/>
     </row>
-    <row r="11" spans="1:37" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:37" ht="14.5" customHeight="1">
       <c r="A11" s="8" t="s">
         <v>30</v>
       </c>
@@ -2688,7 +2706,7 @@
       </c>
       <c r="T11" s="9"/>
       <c r="U11" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="V11" s="9" t="s">
         <v>132</v>
@@ -2701,29 +2719,29 @@
       <c r="Z11" s="9"/>
       <c r="AA11" s="9"/>
       <c r="AB11" s="9" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="AC11" s="9" t="s">
         <v>78</v>
       </c>
       <c r="AD11" s="9"/>
       <c r="AE11" s="9" t="s">
+        <v>269</v>
+      </c>
+      <c r="AF11" s="9" t="s">
+        <v>270</v>
+      </c>
+      <c r="AG11" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="AH11" s="9" t="s">
         <v>272</v>
-      </c>
-      <c r="AF11" s="9" t="s">
-        <v>273</v>
-      </c>
-      <c r="AG11" s="9" t="s">
-        <v>274</v>
-      </c>
-      <c r="AH11" s="9" t="s">
-        <v>275</v>
       </c>
       <c r="AI11" s="9"/>
       <c r="AJ11" s="9"/>
       <c r="AK11" s="9"/>
     </row>
-    <row r="12" spans="1:37" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:37" ht="14.5" customHeight="1">
       <c r="A12" s="6" t="s">
         <v>97</v>
       </c>
@@ -2785,44 +2803,44 @@
         <v>130</v>
       </c>
       <c r="W12" s="7" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="X12" s="7"/>
       <c r="Y12" s="7"/>
       <c r="Z12" s="7"/>
       <c r="AA12" s="7" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="AB12" s="7" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="AC12" s="7" t="s">
         <v>107</v>
       </c>
       <c r="AD12" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="AE12" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="AF12" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="AG12" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="AE12" s="7" t="s">
+      <c r="AH12" s="7" t="s">
         <v>279</v>
       </c>
-      <c r="AF12" s="7" t="s">
-        <v>280</v>
-      </c>
-      <c r="AG12" s="7" t="s">
-        <v>281</v>
-      </c>
-      <c r="AH12" s="7" t="s">
-        <v>282</v>
-      </c>
       <c r="AI12" s="7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="AJ12" s="7"/>
       <c r="AK12" s="7" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="13" spans="1:37" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="13" spans="1:37" ht="14.5" customHeight="1">
       <c r="A13" s="8" t="s">
         <v>98</v>
       </c>
@@ -2884,7 +2902,7 @@
         <v>130</v>
       </c>
       <c r="W13" s="9" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="X13" s="9"/>
       <c r="Y13" s="9"/>
@@ -2895,23 +2913,23 @@
         <v>107</v>
       </c>
       <c r="AD13" s="9" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="AE13" s="9" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="AF13" s="9"/>
       <c r="AG13" s="9"/>
       <c r="AH13" s="9" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="AI13" s="9"/>
       <c r="AJ13" s="9"/>
       <c r="AK13" s="9" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="14" spans="1:37" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="14" spans="1:37" ht="14.5" customHeight="1">
       <c r="A14" s="6" t="s">
         <v>99</v>
       </c>
@@ -2973,7 +2991,7 @@
         <v>130</v>
       </c>
       <c r="W14" s="7" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="X14" s="7"/>
       <c r="Y14" s="7"/>
@@ -2991,10 +3009,10 @@
       <c r="AI14" s="7"/>
       <c r="AJ14" s="7"/>
       <c r="AK14" s="7" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="15" spans="1:37" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="15" spans="1:37" ht="14.5" customHeight="1">
       <c r="A15" s="8" t="s">
         <v>100</v>
       </c>
@@ -3073,7 +3091,7 @@
       <c r="AJ15" s="9"/>
       <c r="AK15" s="9"/>
     </row>
-    <row r="16" spans="1:37" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:37" ht="14.5" customHeight="1">
       <c r="A16" s="6" t="s">
         <v>101</v>
       </c>
@@ -3151,10 +3169,10 @@
       <c r="AI16" s="7"/>
       <c r="AJ16" s="7"/>
       <c r="AK16" s="7" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="17" spans="1:37" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="17" spans="1:37" ht="14.5" customHeight="1">
       <c r="A17" s="8" t="s">
         <v>102</v>
       </c>
@@ -3216,42 +3234,42 @@
         <v>130</v>
       </c>
       <c r="W17" s="9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="X17" s="9"/>
       <c r="Y17" s="9"/>
       <c r="Z17" s="9"/>
       <c r="AA17" s="9" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="AB17" s="9" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="AC17" s="9" t="s">
         <v>107</v>
       </c>
       <c r="AD17" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="AE17" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="AF17" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="AG17" s="9" t="s">
         <v>291</v>
       </c>
-      <c r="AE17" s="9" t="s">
+      <c r="AH17" s="9" t="s">
         <v>292</v>
       </c>
-      <c r="AF17" s="9" t="s">
+      <c r="AI17" s="9" t="s">
         <v>293</v>
-      </c>
-      <c r="AG17" s="9" t="s">
-        <v>294</v>
-      </c>
-      <c r="AH17" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="AI17" s="9" t="s">
-        <v>296</v>
       </c>
       <c r="AJ17" s="9"/>
       <c r="AK17" s="9"/>
     </row>
-    <row r="18" spans="1:37" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:37" ht="14.5" customHeight="1">
       <c r="A18" s="6" t="s">
         <v>103</v>
       </c>
@@ -3313,44 +3331,44 @@
         <v>130</v>
       </c>
       <c r="W18" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="X18" s="7"/>
       <c r="Y18" s="7"/>
       <c r="Z18" s="23" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="AA18" s="7" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="AB18" s="23" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="AC18" s="7" t="s">
         <v>107</v>
       </c>
       <c r="AD18" s="7" t="s">
+        <v>297</v>
+      </c>
+      <c r="AE18" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="AF18" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="AG18" s="7" t="s">
         <v>300</v>
       </c>
-      <c r="AE18" s="7" t="s">
+      <c r="AH18" s="7" t="s">
         <v>301</v>
       </c>
-      <c r="AF18" s="7" t="s">
+      <c r="AI18" s="7" t="s">
         <v>302</v>
-      </c>
-      <c r="AG18" s="7" t="s">
-        <v>303</v>
-      </c>
-      <c r="AH18" s="7" t="s">
-        <v>304</v>
-      </c>
-      <c r="AI18" s="7" t="s">
-        <v>305</v>
       </c>
       <c r="AJ18" s="7"/>
       <c r="AK18" s="7"/>
     </row>
-    <row r="19" spans="1:37" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:37" ht="14.5" customHeight="1">
       <c r="A19" s="8" t="s">
         <v>104</v>
       </c>
@@ -3412,7 +3430,7 @@
         <v>130</v>
       </c>
       <c r="W19" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="X19" s="9"/>
       <c r="Y19" s="9"/>
@@ -3423,27 +3441,27 @@
         <v>107</v>
       </c>
       <c r="AD19" s="9" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="AE19" s="9" t="s">
+        <v>303</v>
+      </c>
+      <c r="AF19" s="9" t="s">
+        <v>304</v>
+      </c>
+      <c r="AG19" s="9" t="s">
+        <v>305</v>
+      </c>
+      <c r="AH19" s="9" t="s">
         <v>306</v>
       </c>
-      <c r="AF19" s="9" t="s">
+      <c r="AI19" s="24" t="s">
         <v>307</v>
-      </c>
-      <c r="AG19" s="9" t="s">
-        <v>308</v>
-      </c>
-      <c r="AH19" s="9" t="s">
-        <v>309</v>
-      </c>
-      <c r="AI19" s="24" t="s">
-        <v>310</v>
       </c>
       <c r="AJ19" s="9"/>
       <c r="AK19" s="9"/>
     </row>
-    <row r="20" spans="1:37" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:37" ht="14.5" customHeight="1">
       <c r="A20" s="6" t="s">
         <v>105</v>
       </c>
@@ -3491,12 +3509,12 @@
         <v>130</v>
       </c>
       <c r="W20" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="X20" s="7"/>
       <c r="Y20" s="7"/>
       <c r="Z20" s="7" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="AA20" s="7"/>
       <c r="AB20" s="7"/>
@@ -3504,10 +3522,10 @@
         <v>107</v>
       </c>
       <c r="AD20" s="7" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="AE20" s="7" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="AF20" s="7"/>
       <c r="AG20" s="7"/>
@@ -3516,7 +3534,7 @@
       <c r="AJ20" s="7"/>
       <c r="AK20" s="7"/>
     </row>
-    <row r="21" spans="1:37" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:37" ht="14.5" customHeight="1">
       <c r="A21" s="8" t="s">
         <v>106</v>
       </c>
@@ -3576,13 +3594,13 @@
         <v>130</v>
       </c>
       <c r="W21" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="X21" s="9"/>
       <c r="Y21" s="9"/>
       <c r="Z21" s="9"/>
       <c r="AA21" s="9" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="AB21" s="9"/>
       <c r="AC21" s="9" t="s">
@@ -3591,21 +3609,21 @@
       <c r="AD21" s="9"/>
       <c r="AE21" s="9"/>
       <c r="AF21" s="9" t="s">
+        <v>311</v>
+      </c>
+      <c r="AG21" s="9" t="s">
+        <v>312</v>
+      </c>
+      <c r="AH21" s="9" t="s">
+        <v>313</v>
+      </c>
+      <c r="AI21" s="9" t="s">
         <v>314</v>
-      </c>
-      <c r="AG21" s="9" t="s">
-        <v>315</v>
-      </c>
-      <c r="AH21" s="9" t="s">
-        <v>316</v>
-      </c>
-      <c r="AI21" s="9" t="s">
-        <v>317</v>
       </c>
       <c r="AJ21" s="9"/>
       <c r="AK21" s="9"/>
     </row>
-    <row r="22" spans="1:37" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:37" ht="14.5" customHeight="1">
       <c r="A22" s="6" t="s">
         <v>135</v>
       </c>
@@ -3643,11 +3661,11 @@
       </c>
       <c r="T22" s="7"/>
       <c r="U22" s="12" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="V22" s="7"/>
       <c r="W22" s="7" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="X22" s="7"/>
       <c r="Y22" s="7"/>
@@ -3655,7 +3673,7 @@
       <c r="AA22" s="7"/>
       <c r="AB22" s="7"/>
       <c r="AC22" s="7" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="AD22" s="7"/>
       <c r="AE22" s="7"/>
@@ -3666,7 +3684,7 @@
       <c r="AJ22" s="7"/>
       <c r="AK22" s="6"/>
     </row>
-    <row r="23" spans="1:37" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:37" ht="14.5" customHeight="1">
       <c r="A23" s="8" t="s">
         <v>136</v>
       </c>
@@ -3704,11 +3722,11 @@
       </c>
       <c r="T23" s="9"/>
       <c r="U23" s="13" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="V23" s="9"/>
       <c r="W23" s="9" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="X23" s="9"/>
       <c r="Y23" s="9"/>
@@ -3716,7 +3734,7 @@
       <c r="AA23" s="9"/>
       <c r="AB23" s="9"/>
       <c r="AC23" s="9" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="AD23" s="9"/>
       <c r="AE23" s="9"/>
@@ -3727,7 +3745,7 @@
       <c r="AJ23" s="9"/>
       <c r="AK23" s="8"/>
     </row>
-    <row r="24" spans="1:37" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:37" ht="14.5" customHeight="1">
       <c r="A24" s="6" t="s">
         <v>137</v>
       </c>
@@ -3765,11 +3783,11 @@
       </c>
       <c r="T24" s="7"/>
       <c r="U24" s="12" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="V24" s="7"/>
       <c r="W24" s="7" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="X24" s="7"/>
       <c r="Y24" s="7"/>
@@ -3777,7 +3795,7 @@
       <c r="AA24" s="7"/>
       <c r="AB24" s="7"/>
       <c r="AC24" s="7" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="AD24" s="7"/>
       <c r="AE24" s="7"/>
@@ -3788,7 +3806,7 @@
       <c r="AJ24" s="7"/>
       <c r="AK24" s="6"/>
     </row>
-    <row r="25" spans="1:37" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:37" ht="14.5" customHeight="1">
       <c r="A25" s="8" t="s">
         <v>138</v>
       </c>
@@ -3826,11 +3844,11 @@
       </c>
       <c r="T25" s="9"/>
       <c r="U25" s="13" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="V25" s="9"/>
       <c r="W25" s="9" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="X25" s="9"/>
       <c r="Y25" s="9"/>
@@ -3838,7 +3856,7 @@
       <c r="AA25" s="9"/>
       <c r="AB25" s="9"/>
       <c r="AC25" s="9" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="AD25" s="9"/>
       <c r="AE25" s="9"/>
@@ -3849,7 +3867,7 @@
       <c r="AJ25" s="9"/>
       <c r="AK25" s="8"/>
     </row>
-    <row r="26" spans="1:37" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:37" ht="14.5" customHeight="1">
       <c r="A26" s="6" t="s">
         <v>139</v>
       </c>
@@ -3885,11 +3903,11 @@
       </c>
       <c r="T26" s="7"/>
       <c r="U26" s="12" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="V26" s="7"/>
       <c r="W26" s="7" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="X26" s="7"/>
       <c r="Y26" s="7"/>
@@ -3897,7 +3915,7 @@
       <c r="AA26" s="7"/>
       <c r="AB26" s="7"/>
       <c r="AC26" s="7" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="AD26" s="7"/>
       <c r="AE26" s="7"/>
@@ -3908,7 +3926,7 @@
       <c r="AJ26" s="7"/>
       <c r="AK26" s="6"/>
     </row>
-    <row r="27" spans="1:37" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:37" ht="14.5" customHeight="1">
       <c r="A27" s="8" t="s">
         <v>70</v>
       </c>
@@ -3964,7 +3982,7 @@
         <v>71</v>
       </c>
       <c r="U27" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="V27" s="9" t="s">
         <v>129</v>
@@ -3975,11 +3993,11 @@
       <c r="X27" s="9"/>
       <c r="Y27" s="9"/>
       <c r="Z27" s="21" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="AA27" s="9"/>
       <c r="AB27" s="21" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="AC27" s="9" t="s">
         <v>77</v>
@@ -3989,13 +4007,13 @@
       <c r="AF27" s="9"/>
       <c r="AG27" s="9"/>
       <c r="AH27" s="9" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="AI27" s="9"/>
       <c r="AJ27" s="9"/>
       <c r="AK27" s="9"/>
     </row>
-    <row r="28" spans="1:37" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:37" ht="14.5" customHeight="1">
       <c r="A28" s="6" t="s">
         <v>69</v>
       </c>
@@ -4049,7 +4067,7 @@
       </c>
       <c r="T28" s="7"/>
       <c r="U28" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="V28" s="7" t="s">
         <v>128</v>
@@ -4060,31 +4078,31 @@
       <c r="X28" s="7"/>
       <c r="Y28" s="7"/>
       <c r="Z28" s="7" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="AA28" s="7"/>
       <c r="AB28" s="23" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="AC28" s="7" t="s">
         <v>77</v>
       </c>
       <c r="AD28" s="7"/>
       <c r="AE28" s="7" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="AF28" s="7" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="AG28" s="7"/>
       <c r="AH28" s="7" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="AI28" s="7"/>
       <c r="AJ28" s="7"/>
       <c r="AK28" s="7"/>
     </row>
-    <row r="29" spans="1:37" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:37" ht="14.5" customHeight="1">
       <c r="A29" s="8" t="s">
         <v>75</v>
       </c>
@@ -4163,7 +4181,7 @@
       <c r="AJ29" s="9"/>
       <c r="AK29" s="9"/>
     </row>
-    <row r="30" spans="1:37" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:37" ht="14.5" customHeight="1">
       <c r="A30" s="6" t="s">
         <v>74</v>
       </c>
@@ -4215,18 +4233,18 @@
       </c>
       <c r="T30" s="7"/>
       <c r="U30" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="V30" s="7" t="s">
         <v>132</v>
       </c>
       <c r="W30" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="X30" s="7"/>
       <c r="Y30" s="7"/>
       <c r="Z30" s="23" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="AA30" s="7"/>
       <c r="AB30" s="7"/>
@@ -4234,19 +4252,19 @@
         <v>77</v>
       </c>
       <c r="AD30" s="7" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="AE30" s="7"/>
       <c r="AF30" s="7"/>
       <c r="AG30" s="7"/>
       <c r="AH30" s="29" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="AI30" s="7"/>
       <c r="AJ30" s="7"/>
       <c r="AK30" s="7"/>
     </row>
-    <row r="31" spans="1:37" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:37" ht="14.5" customHeight="1">
       <c r="A31" s="8" t="s">
         <v>72</v>
       </c>
@@ -4323,7 +4341,7 @@
       <c r="AJ31" s="9"/>
       <c r="AK31" s="9"/>
     </row>
-    <row r="32" spans="1:37" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:37" ht="14.5" customHeight="1">
       <c r="A32" s="6" t="s">
         <v>32</v>
       </c>
@@ -4396,13 +4414,13 @@
       <c r="AF32" s="7"/>
       <c r="AG32" s="7"/>
       <c r="AH32" s="7" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="AI32" s="7"/>
       <c r="AJ32" s="7"/>
       <c r="AK32" s="7"/>
     </row>
-    <row r="33" spans="1:37" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:37" ht="14.5" customHeight="1">
       <c r="A33" s="8" t="s">
         <v>73</v>
       </c>
@@ -4463,27 +4481,27 @@
       <c r="Z33" s="9"/>
       <c r="AA33" s="9"/>
       <c r="AB33" s="9" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="AC33" s="9" t="s">
         <v>77</v>
       </c>
       <c r="AD33" s="9" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="AE33" s="9"/>
       <c r="AF33" s="9"/>
       <c r="AG33" s="9"/>
       <c r="AH33" s="21" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="AI33" s="9"/>
       <c r="AJ33" s="9"/>
       <c r="AK33" s="9" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="34" spans="1:37" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="34" spans="1:37" ht="14.5" customHeight="1">
       <c r="A34" s="6" t="s">
         <v>33</v>
       </c>
@@ -4548,11 +4566,11 @@
         <v>77</v>
       </c>
       <c r="AD34" s="23" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="AE34" s="7"/>
       <c r="AF34" s="7" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="AG34" s="7"/>
       <c r="AH34" s="7"/>
@@ -4560,7 +4578,7 @@
       <c r="AJ34" s="7"/>
       <c r="AK34" s="7"/>
     </row>
-    <row r="35" spans="1:37" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:37" ht="14.5" customHeight="1">
       <c r="A35" s="8" t="s">
         <v>76</v>
       </c>
@@ -4615,24 +4633,24 @@
       </c>
       <c r="T35" s="9"/>
       <c r="U35" s="9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="V35" s="9" t="s">
         <v>132</v>
       </c>
       <c r="W35" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="X35" s="9"/>
       <c r="Y35" s="9"/>
       <c r="Z35" s="9" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="AA35" s="9" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="AB35" s="9" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="AC35" s="9" t="s">
         <v>91</v>
@@ -4640,19 +4658,19 @@
       <c r="AD35" s="9"/>
       <c r="AE35" s="9"/>
       <c r="AF35" s="9" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="AG35" s="9"/>
       <c r="AH35" s="9" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="AI35" s="9"/>
       <c r="AJ35" s="9"/>
       <c r="AK35" s="9"/>
     </row>
-    <row r="36" spans="1:37" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:37" ht="14.5" customHeight="1">
       <c r="A36" s="6" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="B36" s="6">
         <v>0.5</v>
@@ -4721,13 +4739,13 @@
       <c r="AF36" s="6"/>
       <c r="AG36" s="6"/>
       <c r="AH36" s="6" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="AI36" s="6"/>
       <c r="AJ36" s="6"/>
       <c r="AK36" s="6"/>
     </row>
-    <row r="37" spans="1:37" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:37" ht="14.5" customHeight="1">
       <c r="A37" s="8" t="s">
         <v>14</v>
       </c>
@@ -4785,20 +4803,20 @@
         <v>92</v>
       </c>
       <c r="W37" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="X37" s="9" t="s">
         <v>93</v>
       </c>
       <c r="Y37" s="9"/>
       <c r="Z37" s="9" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="AA37" s="21" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="AB37" s="9" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="AC37" s="9"/>
       <c r="AD37" s="9"/>
@@ -4807,12 +4825,12 @@
       <c r="AG37" s="9"/>
       <c r="AH37" s="9"/>
       <c r="AI37" s="9" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="AJ37" s="9"/>
       <c r="AK37" s="9"/>
     </row>
-    <row r="38" spans="1:37" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:37" ht="14.5" customHeight="1">
       <c r="A38" s="30" t="s">
         <v>15</v>
       </c>
@@ -4859,7 +4877,7 @@
       </c>
       <c r="T38" s="7"/>
       <c r="U38" s="7" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="V38" s="7" t="s">
         <v>90</v>
@@ -4896,7 +4914,7 @@
       <c r="AJ38" s="7"/>
       <c r="AK38" s="7"/>
     </row>
-    <row r="39" spans="1:37" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:37" ht="14.5" customHeight="1">
       <c r="A39" s="31" t="s">
         <v>16</v>
       </c>
@@ -4942,7 +4960,7 @@
       </c>
       <c r="T39" s="9"/>
       <c r="U39" s="9" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="V39" s="9" t="s">
         <v>89</v>
@@ -4979,7 +4997,7 @@
       <c r="AJ39" s="9"/>
       <c r="AK39" s="9"/>
     </row>
-    <row r="40" spans="1:37" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:37" ht="14.5" customHeight="1">
       <c r="A40" s="30" t="s">
         <v>35</v>
       </c>
@@ -5026,7 +5044,7 @@
       </c>
       <c r="T40" s="7"/>
       <c r="U40" s="7" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="V40" s="7" t="s">
         <v>89</v>
@@ -5063,12 +5081,12 @@
       <c r="AJ40" s="7"/>
       <c r="AK40" s="7"/>
     </row>
-    <row r="41" spans="1:37" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:37" ht="14.5" customHeight="1">
       <c r="A41" s="31" t="s">
         <v>36</v>
       </c>
       <c r="B41" s="8">
-        <v>1.77E-2</v>
+        <v>0.13320000000000001</v>
       </c>
       <c r="C41" s="8">
         <v>6.0100000000000001E-2</v>
@@ -5107,9 +5125,11 @@
       <c r="S41" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="T41" s="9"/>
+      <c r="T41" s="9" t="s">
+        <v>360</v>
+      </c>
       <c r="U41" s="9" t="s">
-        <v>166</v>
+        <v>359</v>
       </c>
       <c r="V41" s="9" t="s">
         <v>89</v>
@@ -5146,7 +5166,7 @@
       <c r="AJ41" s="9"/>
       <c r="AK41" s="9"/>
     </row>
-    <row r="42" spans="1:37" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:37" ht="14.5" customHeight="1">
       <c r="A42" s="6" t="s">
         <v>37</v>
       </c>
@@ -5211,29 +5231,29 @@
       <c r="X42" s="7"/>
       <c r="Y42" s="7"/>
       <c r="Z42" s="23" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="AA42" s="7"/>
       <c r="AB42" s="23" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="AC42" s="7" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="AD42" s="7"/>
       <c r="AE42" s="7"/>
       <c r="AF42" s="7"/>
       <c r="AG42" s="23" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="AH42" s="7"/>
       <c r="AI42" s="7"/>
       <c r="AJ42" s="7"/>
       <c r="AK42" s="7" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="43" spans="1:37" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="43" spans="1:37" ht="14.5" customHeight="1">
       <c r="A43" s="8" t="s">
         <v>125</v>
       </c>
@@ -5288,52 +5308,52 @@
       <c r="S43" s="8"/>
       <c r="T43" s="8"/>
       <c r="U43" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="V43" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="V43" s="8" t="s">
-        <v>172</v>
-      </c>
       <c r="W43" s="8" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="X43" s="8" t="s">
         <v>127</v>
       </c>
       <c r="Y43" s="8"/>
       <c r="Z43" s="24" t="s">
+        <v>344</v>
+      </c>
+      <c r="AA43" s="8" t="s">
+        <v>345</v>
+      </c>
+      <c r="AB43" s="24" t="s">
+        <v>340</v>
+      </c>
+      <c r="AC43" s="8" t="s">
+        <v>346</v>
+      </c>
+      <c r="AD43" s="8" t="s">
         <v>347</v>
       </c>
-      <c r="AA43" s="8" t="s">
-        <v>348</v>
-      </c>
-      <c r="AB43" s="24" t="s">
-        <v>343</v>
-      </c>
-      <c r="AC43" s="8" t="s">
-        <v>349</v>
-      </c>
-      <c r="AD43" s="8" t="s">
-        <v>350</v>
-      </c>
       <c r="AE43" s="8" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="AF43" s="8" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="AG43" s="8" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="AH43" s="8" t="s">
         <v>127</v>
       </c>
       <c r="AI43" s="8" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="AJ43" s="8"/>
       <c r="AK43" s="9"/>
     </row>
-    <row r="44" spans="1:37" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:37" ht="14.5" customHeight="1">
       <c r="A44" s="30" t="s">
         <v>38</v>
       </c>
@@ -5383,7 +5403,7 @@
       </c>
       <c r="T44" s="6"/>
       <c r="U44" s="6" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="V44" s="7" t="s">
         <v>88</v>
@@ -5394,7 +5414,7 @@
       <c r="X44" s="7"/>
       <c r="Y44" s="7"/>
       <c r="Z44" s="7" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="AA44" s="7"/>
       <c r="AB44" s="7"/>
@@ -5424,7 +5444,7 @@
       </c>
       <c r="AK44" s="7"/>
     </row>
-    <row r="45" spans="1:37" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:37" ht="14.5" customHeight="1">
       <c r="A45" s="31" t="s">
         <v>39</v>
       </c>
@@ -5474,7 +5494,7 @@
       </c>
       <c r="T45" s="8"/>
       <c r="U45" s="8" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="V45" s="9" t="s">
         <v>88</v>
@@ -5485,7 +5505,7 @@
       <c r="X45" s="9"/>
       <c r="Y45" s="9"/>
       <c r="Z45" s="9" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="AA45" s="9"/>
       <c r="AB45" s="9"/>
@@ -5515,7 +5535,7 @@
       </c>
       <c r="AK45" s="9"/>
     </row>
-    <row r="46" spans="1:37" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:37" ht="14.5" customHeight="1">
       <c r="A46" s="30" t="s">
         <v>40</v>
       </c>
@@ -5565,7 +5585,7 @@
       </c>
       <c r="T46" s="6"/>
       <c r="U46" s="6" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="V46" s="7" t="s">
         <v>88</v>
@@ -5604,7 +5624,7 @@
       </c>
       <c r="AK46" s="7"/>
     </row>
-    <row r="47" spans="1:37" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:37" ht="14.5" customHeight="1">
       <c r="A47" s="31" t="s">
         <v>41</v>
       </c>
@@ -5654,7 +5674,7 @@
       </c>
       <c r="T47" s="8"/>
       <c r="U47" s="8" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="V47" s="9" t="s">
         <v>88</v>
@@ -5693,7 +5713,7 @@
       </c>
       <c r="AK47" s="9"/>
     </row>
-    <row r="48" spans="1:37" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:37" ht="14.5" customHeight="1">
       <c r="A48" s="30" t="s">
         <v>42</v>
       </c>
@@ -5743,7 +5763,7 @@
       </c>
       <c r="T48" s="6"/>
       <c r="U48" s="6" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="V48" s="7" t="s">
         <v>88</v>
@@ -5782,7 +5802,7 @@
       </c>
       <c r="AK48" s="7"/>
     </row>
-    <row r="49" spans="1:37" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:37" ht="14.5" customHeight="1">
       <c r="A49" s="33" t="s">
         <v>43</v>
       </c>
@@ -5825,7 +5845,7 @@
       <c r="AJ49" s="17"/>
       <c r="AK49" s="9"/>
     </row>
-    <row r="50" spans="1:37" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:37" ht="14.5" customHeight="1">
       <c r="A50" s="6" t="s">
         <v>44</v>
       </c>
@@ -5868,7 +5888,7 @@
       <c r="AJ50" s="7"/>
       <c r="AK50" s="7"/>
     </row>
-    <row r="51" spans="1:37" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:37" ht="14.5" customHeight="1">
       <c r="A51" s="8" t="s">
         <v>45</v>
       </c>
@@ -5911,7 +5931,7 @@
       <c r="AJ51" s="9"/>
       <c r="AK51" s="9"/>
     </row>
-    <row r="52" spans="1:37" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:37" ht="14.5" customHeight="1">
       <c r="A52" s="6" t="s">
         <v>46</v>
       </c>
@@ -5954,7 +5974,7 @@
       <c r="AJ52" s="7"/>
       <c r="AK52" s="7"/>
     </row>
-    <row r="53" spans="1:37" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:37" ht="14.5" customHeight="1">
       <c r="A53" s="8" t="s">
         <v>47</v>
       </c>
@@ -5997,7 +6017,7 @@
       <c r="AJ53" s="9"/>
       <c r="AK53" s="9"/>
     </row>
-    <row r="54" spans="1:37" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:37" ht="14.5" customHeight="1">
       <c r="A54" s="6" t="s">
         <v>48</v>
       </c>
@@ -6040,7 +6060,7 @@
       <c r="AJ54" s="7"/>
       <c r="AK54" s="7"/>
     </row>
-    <row r="55" spans="1:37" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:37" ht="14.5" customHeight="1">
       <c r="A55" s="8" t="s">
         <v>49</v>
       </c>
@@ -6083,7 +6103,7 @@
       <c r="AJ55" s="9"/>
       <c r="AK55" s="9"/>
     </row>
-    <row r="56" spans="1:37" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:37" ht="14.5" customHeight="1">
       <c r="A56" s="6" t="s">
         <v>50</v>
       </c>
@@ -6126,7 +6146,7 @@
       <c r="AJ56" s="7"/>
       <c r="AK56" s="7"/>
     </row>
-    <row r="57" spans="1:37" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:37" ht="14.5" customHeight="1">
       <c r="A57" s="8" t="s">
         <v>51</v>
       </c>
@@ -6169,7 +6189,7 @@
       <c r="AJ57" s="9"/>
       <c r="AK57" s="9"/>
     </row>
-    <row r="58" spans="1:37" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:37" ht="14.5" customHeight="1">
       <c r="A58" s="6" t="s">
         <v>52</v>
       </c>
@@ -6212,7 +6232,7 @@
       <c r="AJ58" s="7"/>
       <c r="AK58" s="7"/>
     </row>
-    <row r="59" spans="1:37" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:37" ht="14.5" customHeight="1">
       <c r="A59" s="8" t="s">
         <v>53</v>
       </c>
@@ -6255,7 +6275,7 @@
       <c r="AJ59" s="9"/>
       <c r="AK59" s="9"/>
     </row>
-    <row r="60" spans="1:37" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:37" ht="14.5" customHeight="1">
       <c r="A60" s="6" t="s">
         <v>54</v>
       </c>
@@ -6298,7 +6318,7 @@
       <c r="AJ60" s="7"/>
       <c r="AK60" s="7"/>
     </row>
-    <row r="61" spans="1:37" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:37" ht="14.5" customHeight="1">
       <c r="A61" s="8" t="s">
         <v>55</v>
       </c>
@@ -6341,7 +6361,7 @@
       <c r="AJ61" s="9"/>
       <c r="AK61" s="9"/>
     </row>
-    <row r="62" spans="1:37" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:37" ht="14.5" customHeight="1">
       <c r="A62" s="6" t="s">
         <v>56</v>
       </c>
@@ -6384,7 +6404,7 @@
       <c r="AJ62" s="7"/>
       <c r="AK62" s="7"/>
     </row>
-    <row r="63" spans="1:37" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:37" ht="14.5" customHeight="1">
       <c r="A63" s="8" t="s">
         <v>57</v>
       </c>
@@ -6427,7 +6447,7 @@
       <c r="AJ63" s="9"/>
       <c r="AK63" s="9"/>
     </row>
-    <row r="64" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:37">
       <c r="A64" s="6" t="s">
         <v>58</v>
       </c>
@@ -6470,7 +6490,7 @@
       <c r="AJ64" s="7"/>
       <c r="AK64" s="7"/>
     </row>
-    <row r="65" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:37">
       <c r="A65" s="8" t="s">
         <v>59</v>
       </c>
@@ -6513,7 +6533,7 @@
       <c r="AJ65" s="9"/>
       <c r="AK65" s="9"/>
     </row>
-    <row r="66" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:37">
       <c r="A66" s="6" t="s">
         <v>60</v>
       </c>
@@ -6556,7 +6576,7 @@
       <c r="AJ66" s="7"/>
       <c r="AK66" s="7"/>
     </row>
-    <row r="67" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:37">
       <c r="A67" s="8" t="s">
         <v>61</v>
       </c>
@@ -6599,7 +6619,7 @@
       <c r="AJ67" s="9"/>
       <c r="AK67" s="9"/>
     </row>
-    <row r="68" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:37">
       <c r="A68" s="6" t="s">
         <v>62</v>
       </c>
@@ -6642,7 +6662,7 @@
       <c r="AJ68" s="7"/>
       <c r="AK68" s="7"/>
     </row>
-    <row r="69" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:37">
       <c r="A69" s="8" t="s">
         <v>63</v>
       </c>
@@ -6685,7 +6705,7 @@
       <c r="AJ69" s="9"/>
       <c r="AK69" s="9"/>
     </row>
-    <row r="70" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:37">
       <c r="A70" s="6" t="s">
         <v>64</v>
       </c>
@@ -6728,7 +6748,7 @@
       <c r="AJ70" s="7"/>
       <c r="AK70" s="7"/>
     </row>
-    <row r="71" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:37">
       <c r="A71" s="8" t="s">
         <v>65</v>
       </c>
@@ -6771,7 +6791,7 @@
       <c r="AJ71" s="9"/>
       <c r="AK71" s="9"/>
     </row>
-    <row r="72" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:37">
       <c r="A72" s="6" t="s">
         <v>66</v>
       </c>
@@ -6814,7 +6834,7 @@
       <c r="AJ72" s="7"/>
       <c r="AK72" s="7"/>
     </row>
-    <row r="73" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:37">
       <c r="A73" s="8" t="s">
         <v>67</v>
       </c>
@@ -6857,7 +6877,7 @@
       <c r="AJ73" s="9"/>
       <c r="AK73" s="9"/>
     </row>
-    <row r="74" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:37">
       <c r="A74" s="35" t="s">
         <v>68</v>
       </c>
@@ -6933,7 +6953,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6945,7 +6965,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6957,7 +6977,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6969,7 +6989,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6981,7 +7001,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6995,43 +7015,43 @@
       <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="9" max="9" width="29.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="B1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E1" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B2" t="s">
+        <v>208</v>
+      </c>
+      <c r="C2" t="s">
+        <v>209</v>
+      </c>
+      <c r="D2" t="s">
+        <v>210</v>
+      </c>
+      <c r="E2" t="s">
         <v>211</v>
       </c>
-      <c r="C2" t="s">
-        <v>212</v>
-      </c>
-      <c r="D2" t="s">
-        <v>213</v>
-      </c>
-      <c r="E2" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>2001</v>
       </c>
@@ -7042,7 +7062,7 @@
         <v>58.591498999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>2002</v>
       </c>
@@ -7053,7 +7073,7 @@
         <v>67.924413999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>2003</v>
       </c>
@@ -7064,7 +7084,7 @@
         <v>76.145567</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>2004</v>
       </c>
@@ -7082,7 +7102,7 @@
         <v>85.971186000000003</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>2005</v>
       </c>
@@ -7100,7 +7120,7 @@
         <v>96.04539299999999</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>2006</v>
       </c>
@@ -7118,7 +7138,7 @@
         <v>105.140455</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>2007</v>
       </c>
@@ -7136,7 +7156,7 @@
         <v>121.12909199999999</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>2008</v>
       </c>
@@ -7154,7 +7174,7 @@
         <v>125.57747800000001</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>2009</v>
       </c>
@@ -7172,7 +7192,7 @@
         <v>99.382306999999997</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12">
         <v>2010</v>
       </c>
@@ -7190,7 +7210,7 @@
         <v>143.25536400000001</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5">
       <c r="A13">
         <v>2011</v>
       </c>
@@ -7208,7 +7228,7 @@
         <v>177.108566</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5">
       <c r="A14">
         <v>2012</v>
       </c>
@@ -7226,7 +7246,7 @@
         <v>183.31275300000004</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="A15">
         <v>2013</v>
       </c>
@@ -7244,7 +7264,7 @@
         <v>172.04403400000001</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="A16">
         <v>2014</v>
       </c>
@@ -7262,7 +7282,7 @@
         <v>186.019372</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5">
       <c r="A17">
         <v>2015</v>
       </c>
@@ -7280,7 +7300,7 @@
         <v>201.32204200000001</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5">
       <c r="A18">
         <v>2016</v>
       </c>
@@ -7298,7 +7318,7 @@
         <v>246.11897900000002</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5">
       <c r="A19">
         <v>2017</v>
       </c>
@@ -7316,7 +7336,7 @@
         <v>312.55251800000002</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5">
       <c r="A20">
         <v>2018</v>
       </c>
@@ -7334,7 +7354,7 @@
         <v>361.04267200000004</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5">
       <c r="A21">
         <v>2019</v>
       </c>
@@ -7361,11 +7381,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F73D63CC-D9E2-4D18-93CD-FFAA257617FA}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="19.83203125" customWidth="1"/>
     <col min="3" max="3" width="21.33203125" customWidth="1"/>
@@ -7374,44 +7394,44 @@
     <col min="6" max="6" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="B1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C1" t="s">
+        <v>192</v>
+      </c>
+      <c r="D1" t="s">
+        <v>195</v>
+      </c>
+      <c r="E1" t="s">
+        <v>189</v>
+      </c>
+      <c r="F1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C2" t="s">
+        <v>206</v>
+      </c>
+      <c r="D2" t="s">
+        <v>194</v>
+      </c>
+      <c r="E2" t="s">
         <v>190</v>
       </c>
-      <c r="C1" t="s">
-        <v>194</v>
-      </c>
-      <c r="D1" t="s">
-        <v>197</v>
-      </c>
-      <c r="E1" t="s">
-        <v>191</v>
-      </c>
-      <c r="F1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>182</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="F2" t="s">
         <v>193</v>
       </c>
-      <c r="C2" t="s">
-        <v>208</v>
-      </c>
-      <c r="D2" t="s">
-        <v>196</v>
-      </c>
-      <c r="E2" t="s">
-        <v>192</v>
-      </c>
-      <c r="F2" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:9" ht="16">
       <c r="A3">
         <v>2001</v>
       </c>
@@ -7432,7 +7452,7 @@
       </c>
       <c r="I3" s="4"/>
     </row>
-    <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="16">
       <c r="A4">
         <v>2002</v>
       </c>
@@ -7453,7 +7473,7 @@
       </c>
       <c r="I4" s="4"/>
     </row>
-    <row r="5" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="16">
       <c r="A5">
         <v>2003</v>
       </c>
@@ -7474,7 +7494,7 @@
       </c>
       <c r="I5" s="4"/>
     </row>
-    <row r="6" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="16">
       <c r="A6">
         <v>2004</v>
       </c>
@@ -7495,7 +7515,7 @@
       </c>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="16">
       <c r="A7">
         <v>2005</v>
       </c>
@@ -7516,7 +7536,7 @@
       </c>
       <c r="I7" s="4"/>
     </row>
-    <row r="8" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="16">
       <c r="A8">
         <v>2006</v>
       </c>
@@ -7537,7 +7557,7 @@
       </c>
       <c r="I8" s="4"/>
     </row>
-    <row r="9" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="16">
       <c r="A9">
         <v>2007</v>
       </c>
@@ -7558,7 +7578,7 @@
       </c>
       <c r="I9" s="4"/>
     </row>
-    <row r="10" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="16">
       <c r="A10">
         <v>2008</v>
       </c>
@@ -7579,7 +7599,7 @@
       </c>
       <c r="I10" s="4"/>
     </row>
-    <row r="11" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="16">
       <c r="A11">
         <v>2009</v>
       </c>
@@ -7600,7 +7620,7 @@
       </c>
       <c r="I11" s="4"/>
     </row>
-    <row r="12" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="16">
       <c r="A12">
         <v>2010</v>
       </c>
@@ -7621,7 +7641,7 @@
       </c>
       <c r="I12" s="4"/>
     </row>
-    <row r="13" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="16">
       <c r="A13">
         <v>2011</v>
       </c>
@@ -7642,7 +7662,7 @@
       </c>
       <c r="I13" s="4"/>
     </row>
-    <row r="14" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="16">
       <c r="A14">
         <v>2012</v>
       </c>
@@ -7663,7 +7683,7 @@
       </c>
       <c r="I14" s="4"/>
     </row>
-    <row r="15" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="16">
       <c r="A15">
         <v>2013</v>
       </c>
@@ -7684,7 +7704,7 @@
       </c>
       <c r="I15" s="4"/>
     </row>
-    <row r="16" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="16">
       <c r="A16">
         <v>2014</v>
       </c>
@@ -7705,7 +7725,7 @@
       </c>
       <c r="I16" s="4"/>
     </row>
-    <row r="17" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" ht="16">
       <c r="A17">
         <v>2015</v>
       </c>
@@ -7726,7 +7746,7 @@
       </c>
       <c r="I17" s="4"/>
     </row>
-    <row r="18" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" ht="16">
       <c r="A18">
         <v>2016</v>
       </c>
@@ -7747,7 +7767,7 @@
       </c>
       <c r="I18" s="4"/>
     </row>
-    <row r="19" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" ht="16">
       <c r="A19">
         <v>2017</v>
       </c>
@@ -7768,7 +7788,7 @@
       </c>
       <c r="I19" s="4"/>
     </row>
-    <row r="20" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" ht="16">
       <c r="A20">
         <v>2018</v>
       </c>
@@ -7789,7 +7809,7 @@
       </c>
       <c r="I20" s="4"/>
     </row>
-    <row r="21" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" ht="16">
       <c r="A21">
         <v>2019</v>
       </c>
@@ -7825,7 +7845,7 @@
       <selection activeCell="A3" sqref="A3:A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.6640625" bestFit="1" customWidth="1"/>
@@ -7834,47 +7854,47 @@
     <col min="7" max="7" width="21.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14">
       <c r="B1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D1" t="s">
+        <v>195</v>
+      </c>
+      <c r="E1" t="s">
+        <v>201</v>
+      </c>
+      <c r="F1" t="s">
+        <v>196</v>
+      </c>
+      <c r="G1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C2" t="s">
+        <v>204</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="E1" t="s">
-        <v>203</v>
-      </c>
-      <c r="F1" t="s">
-        <v>198</v>
-      </c>
-      <c r="G1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>182</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="C2" t="s">
-        <v>206</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" t="s">
         <v>199</v>
       </c>
-      <c r="G2" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:14" ht="16">
       <c r="A3">
         <v>2001</v>
       </c>
@@ -7900,7 +7920,7 @@
         <v>447.61374899999998</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" ht="16">
       <c r="A4">
         <v>2002</v>
       </c>
@@ -7924,7 +7944,7 @@
         <v>424.685877</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" ht="16">
       <c r="A5">
         <v>2003</v>
       </c>
@@ -7948,7 +7968,7 @@
         <v>470.54162100000002</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" ht="16">
       <c r="A6">
         <v>2004</v>
       </c>
@@ -7972,7 +7992,7 @@
         <v>767.02960299999995</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" ht="16">
       <c r="A7">
         <v>2005</v>
       </c>
@@ -7996,7 +8016,7 @@
         <v>674.22585800000002</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" ht="16">
       <c r="A8">
         <v>2006</v>
       </c>
@@ -8020,7 +8040,7 @@
         <v>671.66403600000001</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" ht="16">
       <c r="A9">
         <v>2007</v>
       </c>
@@ -8045,7 +8065,7 @@
       </c>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" ht="16">
       <c r="A10">
         <v>2008</v>
       </c>
@@ -8072,7 +8092,7 @@
       <c r="J10" s="2"/>
       <c r="L10" s="2"/>
     </row>
-    <row r="11" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" ht="16">
       <c r="A11">
         <v>2009</v>
       </c>
@@ -8100,7 +8120,7 @@
       <c r="L11" s="2"/>
       <c r="N11" s="2"/>
     </row>
-    <row r="12" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" ht="16">
       <c r="A12">
         <v>2010</v>
       </c>
@@ -8128,7 +8148,7 @@
       <c r="L12" s="2"/>
       <c r="N12" s="2"/>
     </row>
-    <row r="13" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" ht="16">
       <c r="A13">
         <v>2011</v>
       </c>
@@ -8156,7 +8176,7 @@
       <c r="L13" s="2"/>
       <c r="N13" s="2"/>
     </row>
-    <row r="14" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" ht="16">
       <c r="A14">
         <v>2012</v>
       </c>
@@ -8185,7 +8205,7 @@
       <c r="L14" s="2"/>
       <c r="N14" s="2"/>
     </row>
-    <row r="15" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" ht="16">
       <c r="A15">
         <v>2013</v>
       </c>
@@ -8213,7 +8233,7 @@
       <c r="L15" s="2"/>
       <c r="N15" s="2"/>
     </row>
-    <row r="16" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" ht="16">
       <c r="A16">
         <v>2014</v>
       </c>
@@ -8241,7 +8261,7 @@
       <c r="L16" s="2"/>
       <c r="N16" s="2"/>
     </row>
-    <row r="17" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" ht="16">
       <c r="A17">
         <v>2015</v>
       </c>
@@ -8269,7 +8289,7 @@
       <c r="L17" s="2"/>
       <c r="N17" s="2"/>
     </row>
-    <row r="18" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" ht="16">
       <c r="A18">
         <v>2016</v>
       </c>
@@ -8297,7 +8317,7 @@
       <c r="L18" s="2"/>
       <c r="N18" s="2"/>
     </row>
-    <row r="19" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" ht="16">
       <c r="A19">
         <v>2017</v>
       </c>
@@ -8325,7 +8345,7 @@
       <c r="L19" s="2"/>
       <c r="N19" s="2"/>
     </row>
-    <row r="20" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" ht="16">
       <c r="A20">
         <v>2018</v>
       </c>
@@ -8353,7 +8373,7 @@
       <c r="L20" s="2"/>
       <c r="N20" s="2"/>
     </row>
-    <row r="21" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" ht="16">
       <c r="A21">
         <v>2019</v>
       </c>
@@ -8380,19 +8400,19 @@
       <c r="J21" s="2"/>
       <c r="N21" s="2"/>
     </row>
-    <row r="22" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" ht="16">
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" ht="16">
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" ht="16">
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" ht="16">
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" ht="16">
       <c r="H26" s="2"/>
     </row>
   </sheetData>
@@ -8408,76 +8428,86 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63DF787E-9CE6-4767-AADB-C0D49F24A7F3}">
-  <dimension ref="A1:Q25"/>
+  <dimension ref="A1:Q41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17">
       <c r="B1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="F1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="G1" t="s">
+        <v>205</v>
+      </c>
+      <c r="H1" t="s">
+        <v>356</v>
+      </c>
+      <c r="L1" t="s">
+        <v>192</v>
+      </c>
+      <c r="M1" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="A2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="C2" t="s">
+        <v>352</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="L1" t="s">
-        <v>194</v>
-      </c>
-      <c r="M1" t="s">
-        <v>194</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>182</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="C2" t="s">
-        <v>355</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="F2" s="1"/>
+      <c r="E2" t="s">
+        <v>354</v>
+      </c>
+      <c r="F2" t="s">
+        <v>354</v>
+      </c>
+      <c r="H2" t="s">
+        <v>357</v>
+      </c>
       <c r="L2" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="M2" s="42"/>
       <c r="Q2" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
       <c r="A3">
         <v>2001</v>
       </c>
-      <c r="B3">
-        <f>B4*D3/D4</f>
-        <v>2.6211738386810759</v>
+      <c r="B3" s="42">
+        <v>3.7280000000000002</v>
       </c>
       <c r="C3">
         <v>32158607.714417279</v>
@@ -8485,6 +8515,15 @@
       <c r="D3">
         <v>2.56</v>
       </c>
+      <c r="E3">
+        <v>0.94684931506849312</v>
+      </c>
+      <c r="F3">
+        <v>3.506849315068493</v>
+      </c>
+      <c r="H3" s="42">
+        <v>3.7280000000000002</v>
+      </c>
       <c r="L3">
         <v>13566761.083007999</v>
       </c>
@@ -8495,13 +8534,12 @@
         <v>11873993.704704</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17">
       <c r="A4">
         <v>2002</v>
       </c>
-      <c r="B4">
-        <f>B5*D4/D5</f>
-        <v>2.6109348783737278</v>
+      <c r="B4" s="42">
+        <v>3.3620000000000001</v>
       </c>
       <c r="C4">
         <v>34756129.686718091</v>
@@ -8509,6 +8547,15 @@
       <c r="D4">
         <v>2.5499999999999998</v>
       </c>
+      <c r="E4">
+        <v>1.0415492957746479</v>
+      </c>
+      <c r="F4">
+        <v>3.591549295774648</v>
+      </c>
+      <c r="H4" s="42">
+        <v>3.3620000000000001</v>
+      </c>
       <c r="L4">
         <v>15261925.167299999</v>
       </c>
@@ -8519,12 +8566,12 @@
         <v>13567145.704704</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17">
       <c r="A5">
         <v>2003</v>
       </c>
-      <c r="B5">
-        <v>2.6006959180663798</v>
+      <c r="B5" s="42">
+        <v>3.206</v>
       </c>
       <c r="C5">
         <v>38240248.805773944</v>
@@ -8532,6 +8579,15 @@
       <c r="D5">
         <v>2.54</v>
       </c>
+      <c r="E5">
+        <v>1.0885714285714287</v>
+      </c>
+      <c r="F5">
+        <v>3.628571428571429</v>
+      </c>
+      <c r="H5" s="42">
+        <v>3.206</v>
+      </c>
       <c r="L5">
         <v>17508670.647999998</v>
       </c>
@@ -8542,12 +8598,12 @@
         <v>15252034.346915999</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17">
       <c r="A6">
         <v>2004</v>
       </c>
-      <c r="B6">
-        <v>3.0508626846620399</v>
+      <c r="B6" s="42">
+        <v>3.512</v>
       </c>
       <c r="C6">
         <v>33392445.494627818</v>
@@ -8555,6 +8611,15 @@
       <c r="D6">
         <v>2.42</v>
       </c>
+      <c r="E6">
+        <v>1.0371428571428571</v>
+      </c>
+      <c r="F6">
+        <v>3.4571428571428573</v>
+      </c>
+      <c r="H6" s="42">
+        <v>3.512</v>
+      </c>
       <c r="L6">
         <v>19169570.399</v>
       </c>
@@ -8565,12 +8630,12 @@
         <v>15749019.786006</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17">
       <c r="A7">
         <v>2005</v>
       </c>
-      <c r="B7">
-        <v>3.1113771591266901</v>
+      <c r="B7" s="42">
+        <v>3.7450000000000001</v>
       </c>
       <c r="C7">
         <v>33248775.81758856</v>
@@ -8578,6 +8643,15 @@
       <c r="D7">
         <v>2.48</v>
       </c>
+      <c r="E7">
+        <v>0.91726027397260279</v>
+      </c>
+      <c r="F7">
+        <v>3.397260273972603</v>
+      </c>
+      <c r="H7" s="42">
+        <v>3.7450000000000001</v>
+      </c>
       <c r="L7">
         <v>20163133.2084</v>
       </c>
@@ -8588,12 +8662,12 @@
         <v>15122391.179784</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17">
       <c r="A8">
         <v>2006</v>
       </c>
-      <c r="B8">
-        <v>3.09207937561865</v>
+      <c r="B8" s="42">
+        <v>3.4239999999999999</v>
       </c>
       <c r="C8">
         <v>30743276.91313928</v>
@@ -8601,6 +8675,15 @@
       <c r="D8">
         <v>2.37</v>
       </c>
+      <c r="E8">
+        <v>1.2761538461538462</v>
+      </c>
+      <c r="F8">
+        <v>3.6461538461538461</v>
+      </c>
+      <c r="H8" s="42">
+        <v>3.4239999999999999</v>
+      </c>
       <c r="L8">
         <v>26549874.226400003</v>
       </c>
@@ -8611,12 +8694,12 @@
         <v>20608702.998528</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17">
       <c r="A9">
         <v>2007</v>
       </c>
-      <c r="B9">
-        <v>3.1150351404490899</v>
+      <c r="B9" s="42">
+        <v>3.552</v>
       </c>
       <c r="C9">
         <v>30864252.603043139</v>
@@ -8624,6 +8707,15 @@
       <c r="D9">
         <v>2.35</v>
       </c>
+      <c r="E9">
+        <v>1.1574626865671642</v>
+      </c>
+      <c r="F9">
+        <v>3.5074626865671643</v>
+      </c>
+      <c r="H9" s="42">
+        <v>3.552</v>
+      </c>
       <c r="L9">
         <v>29720363.140299998</v>
       </c>
@@ -8634,12 +8726,12 @@
         <v>23289317.400419999</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17">
       <c r="A10">
         <v>2008</v>
       </c>
-      <c r="B10">
-        <v>3.7342289806146298</v>
+      <c r="B10" s="42">
+        <v>3.806</v>
       </c>
       <c r="C10">
         <v>35319609.12352629</v>
@@ -8647,7 +8739,15 @@
       <c r="D10">
         <v>2.2799999999999998</v>
       </c>
-      <c r="H10" s="41"/>
+      <c r="E10">
+        <v>1.4577049180327868</v>
+      </c>
+      <c r="F10">
+        <v>3.7377049180327866</v>
+      </c>
+      <c r="H10" s="42">
+        <v>3.806</v>
+      </c>
       <c r="L10">
         <v>35897191.008000001</v>
       </c>
@@ -8658,12 +8758,12 @@
         <v>26830921.217274003</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17">
       <c r="A11">
         <v>2009</v>
       </c>
-      <c r="B11">
-        <v>3.6116350854505699</v>
+      <c r="B11" s="42">
+        <v>3.6116350000000002</v>
       </c>
       <c r="C11">
         <v>38898966.518224157</v>
@@ -8671,7 +8771,15 @@
       <c r="D11">
         <v>2.46</v>
       </c>
-      <c r="H11" s="41"/>
+      <c r="E11">
+        <v>1.7813793103448277</v>
+      </c>
+      <c r="F11">
+        <v>4.2413793103448274</v>
+      </c>
+      <c r="H11" s="42">
+        <v>3.6116350000000002</v>
+      </c>
       <c r="L11">
         <v>40098416.945999995</v>
       </c>
@@ -8682,11 +8790,11 @@
         <v>35094737.355630003</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17">
       <c r="A12">
         <v>2010</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="42">
         <v>4.1711999999999998</v>
       </c>
       <c r="C12">
@@ -8695,7 +8803,15 @@
       <c r="D12">
         <v>2.7545000000000002</v>
       </c>
-      <c r="H12" s="41"/>
+      <c r="E12">
+        <v>1.6710719654124919</v>
+      </c>
+      <c r="F12">
+        <v>4.4255719654124919</v>
+      </c>
+      <c r="H12" s="42">
+        <v>4.1711999999999998</v>
+      </c>
       <c r="L12">
         <v>49760044.376000002</v>
       </c>
@@ -8706,11 +8822,11 @@
         <v>42975239.260650001</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17">
       <c r="A13">
         <v>2011</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="42">
         <v>4.7247000000000003</v>
       </c>
       <c r="C13">
@@ -8719,7 +8835,15 @@
       <c r="D13">
         <v>2.8769</v>
       </c>
-      <c r="H13" s="41"/>
+      <c r="E13">
+        <v>1.6260682952887595</v>
+      </c>
+      <c r="F13">
+        <v>4.5029682952887597</v>
+      </c>
+      <c r="H13" s="42">
+        <v>4.7247000000000003</v>
+      </c>
       <c r="L13">
         <v>61920552.217999995</v>
       </c>
@@ -8730,11 +8854,11 @@
         <v>53778977.547102004</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17">
       <c r="A14">
         <v>2012</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="42">
         <v>4.6726999999999999</v>
       </c>
       <c r="C14">
@@ -8743,7 +8867,15 @@
       <c r="D14">
         <v>2.9571999999999998</v>
       </c>
-      <c r="H14" s="41"/>
+      <c r="E14">
+        <v>1.636490651685955</v>
+      </c>
+      <c r="F14">
+        <v>4.5936906516859546</v>
+      </c>
+      <c r="H14" s="42">
+        <v>4.6726999999999999</v>
+      </c>
       <c r="L14">
         <v>64372413.721000001</v>
       </c>
@@ -8754,11 +8886,11 @@
         <v>56518569.477336004</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17">
       <c r="A15">
         <v>2013</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="42">
         <v>4.5137</v>
       </c>
       <c r="C15">
@@ -8767,7 +8899,15 @@
       <c r="D15">
         <v>3.1667999999999998</v>
       </c>
-      <c r="H15" s="41"/>
+      <c r="E15">
+        <v>1.1952304507245022</v>
+      </c>
+      <c r="F15">
+        <v>4.362030450724502</v>
+      </c>
+      <c r="H15" s="42">
+        <v>4.5137</v>
+      </c>
       <c r="L15">
         <v>53626494.270999998</v>
       </c>
@@ -8778,11 +8918,11 @@
         <v>45537007.619892001</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17">
       <c r="A16">
         <v>2014</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="42">
         <v>4.4260999999999999</v>
       </c>
       <c r="C16">
@@ -8791,7 +8931,15 @@
       <c r="D16">
         <v>3.2705000000000002</v>
       </c>
-      <c r="H16" s="41"/>
+      <c r="E16">
+        <v>1.1295000626595046</v>
+      </c>
+      <c r="F16">
+        <v>4.4000000626595046</v>
+      </c>
+      <c r="H16" s="42">
+        <v>4.4260999999999999</v>
+      </c>
       <c r="L16">
         <v>47384090.369000003</v>
       </c>
@@ -8802,11 +8950,11 @@
         <v>39909789.610542007</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17">
       <c r="A17">
         <v>2015</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="42">
         <v>4.3685</v>
       </c>
       <c r="C17">
@@ -8815,7 +8963,15 @@
       <c r="D17">
         <v>3.3662999999999998</v>
       </c>
-      <c r="H17" s="41"/>
+      <c r="E17">
+        <v>1.0668016412034791</v>
+      </c>
+      <c r="F17">
+        <v>4.4331016412034785</v>
+      </c>
+      <c r="H17" s="42">
+        <v>4.3685</v>
+      </c>
       <c r="L17">
         <v>43305191.195</v>
       </c>
@@ -8826,11 +8982,11 @@
         <v>40209714.238356002</v>
       </c>
     </row>
-    <row r="18" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17">
       <c r="A18">
         <v>2016</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="42">
         <v>4.3914</v>
       </c>
       <c r="C18">
@@ -8839,7 +8995,15 @@
       <c r="D18">
         <v>3.5173000000000001</v>
       </c>
-      <c r="H18" s="41"/>
+      <c r="E18">
+        <v>1.2321408911587837</v>
+      </c>
+      <c r="F18">
+        <v>4.749440891158784</v>
+      </c>
+      <c r="H18" s="42">
+        <v>4.3914</v>
+      </c>
       <c r="L18">
         <v>46124315.173999995</v>
       </c>
@@ -8850,11 +9014,11 @@
         <v>43624963.306727998</v>
       </c>
     </row>
-    <row r="19" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17">
       <c r="A19">
         <v>2017</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="42">
         <v>4.2782999999999998</v>
       </c>
       <c r="C19">
@@ -8863,7 +9027,15 @@
       <c r="D19">
         <v>3.5678000000000001</v>
       </c>
-      <c r="H19" s="41"/>
+      <c r="E19">
+        <v>1.112318600152481</v>
+      </c>
+      <c r="F19">
+        <v>4.6801186001524808</v>
+      </c>
+      <c r="H19" s="42">
+        <v>4.2782999999999998</v>
+      </c>
       <c r="L19">
         <v>45451976.520999998</v>
       </c>
@@ -8874,11 +9046,11 @@
         <v>42306183.016679995</v>
       </c>
     </row>
-    <row r="20" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17">
       <c r="A20">
         <v>2018</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="42">
         <v>4.4542999999999999</v>
       </c>
       <c r="C20">
@@ -8887,7 +9059,15 @@
       <c r="D20">
         <v>3.6536</v>
       </c>
-      <c r="H20" s="41"/>
+      <c r="E20">
+        <v>1.1317010124660076</v>
+      </c>
+      <c r="F20">
+        <v>4.7853010124660074</v>
+      </c>
+      <c r="H20" s="42">
+        <v>4.4542999999999999</v>
+      </c>
       <c r="L20">
         <v>44895298.035000004</v>
       </c>
@@ -8898,11 +9078,11 @@
         <v>40434691.598711997</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17">
       <c r="A21">
         <v>2019</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="42">
         <v>4.3593999999999999</v>
       </c>
       <c r="C21">
@@ -8912,7 +9092,15 @@
       <c r="D21">
         <v>3.5962000000000001</v>
       </c>
-      <c r="H21" s="41"/>
+      <c r="E21">
+        <v>1.2756181422894106</v>
+      </c>
+      <c r="F21">
+        <v>4.8718181422894107</v>
+      </c>
+      <c r="H21" s="42">
+        <v>4.3593999999999999</v>
+      </c>
       <c r="L21">
         <v>52976451.681300007</v>
       </c>
@@ -8924,17 +9112,68 @@
         <v>47712936.086480156</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" ht="19">
       <c r="H22" s="41"/>
     </row>
-    <row r="23" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" ht="19">
+      <c r="C23" s="43"/>
       <c r="H23" s="41"/>
     </row>
-    <row r="24" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" ht="19">
+      <c r="C24" s="43"/>
       <c r="H24" s="41"/>
     </row>
-    <row r="25" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" ht="19">
+      <c r="C25" s="43"/>
       <c r="H25" s="41"/>
+    </row>
+    <row r="26" spans="1:17">
+      <c r="C26" s="43"/>
+    </row>
+    <row r="27" spans="1:17">
+      <c r="C27" s="43"/>
+    </row>
+    <row r="28" spans="1:17">
+      <c r="C28" s="43"/>
+    </row>
+    <row r="29" spans="1:17">
+      <c r="C29" s="43"/>
+    </row>
+    <row r="30" spans="1:17">
+      <c r="C30" s="43"/>
+    </row>
+    <row r="31" spans="1:17">
+      <c r="C31" s="43"/>
+    </row>
+    <row r="32" spans="1:17">
+      <c r="C32" s="43"/>
+    </row>
+    <row r="33" spans="3:3">
+      <c r="C33" s="43"/>
+    </row>
+    <row r="34" spans="3:3">
+      <c r="C34" s="43"/>
+    </row>
+    <row r="35" spans="3:3">
+      <c r="C35" s="43"/>
+    </row>
+    <row r="36" spans="3:3">
+      <c r="C36" s="43"/>
+    </row>
+    <row r="37" spans="3:3">
+      <c r="C37" s="43"/>
+    </row>
+    <row r="38" spans="3:3">
+      <c r="C38" s="43"/>
+    </row>
+    <row r="39" spans="3:3">
+      <c r="C39" s="43"/>
+    </row>
+    <row r="40" spans="3:3">
+      <c r="C40" s="43"/>
+    </row>
+    <row r="41" spans="3:3">
+      <c r="C41" s="43"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8949,11 +9188,11 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -8967,7 +9206,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8981,11 +9220,11 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -8999,7 +9238,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9011,7 +9250,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update nickel, unit error
</commit_message>
<xml_diff>
--- a/data/case study data.xlsx
+++ b/data/case study data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnryter/Dropbox (MIT)/John MIT/Research/generalizationOutside/generalization/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{945CB609-705E-A340-B6E3-C31CC35395D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{136B49C9-915F-C946-9C7C-630C1E7A66F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" xr2:uid="{9C1DBEC5-9C42-494B-AEAA-1D89B674AD0D}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" activeTab="8" xr2:uid="{9C1DBEC5-9C42-494B-AEAA-1D89B674AD0D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="17" r:id="rId1"/>
@@ -4023,9 +4023,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AAEEA05-303F-4351-9872-7B8EAAB6CD92}">
   <dimension ref="A1:AL74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AL22" sqref="AL22"/>
+      <selection pane="bottomLeft" activeCell="L35" sqref="L35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -7118,7 +7118,7 @@
         <v>30613</v>
       </c>
       <c r="L35">
-        <v>2721000</v>
+        <v>3461.4</v>
       </c>
       <c r="M35">
         <v>31968.75</v>
@@ -15243,8 +15243,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3A510BC-6699-4D7F-A1BA-2D5B6A269B1B}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Making train-test split years possible
</commit_message>
<xml_diff>
--- a/data/case study data.xlsx
+++ b/data/case study data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnryter/Dropbox (MIT)/John MIT/Research/generalizationOutside/generalization/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{136B49C9-915F-C946-9C7C-630C1E7A66F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF5C5F8C-063E-5147-A73B-A3B122D7F66E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" activeTab="8" xr2:uid="{9C1DBEC5-9C42-494B-AEAA-1D89B674AD0D}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16040" activeTab="3" xr2:uid="{9C1DBEC5-9C42-494B-AEAA-1D89B674AD0D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="17" r:id="rId1"/>
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="430">
   <si>
     <t>Al</t>
   </si>
@@ -528,12 +528,6 @@
     <t>Highly alloyed: https://www.gold.org/about-gold/about-gold-jewellery, 1% price increase increases recycled supply by 0.6%, page 6: https://www.gold.org/goldhub/research/ups-and-downs-gold-recycling</t>
   </si>
   <si>
-    <t>Cu, Ni, self</t>
-  </si>
-  <si>
-    <t>Sn, self</t>
-  </si>
-  <si>
     <t>World Gold Council https://www.gold.org/goldhub/data/gold-production-by-country</t>
   </si>
   <si>
@@ -1336,6 +1330,51 @@
   </si>
   <si>
     <t>Total minus primary</t>
+  </si>
+  <si>
+    <t>Fit a lognormal distribution such that the min/max would be 0.12-0.2, as described by http://news.chinatungsten.com/en/tungsten-information/95194-ti-12232.html#:~:text=Tungsten%20ore%20grade%20is%20tungsten%20trioxide%20%28WO3%29%20content,ore%2C%20low%20grade%20one%20is%20called%20poor%20ore. Worth noting that grades and prices for tungsten are in WO3 equivalent. Additional concern - highest grade is mentioned to be 1.9%, with many high-grade ores 0.7%. Generally confirmed by https://www.911metallurgist.com/blog/tungsten-metallurgy</t>
+  </si>
+  <si>
+    <t>kt W</t>
+  </si>
+  <si>
+    <t>kt WO3</t>
+  </si>
+  <si>
+    <t>t W</t>
+  </si>
+  <si>
+    <t>https://www.usgs.gov/media/files/tungsten-historical-statistics-data-series-140, using 0.793 W fraction of WO3 to convert from W content to WO3</t>
+  </si>
+  <si>
+    <t>Barruecopardo mine in Spain is ~1.5 kt/yr (https://www.refractorymetal.org/barruecopardo-tungsten-mine/), two different mines claiming to be the largest at 5% of global production (5.285) (https://almonty.com/2020/11/04/construction-of-the-worlds-largest-tungsten-mine-has-begun/#GmediaGallery_35-all-0, https://miningdigital.com/smart-mining/masan-resources-nui-phao-mine-worlds-largest-tungsten-mine), the one claims 30% but I assume they mean 30% of ex-China, dolphin would be 2.92 kt WO3 (https://www.mining-technology.com/projects/dolphin-tungsten-project/, reserve grade 0.73%*400 kt/yr capacity), Drakelands is producing 5 kt concentrate at 65% WO3 so 3.25 kt/yr (https://www.mining-technology.com/projects/hemerdon-ball/), la parilla is 2.5 kt/yr concentrate at 60% WO3 so 1.5 kt WO3 (https://www.mining-technology.com/projects/la-parrilla-tungsten-mine/), Molyhill expected to product 1.24 kt/yr WO3 from 0.31% grade and 400 kt ore/yr (https://www.mining-technology.com/projects/molyhil-tungsten-molybdenum-project-australia/), Sisson will be 5.57 kt APT/yr so 4.95 kt WO3 (https://www.mining-technology.com/projects/sisson-tungsten-molybdenum-project-new-brunswick/, W is 70.4%wt in APT, 79.3%wt of WO3). Values determined by making a distribution from the values reported here and appending a uniform distribution (0,1.5) such that the total sum matched 2019 mine production, then visually fitting a lognromal distribution to the resulting distribution with the same number of data points.</t>
+  </si>
+  <si>
+    <t>61% Cu, rem. Self</t>
+  </si>
+  <si>
+    <t>20% Cu, 13% Au, 35% Pb/Zn, 32% Ag</t>
+  </si>
+  <si>
+    <t>2% Pb, 5% Ni, 0.1% Ag, 92.9% Cu</t>
+  </si>
+  <si>
+    <t>35% Cu, 50% Ni, 15% Co</t>
+  </si>
+  <si>
+    <t>12% Cu, 0.5% Ag, 0.1% Ni, 1% Pb/Zn, 0.32% PGM, 86.08% Au</t>
+  </si>
+  <si>
+    <t>33% Sn, 27% Nb, 40% Ta</t>
+  </si>
+  <si>
+    <t>8% Pb, 77% Cu, 15% Te</t>
+  </si>
+  <si>
+    <t>4% Cu, 2% Au, 3% Ag, 91% Zn</t>
+  </si>
+  <si>
+    <t>Fu et al. 2018. High-resolution insight into material criticality: quantifying risk for byproduct metals, https://onlinelibrary.wiley.com/action/downloadSupplement?doi=10.1111%2Fjiec.12757&amp;file=jiec12757-sup-0001-SuppMat.pdf</t>
   </si>
 </sst>
 </file>
@@ -1347,7 +1386,7 @@
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1440,6 +1479,11 @@
       <name val="Times"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1460,12 +1504,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -1474,7 +1533,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1534,6 +1593,10 @@
     <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="justify"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -4023,9 +4086,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AAEEA05-303F-4351-9872-7B8EAAB6CD92}">
   <dimension ref="A1:AL74"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L35" sqref="L35"/>
+      <selection pane="bottomLeft" activeCell="Z5" sqref="Z5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -4056,10 +4119,10 @@
   <sheetData>
     <row r="1" spans="1:38" s="28" customFormat="1" ht="34" customHeight="1">
       <c r="A1" s="28" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C1" s="28" t="s">
         <v>0</v>
@@ -4107,7 +4170,7 @@
         <v>94</v>
       </c>
       <c r="R1" s="29" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="S1" s="28" t="s">
         <v>95</v>
@@ -4167,7 +4230,7 @@
         <v>108</v>
       </c>
       <c r="AL1" s="28" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="2" spans="1:38" ht="14.5" customHeight="1">
@@ -4175,7 +4238,7 @@
         <v>9</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>10</v>
@@ -4184,10 +4247,10 @@
         <v>10</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>10</v>
+        <v>425</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>147</v>
+        <v>424</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>11</v>
@@ -4199,22 +4262,30 @@
         <v>10</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>148</v>
+        <v>426</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>10</v>
+        <v>423</v>
       </c>
       <c r="L2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
+      <c r="M2" s="5" t="s">
+        <v>422</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>428</v>
+      </c>
       <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
+      <c r="P2" s="5" t="s">
+        <v>421</v>
+      </c>
       <c r="Q2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="R2" s="14"/>
+      <c r="R2" s="14" t="s">
+        <v>427</v>
+      </c>
       <c r="S2" s="5" t="s">
         <v>10</v>
       </c>
@@ -4225,29 +4296,43 @@
       <c r="V2" s="6"/>
       <c r="W2" s="6"/>
       <c r="X2" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="Y2" s="6"/>
+        <v>429</v>
+      </c>
+      <c r="Y2" s="6" t="s">
+        <v>429</v>
+      </c>
       <c r="Z2" s="6"/>
       <c r="AA2" s="6"/>
       <c r="AB2" s="6"/>
-      <c r="AC2" s="6"/>
-      <c r="AD2" s="6"/>
+      <c r="AC2" s="6" t="s">
+        <v>429</v>
+      </c>
+      <c r="AD2" s="6" t="s">
+        <v>429</v>
+      </c>
       <c r="AE2" s="6"/>
-      <c r="AF2" s="6"/>
-      <c r="AG2" s="6"/>
+      <c r="AF2" s="6" t="s">
+        <v>429</v>
+      </c>
+      <c r="AG2" s="6" t="s">
+        <v>429</v>
+      </c>
       <c r="AH2" s="6"/>
-      <c r="AI2" s="6"/>
+      <c r="AI2" s="6" t="s">
+        <v>429</v>
+      </c>
       <c r="AJ2" s="6"/>
       <c r="AK2" s="6"/>
-      <c r="AL2" s="6"/>
+      <c r="AL2" s="6" t="s">
+        <v>429</v>
+      </c>
     </row>
     <row r="3" spans="1:38" ht="14.5" customHeight="1">
       <c r="A3" t="s">
         <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C3">
         <v>99671</v>
@@ -4301,41 +4386,43 @@
         <v>18</v>
       </c>
       <c r="V3" s="7" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="W3" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="X3" s="7"/>
+      <c r="X3" s="6" t="s">
+        <v>146</v>
+      </c>
       <c r="Y3" s="7"/>
       <c r="Z3" s="7"/>
       <c r="AA3" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="AB3" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="AC3" s="17" t="s">
         <v>200</v>
-      </c>
-      <c r="AB3" s="7" t="s">
-        <v>201</v>
-      </c>
-      <c r="AC3" s="17" t="s">
-        <v>202</v>
       </c>
       <c r="AD3" s="7"/>
       <c r="AE3" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="AF3" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="AG3" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="AF3" s="17" t="s">
+      <c r="AH3" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="AG3" s="7" t="s">
+      <c r="AI3" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="AH3" s="7" t="s">
+      <c r="AJ3" s="7" t="s">
         <v>206</v>
-      </c>
-      <c r="AI3" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="AJ3" s="7" t="s">
-        <v>208</v>
       </c>
       <c r="AK3" s="7"/>
       <c r="AL3" s="7"/>
@@ -4345,7 +4432,7 @@
         <v>19</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -4383,7 +4470,7 @@
       <c r="AB4" s="6"/>
       <c r="AC4" s="6"/>
       <c r="AD4" s="6" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="AE4" s="6"/>
       <c r="AF4" s="6"/>
@@ -4399,7 +4486,7 @@
         <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C5">
         <v>0.04</v>
@@ -4450,43 +4537,43 @@
         <v>21</v>
       </c>
       <c r="V5" s="7" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="W5" s="7" t="s">
         <v>132</v>
       </c>
       <c r="X5" s="7" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="Y5" s="7"/>
       <c r="Z5" s="7"/>
       <c r="AA5" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="AB5" s="17" t="s">
+        <v>209</v>
+      </c>
+      <c r="AC5" s="7" t="s">
         <v>210</v>
-      </c>
-      <c r="AB5" s="17" t="s">
-        <v>211</v>
-      </c>
-      <c r="AC5" s="7" t="s">
-        <v>212</v>
       </c>
       <c r="AD5" s="7"/>
       <c r="AE5" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="AF5" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="AG5" s="35" t="s">
+        <v>335</v>
+      </c>
+      <c r="AH5" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="AF5" s="7" t="s">
+      <c r="AI5" s="7" t="s">
         <v>214</v>
       </c>
-      <c r="AG5" s="35" t="s">
-        <v>337</v>
-      </c>
-      <c r="AH5" s="7" t="s">
+      <c r="AJ5" s="7" t="s">
         <v>215</v>
-      </c>
-      <c r="AI5" s="7" t="s">
-        <v>216</v>
-      </c>
-      <c r="AJ5" s="7" t="s">
-        <v>217</v>
       </c>
       <c r="AK5" s="7"/>
       <c r="AL5" s="7"/>
@@ -4496,7 +4583,7 @@
         <v>25</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C6" s="5">
         <v>0.45100000000000001</v>
@@ -4549,49 +4636,49 @@
       </c>
       <c r="U6" s="6"/>
       <c r="V6" s="6" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="W6" s="6" t="s">
         <v>131</v>
       </c>
       <c r="X6" s="6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="Y6" s="6"/>
       <c r="Z6" s="6"/>
       <c r="AA6" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="AB6" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="AC6" s="6" t="s">
         <v>218</v>
-      </c>
-      <c r="AB6" s="6" t="s">
-        <v>219</v>
-      </c>
-      <c r="AC6" s="6" t="s">
-        <v>220</v>
       </c>
       <c r="AD6" s="6" t="s">
         <v>78</v>
       </c>
       <c r="AE6" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="AF6" s="6" t="s">
+        <v>336</v>
+      </c>
+      <c r="AG6" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="AH6" s="19" t="s">
+        <v>325</v>
+      </c>
+      <c r="AI6" s="6" t="s">
         <v>221</v>
       </c>
-      <c r="AF6" s="6" t="s">
-        <v>338</v>
-      </c>
-      <c r="AG6" s="6" t="s">
-        <v>222</v>
-      </c>
-      <c r="AH6" s="19" t="s">
-        <v>327</v>
-      </c>
-      <c r="AI6" s="6" t="s">
-        <v>223</v>
-      </c>
       <c r="AJ6" s="35" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="AK6" s="6"/>
       <c r="AL6" s="35" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="7" spans="1:38" ht="14.5" customHeight="1">
@@ -4599,7 +4686,7 @@
         <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C7">
         <v>0.251</v>
@@ -4654,7 +4741,7 @@
       </c>
       <c r="U7" s="7"/>
       <c r="V7" s="7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="W7" s="7" t="s">
         <v>131</v>
@@ -4665,38 +4752,38 @@
       <c r="Y7" s="7"/>
       <c r="Z7" s="7"/>
       <c r="AA7" s="7" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="AB7" s="1" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="AC7" s="7" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="AD7" s="7" t="s">
         <v>78</v>
       </c>
       <c r="AE7" s="1" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="AF7" s="17" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="AG7" s="17" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="AH7" s="17" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="AI7" s="7" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="AJ7" s="7" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AK7" s="7"/>
       <c r="AL7" s="7" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="8" spans="1:38" ht="14.5" customHeight="1">
@@ -4704,7 +4791,7 @@
         <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C8" s="5">
         <v>0.11899999999999999</v>
@@ -4759,7 +4846,7 @@
       </c>
       <c r="U8" s="6"/>
       <c r="V8" s="6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="W8" s="6" t="s">
         <v>131</v>
@@ -4770,13 +4857,13 @@
       <c r="Y8" s="6"/>
       <c r="Z8" s="6"/>
       <c r="AA8" s="6" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="AB8" s="1" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="AC8" s="6" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="AD8" s="6" t="s">
         <v>78</v>
@@ -4786,7 +4873,7 @@
       <c r="AG8" s="6"/>
       <c r="AH8" s="6"/>
       <c r="AI8" s="6" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="AJ8" s="6"/>
       <c r="AK8" s="6"/>
@@ -4797,7 +4884,7 @@
         <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C9">
         <v>0.11899999999999999</v>
@@ -4851,7 +4938,7 @@
       </c>
       <c r="U9" s="7"/>
       <c r="V9" s="7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="W9" s="7" t="s">
         <v>131</v>
@@ -4862,25 +4949,25 @@
       <c r="Y9" s="7"/>
       <c r="Z9" s="7"/>
       <c r="AA9" s="7" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="AB9" s="1" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="AC9" s="7" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="AD9" s="7" t="s">
         <v>78</v>
       </c>
       <c r="AE9" s="7"/>
       <c r="AF9" s="7" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="AG9" s="7"/>
       <c r="AH9" s="7"/>
       <c r="AI9" s="7" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="AJ9" s="7"/>
       <c r="AK9" s="7"/>
@@ -4891,7 +4978,7 @@
         <v>29</v>
       </c>
       <c r="B10" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C10" s="5">
         <f>1-C11-C7-C9-C8</f>
@@ -4951,7 +5038,7 @@
       </c>
       <c r="U10" s="6"/>
       <c r="V10" s="6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="W10" s="6" t="s">
         <v>131</v>
@@ -4962,25 +5049,25 @@
       <c r="Y10" s="6"/>
       <c r="Z10" s="6"/>
       <c r="AA10" s="6" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="AB10" s="1" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="AC10" s="6" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="AD10" s="6" t="s">
         <v>78</v>
       </c>
       <c r="AE10" s="6"/>
       <c r="AF10" s="7" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="AG10" s="6"/>
       <c r="AH10" s="6"/>
       <c r="AI10" s="6" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="AJ10" s="6"/>
       <c r="AK10" s="6"/>
@@ -4991,7 +5078,7 @@
         <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C11">
         <v>0.27300000000000002</v>
@@ -5045,7 +5132,7 @@
       </c>
       <c r="U11" s="7"/>
       <c r="V11" s="7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="W11" s="7" t="s">
         <v>131</v>
@@ -5057,22 +5144,22 @@
       <c r="Z11" s="7"/>
       <c r="AA11" s="7"/>
       <c r="AB11" s="1" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="AC11" s="7" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="AD11" s="7" t="s">
         <v>78</v>
       </c>
       <c r="AE11" s="7"/>
       <c r="AF11" s="7" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="AG11" s="7"/>
       <c r="AH11" s="7"/>
       <c r="AI11" s="7" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="AJ11" s="7"/>
       <c r="AK11" s="7"/>
@@ -5083,7 +5170,7 @@
         <v>96</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C12" s="5">
         <v>0.9</v>
@@ -5143,41 +5230,41 @@
         <v>129</v>
       </c>
       <c r="X12" s="6" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="Y12" s="6"/>
       <c r="Z12" s="6"/>
       <c r="AA12" s="6"/>
       <c r="AB12" s="6" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="AC12" s="6" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="AD12" s="6" t="s">
         <v>106</v>
       </c>
       <c r="AE12" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="AF12" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="AG12" s="6" t="s">
         <v>242</v>
       </c>
-      <c r="AF12" s="6" t="s">
+      <c r="AH12" s="6" t="s">
         <v>243</v>
       </c>
-      <c r="AG12" s="6" t="s">
+      <c r="AI12" s="6" t="s">
         <v>244</v>
       </c>
-      <c r="AH12" s="6" t="s">
-        <v>245</v>
-      </c>
-      <c r="AI12" s="6" t="s">
-        <v>246</v>
-      </c>
       <c r="AJ12" s="6" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AK12" s="6"/>
       <c r="AL12" s="6" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="13" spans="1:38" ht="14.5" customHeight="1">
@@ -5185,7 +5272,7 @@
         <v>97</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="C13">
         <v>0.95</v>
@@ -5243,7 +5330,7 @@
         <v>129</v>
       </c>
       <c r="X13" s="7" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="Y13" s="7"/>
       <c r="Z13" s="7"/>
@@ -5254,20 +5341,20 @@
         <v>106</v>
       </c>
       <c r="AE13" s="7" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="AF13" s="7" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="AG13" s="7"/>
       <c r="AH13" s="7"/>
       <c r="AI13" s="7" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="AJ13" s="7"/>
       <c r="AK13" s="7"/>
       <c r="AL13" s="7" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="14" spans="1:38" ht="14.5" customHeight="1">
@@ -5275,7 +5362,7 @@
         <v>98</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C14" s="5">
         <v>0.9</v>
@@ -5335,7 +5422,7 @@
         <v>129</v>
       </c>
       <c r="X14" s="6" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="Y14" s="6"/>
       <c r="Z14" s="6"/>
@@ -5353,7 +5440,7 @@
       <c r="AJ14" s="6"/>
       <c r="AK14" s="6"/>
       <c r="AL14" s="6" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="15" spans="1:38" ht="14.5" customHeight="1">
@@ -5361,7 +5448,7 @@
         <v>99</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C15">
         <v>0.95</v>
@@ -5442,7 +5529,7 @@
         <v>100</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C16" s="5">
         <v>0.9</v>
@@ -5518,7 +5605,7 @@
       <c r="AJ16" s="6"/>
       <c r="AK16" s="6"/>
       <c r="AL16" s="6" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="17" spans="1:38" ht="14.5" customHeight="1">
@@ -5526,7 +5613,7 @@
         <v>101</v>
       </c>
       <c r="B17" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C17">
         <v>50</v>
@@ -5585,37 +5672,37 @@
         <v>129</v>
       </c>
       <c r="X17" s="7" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="Y17" s="7"/>
       <c r="Z17" s="7"/>
       <c r="AA17" s="7"/>
       <c r="AB17" s="7" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="AC17" s="7" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="AD17" s="7" t="s">
         <v>106</v>
       </c>
       <c r="AE17" s="17" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="AF17" s="7" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="AG17" s="7" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="AH17" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="AI17" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="AJ17" s="7" t="s">
         <v>255</v>
-      </c>
-      <c r="AI17" s="7" t="s">
-        <v>256</v>
-      </c>
-      <c r="AJ17" s="7" t="s">
-        <v>257</v>
       </c>
       <c r="AK17" s="7"/>
       <c r="AL17" s="7"/>
@@ -5625,7 +5712,7 @@
         <v>102</v>
       </c>
       <c r="B18" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C18" s="5">
         <v>25</v>
@@ -5685,37 +5772,37 @@
         <v>129</v>
       </c>
       <c r="X18" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="Y18" s="6"/>
       <c r="Z18" s="6"/>
       <c r="AA18" s="19" t="s">
+        <v>256</v>
+      </c>
+      <c r="AB18" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="AC18" s="19" t="s">
         <v>258</v>
-      </c>
-      <c r="AB18" s="6" t="s">
-        <v>259</v>
-      </c>
-      <c r="AC18" s="19" t="s">
-        <v>260</v>
       </c>
       <c r="AD18" s="6" t="s">
         <v>106</v>
       </c>
       <c r="AE18" s="17" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="AF18" s="7" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="AG18" s="6" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="AH18" s="6"/>
       <c r="AI18" s="6" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="AJ18" s="6" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="AK18" s="6"/>
       <c r="AL18" s="6"/>
@@ -5725,7 +5812,7 @@
         <v>103</v>
       </c>
       <c r="B19" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C19">
         <v>20</v>
@@ -5784,7 +5871,7 @@
         <v>129</v>
       </c>
       <c r="X19" s="7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="Y19" s="7"/>
       <c r="Z19" s="7"/>
@@ -5795,22 +5882,22 @@
         <v>106</v>
       </c>
       <c r="AE19" s="17" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="AF19" s="7" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="AG19" s="7" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="AH19" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="AI19" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="AJ19" s="1" t="s">
         <v>264</v>
-      </c>
-      <c r="AI19" s="7" t="s">
-        <v>265</v>
-      </c>
-      <c r="AJ19" s="1" t="s">
-        <v>266</v>
       </c>
       <c r="AK19" s="7"/>
       <c r="AL19" s="7"/>
@@ -5820,7 +5907,7 @@
         <v>104</v>
       </c>
       <c r="B20" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C20" s="5">
         <v>15</v>
@@ -5874,12 +5961,12 @@
         <v>129</v>
       </c>
       <c r="X20" s="6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="Y20" s="6"/>
       <c r="Z20" s="6"/>
       <c r="AA20" s="6" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="AB20" s="6"/>
       <c r="AC20" s="6"/>
@@ -5887,16 +5974,16 @@
         <v>106</v>
       </c>
       <c r="AE20" s="17" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="AF20" s="7" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="AG20" s="6" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="AH20" s="6" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="AI20" s="6"/>
       <c r="AJ20" s="6"/>
@@ -5908,7 +5995,7 @@
         <v>105</v>
       </c>
       <c r="B21" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C21">
         <v>15</v>
@@ -5967,34 +6054,34 @@
         <v>129</v>
       </c>
       <c r="X21" s="7" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="Y21" s="7"/>
       <c r="Z21" s="7"/>
       <c r="AA21" s="7"/>
       <c r="AB21" s="7" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="AD21" s="7" t="s">
         <v>106</v>
       </c>
       <c r="AE21" s="17" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="AF21" s="7" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="AG21" s="7" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="AH21" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="AI21" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="AJ21" s="7" t="s">
         <v>269</v>
-      </c>
-      <c r="AI21" s="7" t="s">
-        <v>270</v>
-      </c>
-      <c r="AJ21" s="7" t="s">
-        <v>271</v>
       </c>
       <c r="AK21" s="7"/>
       <c r="AL21" s="7"/>
@@ -6004,7 +6091,7 @@
         <v>134</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C22" s="5">
         <v>0.64749999999999996</v>
@@ -6050,32 +6137,32 @@
       </c>
       <c r="U22" s="6"/>
       <c r="V22" s="6" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="W22" s="6"/>
       <c r="X22" s="6" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="Y22" s="6"/>
       <c r="AA22" s="7"/>
       <c r="AB22" s="17" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="AC22" s="5"/>
       <c r="AD22" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AE22" s="17" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="AF22" s="6" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="AG22" s="19" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="AH22" s="6" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="AI22" s="6"/>
       <c r="AJ22" s="6"/>
@@ -6087,7 +6174,7 @@
         <v>135</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="C23">
         <v>0.72899999999999998</v>
@@ -6128,32 +6215,32 @@
       </c>
       <c r="U23" s="7"/>
       <c r="V23" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="W23" s="7"/>
       <c r="X23" s="7" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="Y23" s="7"/>
       <c r="AA23" s="6"/>
       <c r="AB23" s="17" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="AC23" s="7"/>
       <c r="AD23" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AE23" s="17" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="AF23" s="6" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="AG23" s="19" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="AH23" s="6" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="AI23" s="7"/>
       <c r="AJ23" s="7"/>
@@ -6164,7 +6251,7 @@
         <v>136</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C24" s="5">
         <v>0.76690000000000003</v>
@@ -6210,32 +6297,32 @@
       </c>
       <c r="U24" s="6"/>
       <c r="V24" s="6" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="W24" s="6"/>
       <c r="X24" s="6" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="Y24" s="6"/>
       <c r="AA24" s="7"/>
       <c r="AB24" s="17" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="AC24" s="5"/>
       <c r="AD24" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AE24" s="17" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="AF24" s="6" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="AG24" s="19" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="AH24" s="6" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="AI24" s="6"/>
       <c r="AJ24" s="6"/>
@@ -6247,7 +6334,7 @@
         <v>137</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C25">
         <v>0.46850000000000003</v>
@@ -6288,31 +6375,31 @@
       </c>
       <c r="U25" s="7"/>
       <c r="V25" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="W25" s="7"/>
       <c r="X25" s="7" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="Y25" s="7"/>
       <c r="AA25" s="6"/>
       <c r="AB25" s="17" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="AD25" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AE25" s="17" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="AF25" s="6" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="AG25" s="19" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="AH25" s="6" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="AI25" s="7"/>
       <c r="AJ25" s="7"/>
@@ -6323,7 +6410,7 @@
         <v>138</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="C26" s="5">
         <v>0.75</v>
@@ -6369,31 +6456,31 @@
       </c>
       <c r="U26" s="6"/>
       <c r="V26" s="6" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="W26" s="6"/>
       <c r="X26" s="6" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="Y26" s="6"/>
       <c r="AA26" s="7"/>
       <c r="AB26" s="17" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="AD26" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AE26" s="17" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="AF26" s="6" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="AG26" s="19" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="AH26" s="1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="AI26" s="6"/>
       <c r="AJ26" s="6"/>
@@ -6405,7 +6492,7 @@
         <v>70</v>
       </c>
       <c r="B27" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C27">
         <v>0.34250000000000003</v>
@@ -6457,7 +6544,7 @@
         <v>71</v>
       </c>
       <c r="V27" s="7" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="W27" s="7" t="s">
         <v>128</v>
@@ -6468,23 +6555,23 @@
       <c r="Y27" s="7"/>
       <c r="Z27" s="7"/>
       <c r="AA27" s="17" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="AB27" s="7"/>
       <c r="AC27" s="17" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="AD27" s="7" t="s">
         <v>77</v>
       </c>
       <c r="AE27" s="7"/>
       <c r="AF27" s="7" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="AG27" s="7"/>
       <c r="AH27" s="7"/>
       <c r="AI27" s="7" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="AJ27" s="7"/>
       <c r="AK27" s="7"/>
@@ -6495,7 +6582,7 @@
         <v>69</v>
       </c>
       <c r="B28" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C28" s="5">
         <v>0.24399999999999999</v>
@@ -6547,7 +6634,7 @@
       </c>
       <c r="U28" s="6"/>
       <c r="V28" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="W28" s="6" t="s">
         <v>127</v>
@@ -6558,25 +6645,25 @@
       <c r="Y28" s="6"/>
       <c r="Z28" s="6"/>
       <c r="AA28" s="6" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="AB28" s="6"/>
       <c r="AC28" s="19" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="AD28" s="6" t="s">
         <v>77</v>
       </c>
       <c r="AE28" s="6"/>
       <c r="AF28" s="6" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="AG28" s="6" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="AH28" s="6"/>
       <c r="AI28" s="6" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="AJ28" s="6"/>
       <c r="AK28" s="6"/>
@@ -6587,7 +6674,7 @@
         <v>75</v>
       </c>
       <c r="B29" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -6671,7 +6758,7 @@
         <v>74</v>
       </c>
       <c r="B30" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C30" s="5">
         <v>0.57769999999999999</v>
@@ -6721,18 +6808,18 @@
       </c>
       <c r="U30" s="6"/>
       <c r="V30" s="6" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="W30" s="6" t="s">
         <v>131</v>
       </c>
       <c r="X30" s="6" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="Y30" s="6"/>
       <c r="Z30" s="6"/>
       <c r="AA30" s="19" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="AB30" s="6"/>
       <c r="AC30" s="6"/>
@@ -6740,13 +6827,13 @@
         <v>77</v>
       </c>
       <c r="AE30" s="6" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="AF30" s="6"/>
       <c r="AG30" s="6"/>
       <c r="AH30" s="6"/>
       <c r="AI30" s="22" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="AJ30" s="6"/>
       <c r="AK30" s="6"/>
@@ -6757,7 +6844,7 @@
         <v>72</v>
       </c>
       <c r="B31" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C31">
         <v>0</v>
@@ -6813,7 +6900,7 @@
         <v>130</v>
       </c>
       <c r="X31" s="7" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="Y31" s="7"/>
       <c r="Z31" s="7"/>
@@ -6825,7 +6912,7 @@
       </c>
       <c r="AE31" s="7"/>
       <c r="AF31" s="7" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="AG31" s="7"/>
       <c r="AH31" s="7"/>
@@ -6839,7 +6926,7 @@
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C32" s="5">
         <v>0</v>
@@ -6897,7 +6984,7 @@
         <v>130</v>
       </c>
       <c r="X32" s="7" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="Y32" s="6"/>
       <c r="Z32" s="6"/>
@@ -6909,12 +6996,12 @@
       </c>
       <c r="AE32" s="6"/>
       <c r="AF32" s="7" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="AG32" s="6"/>
       <c r="AH32" s="6"/>
       <c r="AI32" s="6" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="AJ32" s="6"/>
       <c r="AK32" s="6"/>
@@ -6925,7 +7012,7 @@
         <v>73</v>
       </c>
       <c r="B33" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C33">
         <v>0</v>
@@ -6985,24 +7072,24 @@
       <c r="AA33" s="7"/>
       <c r="AB33" s="7"/>
       <c r="AC33" s="7" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="AD33" s="7" t="s">
         <v>77</v>
       </c>
       <c r="AE33" s="7" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="AF33" s="7"/>
       <c r="AG33" s="7"/>
       <c r="AH33" s="7"/>
       <c r="AI33" s="17" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="AJ33" s="7"/>
       <c r="AK33" s="7"/>
       <c r="AL33" s="7" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="34" spans="1:38" ht="14.5" customHeight="1">
@@ -7010,7 +7097,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C34" s="5">
         <v>0</v>
@@ -7075,11 +7162,11 @@
         <v>77</v>
       </c>
       <c r="AE34" s="19" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="AF34" s="6"/>
       <c r="AG34" s="6" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="AH34" s="6"/>
       <c r="AI34" s="6"/>
@@ -7092,7 +7179,7 @@
         <v>76</v>
       </c>
       <c r="B35" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C35">
         <f>64866+33789</f>
@@ -7143,24 +7230,24 @@
       </c>
       <c r="U35" s="7"/>
       <c r="V35" s="7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="W35" s="7" t="s">
         <v>131</v>
       </c>
       <c r="X35" s="7" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="Y35" s="7"/>
       <c r="Z35" s="7"/>
       <c r="AA35" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="AB35" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="AC35" s="7" t="s">
         <v>285</v>
-      </c>
-      <c r="AB35" s="7" t="s">
-        <v>286</v>
-      </c>
-      <c r="AC35" s="7" t="s">
-        <v>287</v>
       </c>
       <c r="AD35" s="7" t="s">
         <v>91</v>
@@ -7168,11 +7255,11 @@
       <c r="AE35" s="7"/>
       <c r="AF35" s="7"/>
       <c r="AG35" s="7" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="AH35" s="7"/>
       <c r="AI35" s="7" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="AJ35" s="7"/>
       <c r="AK35" s="7"/>
@@ -7180,10 +7267,10 @@
     </row>
     <row r="36" spans="1:38" ht="14.5" customHeight="1">
       <c r="A36" s="5" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C36" s="5">
         <v>0.5</v>
@@ -7252,7 +7339,7 @@
       <c r="AG36" s="5"/>
       <c r="AH36" s="5"/>
       <c r="AI36" s="5" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="AJ36" s="5"/>
       <c r="AK36" s="5"/>
@@ -7263,7 +7350,7 @@
         <v>14</v>
       </c>
       <c r="B37" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C37">
         <v>64866</v>
@@ -7317,20 +7404,20 @@
         <v>92</v>
       </c>
       <c r="X37" s="7" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="Y37" s="7" t="s">
         <v>93</v>
       </c>
       <c r="Z37" s="7"/>
       <c r="AA37" s="7" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="AB37" s="17" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="AC37" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="AD37" s="7"/>
       <c r="AE37" s="7"/>
@@ -7339,7 +7426,7 @@
       <c r="AH37" s="7"/>
       <c r="AI37" s="7"/>
       <c r="AJ37" s="7" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="AK37" s="7"/>
       <c r="AL37" s="7"/>
@@ -7349,7 +7436,7 @@
         <v>15</v>
       </c>
       <c r="B38" s="23" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C38" s="5">
         <f>2353/5.1</f>
@@ -7363,7 +7450,9 @@
       </c>
       <c r="F38" s="5"/>
       <c r="G38" s="9"/>
-      <c r="H38" s="5"/>
+      <c r="H38" s="5">
+        <v>1</v>
+      </c>
       <c r="I38" s="5">
         <v>4.5032618547779402</v>
       </c>
@@ -7396,7 +7485,7 @@
       </c>
       <c r="U38" s="6"/>
       <c r="V38" s="6" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="W38" s="6" t="s">
         <v>90</v>
@@ -7406,9 +7495,11 @@
       </c>
       <c r="Y38" s="6"/>
       <c r="Z38" s="6"/>
-      <c r="AA38" s="6"/>
+      <c r="AA38" s="6" t="s">
+        <v>420</v>
+      </c>
       <c r="AB38" s="6" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="AC38" s="6"/>
       <c r="AD38" s="6" t="s">
@@ -7440,7 +7531,7 @@
         <v>16</v>
       </c>
       <c r="B39" s="23" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C39">
         <f>0.995^0.5</f>
@@ -7455,6 +7546,9 @@
         <v>1.0582665070765493</v>
       </c>
       <c r="G39" s="8"/>
+      <c r="H39">
+        <v>0.7</v>
+      </c>
       <c r="I39" s="37">
         <v>0.74194119079264453</v>
       </c>
@@ -7492,7 +7586,7 @@
       </c>
       <c r="U39" s="7"/>
       <c r="V39" s="7" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="W39" s="7" t="s">
         <v>89</v>
@@ -7502,9 +7596,11 @@
       </c>
       <c r="Y39" s="7"/>
       <c r="Z39" s="7"/>
-      <c r="AA39" s="7"/>
+      <c r="AA39" s="6" t="s">
+        <v>420</v>
+      </c>
       <c r="AB39" s="7" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="AC39" s="7"/>
       <c r="AD39" s="7" t="s">
@@ -7536,7 +7632,7 @@
         <v>35</v>
       </c>
       <c r="B40" s="23" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C40" s="5">
         <f>39.886/1.93</f>
@@ -7549,7 +7645,9 @@
         <v>2.2100000000000001E-4</v>
       </c>
       <c r="F40" s="5"/>
-      <c r="H40" s="5"/>
+      <c r="H40" s="5">
+        <v>0.7</v>
+      </c>
       <c r="I40" s="38">
         <v>1.0968131213886334</v>
       </c>
@@ -7582,7 +7680,7 @@
       </c>
       <c r="U40" s="6"/>
       <c r="V40" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="W40" s="6" t="s">
         <v>89</v>
@@ -7592,9 +7690,11 @@
       </c>
       <c r="Y40" s="6"/>
       <c r="Z40" s="6"/>
-      <c r="AA40" s="6"/>
+      <c r="AA40" s="6" t="s">
+        <v>415</v>
+      </c>
       <c r="AB40" s="6" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="AC40" s="6"/>
       <c r="AD40" s="6" t="s">
@@ -7626,7 +7726,7 @@
         <v>36</v>
       </c>
       <c r="B41" s="23" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C41">
         <f>0.1332^0.5</f>
@@ -7640,6 +7740,9 @@
         <v>0.95105399999999995</v>
       </c>
       <c r="G41" s="8"/>
+      <c r="H41">
+        <v>0.35</v>
+      </c>
       <c r="I41" s="37">
         <v>0.57791694994750731</v>
       </c>
@@ -7674,10 +7777,10 @@
         <v>34</v>
       </c>
       <c r="U41" s="7" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="V41" s="7" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="W41" s="7" t="s">
         <v>89</v>
@@ -7687,9 +7790,11 @@
       </c>
       <c r="Y41" s="7"/>
       <c r="Z41" s="7"/>
-      <c r="AA41" s="7"/>
+      <c r="AA41" s="6" t="s">
+        <v>415</v>
+      </c>
       <c r="AB41" s="6" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="AC41" s="7"/>
       <c r="AD41" s="7" t="s">
@@ -7721,7 +7826,7 @@
         <v>37</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C42" s="5">
         <v>1807.7719999999999</v>
@@ -7785,28 +7890,28 @@
       <c r="Y42" s="6"/>
       <c r="Z42" s="6"/>
       <c r="AA42" s="19" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="AB42" s="6"/>
       <c r="AC42" s="19" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="AD42" s="6" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="AE42" s="6"/>
       <c r="AF42" s="35" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="AG42" s="6"/>
       <c r="AH42" s="19" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="AI42" s="6"/>
       <c r="AJ42" s="6"/>
       <c r="AK42" s="6"/>
       <c r="AL42" s="6" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="43" spans="1:38" ht="14.5" customHeight="1">
@@ -7814,7 +7919,7 @@
         <v>124</v>
       </c>
       <c r="B43" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C43">
         <v>706</v>
@@ -7863,46 +7968,46 @@
       </c>
       <c r="R43" s="16"/>
       <c r="V43" t="s">
+        <v>164</v>
+      </c>
+      <c r="W43" t="s">
         <v>166</v>
       </c>
-      <c r="W43" t="s">
-        <v>168</v>
-      </c>
       <c r="X43" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="Y43" t="s">
         <v>126</v>
       </c>
       <c r="AA43" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="AB43" t="s">
+        <v>296</v>
+      </c>
+      <c r="AC43" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="AD43" t="s">
         <v>297</v>
       </c>
-      <c r="AB43" t="s">
+      <c r="AE43" t="s">
         <v>298</v>
       </c>
-      <c r="AC43" s="1" t="s">
+      <c r="AF43" t="s">
         <v>332</v>
       </c>
-      <c r="AD43" t="s">
-        <v>299</v>
-      </c>
-      <c r="AE43" t="s">
-        <v>300</v>
-      </c>
-      <c r="AF43" t="s">
-        <v>334</v>
-      </c>
       <c r="AG43" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="AH43" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="AI43" t="s">
         <v>126</v>
       </c>
       <c r="AJ43" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="AL43" s="7"/>
     </row>
@@ -7911,7 +8016,7 @@
         <v>38</v>
       </c>
       <c r="B44" s="23" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C44" s="5">
         <v>0</v>
@@ -7961,7 +8066,7 @@
       </c>
       <c r="U44" s="5"/>
       <c r="V44" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="W44" s="6" t="s">
         <v>88</v>
@@ -7972,10 +8077,10 @@
       <c r="Y44" s="6"/>
       <c r="Z44" s="6"/>
       <c r="AA44" s="6" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="AB44" s="6" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="AC44" s="6"/>
       <c r="AD44" s="6" t="s">
@@ -8009,7 +8114,7 @@
         <v>39</v>
       </c>
       <c r="B45" s="23" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C45">
         <v>1</v>
@@ -8056,7 +8161,7 @@
         <v>34</v>
       </c>
       <c r="V45" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="W45" s="7" t="s">
         <v>88</v>
@@ -8067,7 +8172,7 @@
       <c r="Y45" s="7"/>
       <c r="Z45" s="7"/>
       <c r="AA45" s="7" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="AB45" s="6"/>
       <c r="AC45" s="7"/>
@@ -8102,7 +8207,7 @@
         <v>40</v>
       </c>
       <c r="B46" s="23" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C46" s="5">
         <v>0</v>
@@ -8152,7 +8257,7 @@
       </c>
       <c r="U46" s="5"/>
       <c r="V46" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="W46" s="6" t="s">
         <v>88</v>
@@ -8196,7 +8301,7 @@
         <v>41</v>
       </c>
       <c r="B47" s="23" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C47">
         <v>0</v>
@@ -8242,7 +8347,7 @@
         <v>34</v>
       </c>
       <c r="V47" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="W47" s="7" t="s">
         <v>88</v>
@@ -8286,7 +8391,7 @@
         <v>42</v>
       </c>
       <c r="B48" s="23" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C48" s="5">
         <v>0</v>
@@ -8336,7 +8441,7 @@
       </c>
       <c r="U48" s="5"/>
       <c r="V48" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="W48" s="6" t="s">
         <v>88</v>
@@ -9395,30 +9500,30 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="B1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D1" t="s">
         <v>182</v>
       </c>
-      <c r="D1" t="s">
-        <v>184</v>
-      </c>
       <c r="E1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="E2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -9858,30 +9963,30 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="B1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D1" t="s">
         <v>182</v>
       </c>
-      <c r="D1" t="s">
-        <v>184</v>
-      </c>
       <c r="E1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B2" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="E2" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -10207,39 +10312,39 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="B1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D1" t="s">
         <v>182</v>
       </c>
-      <c r="D1" t="s">
-        <v>184</v>
-      </c>
       <c r="E1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B2" t="s">
+        <v>321</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="E2" t="s">
+        <v>324</v>
+      </c>
+      <c r="H2" t="s">
         <v>323</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="E2" t="s">
-        <v>326</v>
-      </c>
-      <c r="H2" t="s">
-        <v>325</v>
-      </c>
       <c r="I2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="J2" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -10677,25 +10782,25 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="B1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D1" t="s">
         <v>182</v>
       </c>
-      <c r="D1" t="s">
-        <v>184</v>
-      </c>
       <c r="E1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B2" s="1"/>
       <c r="D2" s="1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="16">
@@ -10892,25 +10997,25 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="B1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D1" t="s">
         <v>182</v>
       </c>
-      <c r="D1" t="s">
-        <v>184</v>
-      </c>
       <c r="E1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B2" s="1"/>
       <c r="D2" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="16">
@@ -11086,33 +11191,33 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="B1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E1" t="s">
         <v>182</v>
-      </c>
-      <c r="E1" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C2" t="s">
+        <v>195</v>
+      </c>
+      <c r="D2" t="s">
         <v>196</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>197</v>
-      </c>
-      <c r="D2" t="s">
-        <v>198</v>
-      </c>
-      <c r="E2" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -11460,39 +11565,39 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="B1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D1" t="s">
         <v>182</v>
       </c>
-      <c r="D1" t="s">
-        <v>184</v>
-      </c>
       <c r="E1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C2" t="s">
+        <v>192</v>
+      </c>
+      <c r="D2" t="s">
         <v>181</v>
       </c>
-      <c r="C2" t="s">
-        <v>194</v>
-      </c>
-      <c r="D2" t="s">
-        <v>183</v>
-      </c>
       <c r="E2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F2" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="16">
@@ -11939,42 +12044,42 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="B1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D1" t="s">
         <v>182</v>
       </c>
-      <c r="D1" t="s">
-        <v>184</v>
-      </c>
       <c r="E1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="G1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="C2" t="s">
-        <v>192</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>189</v>
-      </c>
       <c r="F2" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="G2" t="s">
         <v>186</v>
-      </c>
-      <c r="G2" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="16">
@@ -12513,8 +12618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63DF787E-9CE6-4767-AADB-C0D49F24A7F3}">
   <dimension ref="A1:Q41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -12525,64 +12630,64 @@
   <sheetData>
     <row r="1" spans="1:17">
       <c r="B1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D1" t="s">
         <v>182</v>
       </c>
-      <c r="D1" t="s">
-        <v>184</v>
-      </c>
       <c r="E1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="G1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="H1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="L1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="M1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="Q1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="2" spans="1:17">
       <c r="A2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="C2" t="s">
+        <v>303</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="E2" t="s">
+        <v>305</v>
+      </c>
+      <c r="F2" t="s">
+        <v>305</v>
+      </c>
+      <c r="H2" t="s">
         <v>308</v>
       </c>
-      <c r="C2" t="s">
-        <v>305</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="E2" t="s">
-        <v>307</v>
-      </c>
-      <c r="F2" t="s">
-        <v>307</v>
-      </c>
-      <c r="H2" t="s">
-        <v>310</v>
-      </c>
       <c r="L2" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="M2" s="32"/>
       <c r="Q2" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -13265,188 +13370,615 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E4E14CA-A602-4FF7-9D44-04838930B2AC}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D21"/>
+    <sheetView zoomScale="83" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:13">
       <c r="B1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D1" t="s">
         <v>182</v>
       </c>
-      <c r="D1" t="s">
-        <v>184</v>
-      </c>
       <c r="E1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+        <v>188</v>
+      </c>
+      <c r="K1" t="s">
+        <v>418</v>
+      </c>
+      <c r="L1" t="s">
+        <v>416</v>
+      </c>
+      <c r="M1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B2" s="1"/>
       <c r="D2" s="1" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="16">
+        <v>419</v>
+      </c>
+      <c r="J2">
+        <v>1990</v>
+      </c>
+      <c r="K2" s="39">
+        <v>51900</v>
+      </c>
+      <c r="L2">
+        <f>K2/1000</f>
+        <v>51.9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3">
+        <v>1990</v>
+      </c>
+      <c r="D3">
+        <f>L2/0.793</f>
+        <v>65.44766708701134</v>
+      </c>
+      <c r="J3">
+        <v>1991</v>
+      </c>
+      <c r="K3" s="39">
+        <v>48200</v>
+      </c>
+      <c r="L3">
+        <f t="shared" ref="L3:L31" si="0">K3/1000</f>
+        <v>48.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4">
+        <v>1991</v>
+      </c>
+      <c r="D4">
+        <f>L3/0.793</f>
+        <v>60.781841109709966</v>
+      </c>
+      <c r="J4">
+        <v>1992</v>
+      </c>
+      <c r="K4" s="39">
+        <v>42900</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="0"/>
+        <v>42.9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5">
+        <v>1992</v>
+      </c>
+      <c r="D5">
+        <f>L4/0.793</f>
+        <v>54.0983606557377</v>
+      </c>
+      <c r="J5">
+        <v>1993</v>
+      </c>
+      <c r="K5" s="39">
+        <v>34300</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="0"/>
+        <v>34.299999999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6">
+        <v>1993</v>
+      </c>
+      <c r="D6">
+        <f>L5/0.793</f>
+        <v>43.253467843631775</v>
+      </c>
+      <c r="J6">
+        <v>1994</v>
+      </c>
+      <c r="K6" s="39">
+        <v>34000</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7">
+        <v>1994</v>
+      </c>
+      <c r="D7">
+        <f>L6/0.793</f>
+        <v>42.875157629255988</v>
+      </c>
+      <c r="J7">
+        <v>1995</v>
+      </c>
+      <c r="K7" s="39">
+        <v>38500</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="0"/>
+        <v>38.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8">
+        <v>1995</v>
+      </c>
+      <c r="D8">
+        <f>L7/0.793</f>
+        <v>48.549810844892811</v>
+      </c>
+      <c r="J8">
+        <v>1996</v>
+      </c>
+      <c r="K8" s="39">
+        <v>34700</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="0"/>
+        <v>34.700000000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9">
+        <v>1996</v>
+      </c>
+      <c r="D9">
+        <f>L8/0.793</f>
+        <v>43.757881462799496</v>
+      </c>
+      <c r="J9">
+        <v>1997</v>
+      </c>
+      <c r="K9" s="39">
+        <v>33200</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="0"/>
+        <v>33.200000000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10">
+        <v>1997</v>
+      </c>
+      <c r="D10">
+        <f>L9/0.793</f>
+        <v>41.86633039092056</v>
+      </c>
+      <c r="J10">
+        <v>1998</v>
+      </c>
+      <c r="K10" s="39">
+        <v>37000</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11">
+        <v>1998</v>
+      </c>
+      <c r="D11">
+        <f>L10/0.793</f>
+        <v>46.658259773013867</v>
+      </c>
+      <c r="J11">
+        <v>1999</v>
+      </c>
+      <c r="K11" s="39">
+        <v>37700</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="0"/>
+        <v>37.700000000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12">
+        <v>1999</v>
+      </c>
+      <c r="D12">
+        <f>L11/0.793</f>
+        <v>47.540983606557376</v>
+      </c>
+      <c r="J12">
+        <v>2000</v>
+      </c>
+      <c r="K12" s="39">
+        <v>44000</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="16">
+      <c r="A13">
+        <v>2000</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13">
+        <f>L12/0.793</f>
+        <v>55.485498108448922</v>
+      </c>
+      <c r="J13">
         <v>2001</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3">
-        <v>35.143000000000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4">
+      <c r="K13" s="40">
+        <v>50800</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="0"/>
+        <v>50.8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14">
+        <v>2001</v>
+      </c>
+      <c r="D14">
+        <f>L13/0.793</f>
+        <v>64.060529634300124</v>
+      </c>
+      <c r="J14">
         <v>2002</v>
       </c>
-      <c r="D4">
-        <v>45.418999999999997</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5">
+      <c r="K14" s="40">
+        <v>47000</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15">
+        <v>2002</v>
+      </c>
+      <c r="D15">
+        <f>L14/0.793</f>
+        <v>59.268600252206809</v>
+      </c>
+      <c r="J15">
         <v>2003</v>
       </c>
-      <c r="D5">
-        <v>48.030999999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6">
+      <c r="K15" s="40">
+        <v>47200</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="0"/>
+        <v>47.2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16">
+        <v>2003</v>
+      </c>
+      <c r="D16">
+        <f>L15/0.793</f>
+        <v>59.52080706179067</v>
+      </c>
+      <c r="J16">
         <v>2004</v>
       </c>
-      <c r="D6">
-        <v>66.912000000000006</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7">
+      <c r="K16" s="40">
+        <v>66300</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="0"/>
+        <v>66.3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17">
+        <v>2004</v>
+      </c>
+      <c r="D17">
+        <f>L16/0.793</f>
+        <v>83.606557377049171</v>
+      </c>
+      <c r="J17">
         <v>2005</v>
       </c>
-      <c r="D7">
-        <v>60.619</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8">
+      <c r="K17" s="40">
+        <v>59500</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="0"/>
+        <v>59.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18">
+        <v>2005</v>
+      </c>
+      <c r="D18">
+        <f>L17/0.793</f>
+        <v>75.031525851197983</v>
+      </c>
+      <c r="J18">
         <v>2006</v>
       </c>
-      <c r="D8">
-        <v>60.347000000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9">
+      <c r="K18" s="40">
+        <v>56600</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="0"/>
+        <v>56.6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19">
+        <v>2006</v>
+      </c>
+      <c r="D19">
+        <f>L18/0.793</f>
+        <v>71.37452711223203</v>
+      </c>
+      <c r="J19">
         <v>2007</v>
       </c>
-      <c r="D9">
-        <v>58.36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10">
+      <c r="K19" s="40">
+        <v>53600</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="0"/>
+        <v>53.6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20">
+        <v>2007</v>
+      </c>
+      <c r="D20">
+        <f>L19/0.793</f>
+        <v>67.591424968474143</v>
+      </c>
+      <c r="J20">
         <v>2008</v>
       </c>
-      <c r="D10">
-        <v>66.736999999999995</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11">
+      <c r="K20" s="40">
+        <v>61900</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="0"/>
+        <v>61.9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21">
+        <v>2008</v>
+      </c>
+      <c r="D21">
+        <f>L20/0.793</f>
+        <v>78.058007566204282</v>
+      </c>
+      <c r="J21">
         <v>2009</v>
       </c>
-      <c r="D11">
-        <v>63.31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12">
+      <c r="K21" s="40">
+        <v>61200</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="0"/>
+        <v>61.2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22">
+        <v>2009</v>
+      </c>
+      <c r="D22">
+        <f>L21/0.793</f>
+        <v>77.175283732660787</v>
+      </c>
+      <c r="J22">
         <v>2010</v>
       </c>
-      <c r="D12">
-        <v>63.418999999999997</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13">
+      <c r="K22" s="40">
+        <v>68400</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="0"/>
+        <v>68.400000000000006</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23">
+        <v>2010</v>
+      </c>
+      <c r="D23">
+        <f>L22/0.793</f>
+        <v>86.254728877679696</v>
+      </c>
+      <c r="J23">
         <v>2011</v>
       </c>
-      <c r="D13">
-        <v>73.025000000000006</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14">
+      <c r="K23" s="40">
+        <v>73900</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="0"/>
+        <v>73.900000000000006</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24">
+        <v>2011</v>
+      </c>
+      <c r="D24">
+        <f>L23/0.793</f>
+        <v>93.190416141235815</v>
+      </c>
+      <c r="J24">
         <v>2012</v>
       </c>
-      <c r="D14">
-        <v>74.018000000000001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15">
+      <c r="K24" s="40">
+        <v>77700</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="0"/>
+        <v>77.7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25">
+        <v>2012</v>
+      </c>
+      <c r="D25">
+        <f>L24/0.793</f>
+        <v>97.98234552332913</v>
+      </c>
+      <c r="J25">
         <v>2013</v>
       </c>
-      <c r="D15">
-        <v>76.650999999999996</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16">
+      <c r="K25" s="40">
+        <v>79400</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="0"/>
+        <v>79.400000000000006</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26">
+        <v>2013</v>
+      </c>
+      <c r="D26">
+        <f>L25/0.793</f>
+        <v>100.12610340479193</v>
+      </c>
+      <c r="J26">
         <v>2014</v>
       </c>
-      <c r="D16">
-        <v>80.634</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17">
+      <c r="K26" s="40">
+        <v>82100</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="0"/>
+        <v>82.1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27">
+        <v>2014</v>
+      </c>
+      <c r="D27">
+        <f>L26/0.793</f>
+        <v>103.53089533417401</v>
+      </c>
+      <c r="J27">
         <v>2015</v>
       </c>
-      <c r="D17">
-        <v>83.010999999999996</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18">
+      <c r="K27" s="40">
+        <v>83700</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="0"/>
+        <v>83.7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28">
+        <v>2015</v>
+      </c>
+      <c r="D28">
+        <f>L27/0.793</f>
+        <v>105.54854981084489</v>
+      </c>
+      <c r="J28">
         <v>2016</v>
       </c>
-      <c r="D18">
-        <v>80.393000000000001</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19">
+      <c r="K28" s="40">
+        <v>78400</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="0"/>
+        <v>78.400000000000006</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29">
+        <v>2016</v>
+      </c>
+      <c r="D29">
+        <f>L28/0.793</f>
+        <v>98.865069356872638</v>
+      </c>
+      <c r="J29">
         <v>2017</v>
       </c>
-      <c r="D19">
-        <v>83.572999999999993</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20">
+      <c r="K29" s="40">
+        <v>81400</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="0"/>
+        <v>81.400000000000006</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30">
+        <v>2017</v>
+      </c>
+      <c r="D30">
+        <f>L29/0.793</f>
+        <v>102.64817150063053</v>
+      </c>
+      <c r="J30">
         <v>2018</v>
       </c>
-      <c r="D20">
-        <v>81.186999999999998</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21">
+      <c r="K30" s="40">
+        <v>82200</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="0"/>
+        <v>82.2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="A31">
+        <v>2018</v>
+      </c>
+      <c r="D31">
+        <f>L30/0.793</f>
+        <v>103.65699873896595</v>
+      </c>
+      <c r="J31">
         <v>2019</v>
       </c>
-      <c r="D21">
-        <v>90.4</v>
+      <c r="K31" s="40">
+        <v>83800</v>
+      </c>
+      <c r="L31">
+        <f t="shared" si="0"/>
+        <v>83.8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32">
+        <v>2019</v>
+      </c>
+      <c r="D32">
+        <f>L31/0.793</f>
+        <v>105.67465321563681</v>
       </c>
     </row>
   </sheetData>
@@ -13469,24 +14001,24 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="B1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D1" t="s">
         <v>182</v>
       </c>
-      <c r="D1" t="s">
-        <v>184</v>
-      </c>
       <c r="E1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D2" s="1"/>
     </row>
@@ -13972,24 +14504,24 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="B1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D1" t="s">
         <v>182</v>
       </c>
-      <c r="D1" t="s">
-        <v>184</v>
-      </c>
       <c r="E1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D2" s="1"/>
     </row>
@@ -14419,30 +14951,30 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="B1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D1" t="s">
         <v>182</v>
       </c>
-      <c r="D1" t="s">
-        <v>184</v>
-      </c>
       <c r="E1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="E2" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -15243,7 +15775,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3A510BC-6699-4D7F-A1BA-2D5B6A269B1B}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
@@ -15251,30 +15783,30 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="B1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D1" t="s">
         <v>182</v>
       </c>
-      <c r="D1" t="s">
-        <v>184</v>
-      </c>
       <c r="E1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="16">

</xml_diff>

<commit_message>
add mcpe0 compatibility, others
- added mcpe0 filename changes and capability, where mcpe is for mine_cost_price_elas, since it may be that we don't actually want that variable in the system and this sets it to zero. My thought is that for cases where price increases, it causes mine costs to increase as well, which can drive bad feedback loops and also (e.g. copper) limit how high the ore grade elasticity to cumulative production gets. But from a reality-based perspective, this was likely due to the oil price correlation between mine costs and commodity price, so it makes sense that if we're pulling that effect out of price we should remove it here too.
- made sure historical_data loads went correctly, with historical_price_rolling_window getting pulled in correctly
^ it seemed that mine pre-tuning wasn't getting the rolling mean version of price.
- updated case study data.xlsx, since some of the variables weren't consistent between the Sheet1 and their commodity time series page.
</commit_message>
<xml_diff>
--- a/data/case study data.xlsx
+++ b/data/case study data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnryter/Dropbox (MIT)/John MIT/Research/generalizationOutside/generalization/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8388C87-F2D9-2549-8645-3FC9BCF80B0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82985BEA-1269-834D-BE9A-65C172417B24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="500" windowWidth="28800" windowHeight="16040" xr2:uid="{9C1DBEC5-9C42-494B-AEAA-1D89B674AD0D}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{9C1DBEC5-9C42-494B-AEAA-1D89B674AD0D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="17" r:id="rId1"/>
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="437">
   <si>
     <t>Al</t>
   </si>
@@ -630,9 +630,6 @@
     <t>Primary commodity price</t>
   </si>
   <si>
-    <t>baseline_scenario.xlsx for aluminum, sheet smelter_prod</t>
-  </si>
-  <si>
     <t>Primary supply</t>
   </si>
   <si>
@@ -1390,6 +1387,15 @@
   </si>
   <si>
     <t xml:space="preserve">Fraction of global mine production coming from SX-EW process, or any other process that produces the refined product directly rather than having it pass through a refinery (e.g. lithium brines) </t>
+  </si>
+  <si>
+    <t>baseline_scenario.xlsx for aluminum, sheet smelter_prod (trying to account for bauxite/alumina used for things other than aluminum)</t>
+  </si>
+  <si>
+    <t>Primary supply (BGS)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Silver Institute, World Silver Surveys, taking the most recent  value reported in the surveys from 2005-2022, https://www.silverinstitute.org/all-world-silver-surveys/. </t>
   </si>
 </sst>
 </file>
@@ -3680,13 +3686,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>86</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>533400</xdr:colOff>
       <xdr:row>100</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
@@ -4103,8 +4109,8 @@
   <dimension ref="A1:AL74"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="114" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B51" sqref="B51"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -4135,10 +4141,10 @@
   <sheetData>
     <row r="1" spans="1:38" s="28" customFormat="1" ht="34" customHeight="1">
       <c r="A1" s="28" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C1" s="28" t="s">
         <v>0</v>
@@ -4186,7 +4192,7 @@
         <v>94</v>
       </c>
       <c r="R1" s="29" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="S1" s="28" t="s">
         <v>95</v>
@@ -4246,7 +4252,7 @@
         <v>108</v>
       </c>
       <c r="AL1" s="28" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="2" spans="1:38" ht="14.5" customHeight="1">
@@ -4254,7 +4260,7 @@
         <v>9</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>10</v>
@@ -4263,10 +4269,10 @@
         <v>10</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>11</v>
@@ -4278,29 +4284,29 @@
         <v>10</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="L2" s="5" t="s">
         <v>10</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="O2" s="5"/>
       <c r="P2" s="5" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="Q2" s="5" t="s">
         <v>10</v>
       </c>
       <c r="R2" s="14" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="S2" s="5" t="s">
         <v>10</v>
@@ -4312,35 +4318,35 @@
       <c r="V2" s="6"/>
       <c r="W2" s="6"/>
       <c r="X2" s="6" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="Y2" s="6" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="Z2" s="6"/>
       <c r="AA2" s="6"/>
       <c r="AB2" s="6"/>
       <c r="AC2" s="6" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="AD2" s="6" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="AE2" s="6"/>
       <c r="AF2" s="6" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="AG2" s="6" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="AH2" s="6"/>
       <c r="AI2" s="6" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="AJ2" s="6"/>
       <c r="AK2" s="6"/>
       <c r="AL2" s="6" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="3" spans="1:38" ht="14.5" customHeight="1">
@@ -4348,10 +4354,10 @@
         <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C3">
-        <v>99671</v>
+        <v>85768.388145129153</v>
       </c>
       <c r="D3">
         <v>1767000</v>
@@ -4368,14 +4374,14 @@
       <c r="J3">
         <v>2.4049999999999998</v>
       </c>
-      <c r="K3" s="15">
-        <v>23600</v>
+      <c r="K3">
+        <v>30046.0829493087</v>
       </c>
       <c r="L3">
         <v>3226.8622280817385</v>
       </c>
       <c r="M3">
-        <v>26.7</v>
+        <v>26.704941782475718</v>
       </c>
       <c r="N3">
         <v>17448.642054092597</v>
@@ -4413,32 +4419,32 @@
       <c r="Y3" s="7"/>
       <c r="Z3" s="7"/>
       <c r="AA3" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="AB3" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="AB3" s="7" t="s">
+      <c r="AC3" s="17" t="s">
         <v>199</v>
-      </c>
-      <c r="AC3" s="17" t="s">
-        <v>200</v>
       </c>
       <c r="AD3" s="7"/>
       <c r="AE3" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="AF3" s="17" t="s">
         <v>201</v>
       </c>
-      <c r="AF3" s="17" t="s">
+      <c r="AG3" s="7" t="s">
         <v>202</v>
       </c>
-      <c r="AG3" s="7" t="s">
+      <c r="AH3" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="AH3" s="7" t="s">
+      <c r="AI3" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="AI3" s="7" t="s">
+      <c r="AJ3" s="7" t="s">
         <v>205</v>
-      </c>
-      <c r="AJ3" s="7" t="s">
-        <v>206</v>
       </c>
       <c r="AK3" s="7"/>
       <c r="AL3" s="7"/>
@@ -4448,7 +4454,7 @@
         <v>19</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -4486,7 +4492,7 @@
       <c r="AB4" s="6"/>
       <c r="AC4" s="6"/>
       <c r="AD4" s="6" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="AE4" s="6"/>
       <c r="AF4" s="6"/>
@@ -4502,7 +4508,7 @@
         <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C5">
         <v>0.04</v>
@@ -4553,43 +4559,43 @@
         <v>21</v>
       </c>
       <c r="V5" s="7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="W5" s="7" t="s">
         <v>132</v>
       </c>
       <c r="X5" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="Y5" s="7"/>
       <c r="Z5" s="7"/>
       <c r="AA5" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="AB5" s="17" t="s">
         <v>208</v>
       </c>
-      <c r="AB5" s="17" t="s">
+      <c r="AC5" s="7" t="s">
         <v>209</v>
-      </c>
-      <c r="AC5" s="7" t="s">
-        <v>210</v>
       </c>
       <c r="AD5" s="7"/>
       <c r="AE5" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="AF5" s="7" t="s">
         <v>211</v>
       </c>
-      <c r="AF5" s="7" t="s">
+      <c r="AG5" s="35" t="s">
+        <v>333</v>
+      </c>
+      <c r="AH5" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="AG5" s="35" t="s">
-        <v>334</v>
-      </c>
-      <c r="AH5" s="7" t="s">
+      <c r="AI5" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="AI5" s="7" t="s">
+      <c r="AJ5" s="7" t="s">
         <v>214</v>
-      </c>
-      <c r="AJ5" s="7" t="s">
-        <v>215</v>
       </c>
       <c r="AK5" s="7"/>
       <c r="AL5" s="7"/>
@@ -4599,7 +4605,7 @@
         <v>25</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C6" s="5">
         <v>0.45100000000000001</v>
@@ -4663,38 +4669,38 @@
       <c r="Y6" s="6"/>
       <c r="Z6" s="6"/>
       <c r="AA6" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="AB6" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="AB6" s="6" t="s">
+      <c r="AC6" s="6" t="s">
         <v>217</v>
-      </c>
-      <c r="AC6" s="6" t="s">
-        <v>218</v>
       </c>
       <c r="AD6" s="6" t="s">
         <v>78</v>
       </c>
       <c r="AE6" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="AF6" s="6" t="s">
+        <v>334</v>
+      </c>
+      <c r="AG6" s="6" t="s">
         <v>219</v>
       </c>
-      <c r="AF6" s="6" t="s">
-        <v>335</v>
-      </c>
-      <c r="AG6" s="6" t="s">
+      <c r="AH6" s="19" t="s">
+        <v>323</v>
+      </c>
+      <c r="AI6" s="6" t="s">
         <v>220</v>
       </c>
-      <c r="AH6" s="19" t="s">
-        <v>324</v>
-      </c>
-      <c r="AI6" s="6" t="s">
-        <v>221</v>
-      </c>
       <c r="AJ6" s="35" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="AK6" s="6"/>
       <c r="AL6" s="35" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="7" spans="1:38" ht="14.5" customHeight="1">
@@ -4702,7 +4708,7 @@
         <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C7">
         <v>0.251</v>
@@ -4768,38 +4774,38 @@
       <c r="Y7" s="7"/>
       <c r="Z7" s="7"/>
       <c r="AA7" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="AB7" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="AC7" s="7" t="s">
         <v>222</v>
-      </c>
-      <c r="AB7" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="AC7" s="7" t="s">
-        <v>223</v>
       </c>
       <c r="AD7" s="7" t="s">
         <v>78</v>
       </c>
       <c r="AE7" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="AF7" s="17" t="s">
+        <v>341</v>
+      </c>
+      <c r="AG7" s="17" t="s">
+        <v>337</v>
+      </c>
+      <c r="AH7" s="17" t="s">
         <v>342</v>
       </c>
-      <c r="AG7" s="17" t="s">
-        <v>338</v>
-      </c>
-      <c r="AH7" s="17" t="s">
-        <v>343</v>
-      </c>
       <c r="AI7" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AJ7" s="7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="AK7" s="7"/>
       <c r="AL7" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="8" spans="1:38" ht="14.5" customHeight="1">
@@ -4807,7 +4813,7 @@
         <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C8" s="5">
         <v>0.11899999999999999</v>
@@ -4873,13 +4879,13 @@
       <c r="Y8" s="6"/>
       <c r="Z8" s="6"/>
       <c r="AA8" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="AB8" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="AC8" s="6" t="s">
         <v>226</v>
-      </c>
-      <c r="AB8" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="AC8" s="6" t="s">
-        <v>227</v>
       </c>
       <c r="AD8" s="6" t="s">
         <v>78</v>
@@ -4889,7 +4895,7 @@
       <c r="AG8" s="6"/>
       <c r="AH8" s="6"/>
       <c r="AI8" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AJ8" s="6"/>
       <c r="AK8" s="6"/>
@@ -4900,7 +4906,7 @@
         <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C9">
         <v>0.11899999999999999</v>
@@ -4965,25 +4971,25 @@
       <c r="Y9" s="7"/>
       <c r="Z9" s="7"/>
       <c r="AA9" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="AB9" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="AC9" s="7" t="s">
         <v>229</v>
-      </c>
-      <c r="AB9" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="AC9" s="7" t="s">
-        <v>230</v>
       </c>
       <c r="AD9" s="7" t="s">
         <v>78</v>
       </c>
       <c r="AE9" s="7"/>
       <c r="AF9" s="7" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="AG9" s="7"/>
       <c r="AH9" s="7"/>
       <c r="AI9" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="AJ9" s="7"/>
       <c r="AK9" s="7"/>
@@ -4994,7 +5000,7 @@
         <v>29</v>
       </c>
       <c r="B10" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C10" s="5">
         <f>1-C11-C7-C9-C8</f>
@@ -5065,25 +5071,25 @@
       <c r="Y10" s="6"/>
       <c r="Z10" s="6"/>
       <c r="AA10" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="AB10" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="AC10" s="6" t="s">
         <v>233</v>
-      </c>
-      <c r="AB10" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="AC10" s="6" t="s">
-        <v>234</v>
       </c>
       <c r="AD10" s="6" t="s">
         <v>78</v>
       </c>
       <c r="AE10" s="6"/>
       <c r="AF10" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="AG10" s="6"/>
       <c r="AH10" s="6"/>
       <c r="AI10" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="AJ10" s="6"/>
       <c r="AK10" s="6"/>
@@ -5094,7 +5100,7 @@
         <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C11">
         <v>0.27300000000000002</v>
@@ -5160,22 +5166,22 @@
       <c r="Z11" s="7"/>
       <c r="AA11" s="7"/>
       <c r="AB11" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="AC11" s="7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="AD11" s="7" t="s">
         <v>78</v>
       </c>
       <c r="AE11" s="7"/>
       <c r="AF11" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="AG11" s="7"/>
       <c r="AH11" s="7"/>
       <c r="AI11" s="7" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="AJ11" s="7"/>
       <c r="AK11" s="7"/>
@@ -5186,7 +5192,7 @@
         <v>96</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C12" s="5">
         <v>0.9</v>
@@ -5252,35 +5258,35 @@
       <c r="Z12" s="6"/>
       <c r="AA12" s="6"/>
       <c r="AB12" s="6" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="AC12" s="6" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AD12" s="6" t="s">
         <v>106</v>
       </c>
       <c r="AE12" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="AF12" s="6" t="s">
         <v>240</v>
       </c>
-      <c r="AF12" s="6" t="s">
+      <c r="AG12" s="6" t="s">
         <v>241</v>
       </c>
-      <c r="AG12" s="6" t="s">
+      <c r="AH12" s="6" t="s">
         <v>242</v>
       </c>
-      <c r="AH12" s="6" t="s">
+      <c r="AI12" s="6" t="s">
         <v>243</v>
       </c>
-      <c r="AI12" s="6" t="s">
-        <v>244</v>
-      </c>
       <c r="AJ12" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="AK12" s="6"/>
       <c r="AL12" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="13" spans="1:38" ht="14.5" customHeight="1">
@@ -5288,7 +5294,7 @@
         <v>97</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C13">
         <v>0.95</v>
@@ -5357,20 +5363,20 @@
         <v>106</v>
       </c>
       <c r="AE13" s="7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="AF13" s="7" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AG13" s="7"/>
       <c r="AH13" s="7"/>
       <c r="AI13" s="7" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="AJ13" s="7"/>
       <c r="AK13" s="7"/>
       <c r="AL13" s="7" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="14" spans="1:38" ht="14.5" customHeight="1">
@@ -5378,7 +5384,7 @@
         <v>98</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C14" s="5">
         <v>0.9</v>
@@ -5456,7 +5462,7 @@
       <c r="AJ14" s="6"/>
       <c r="AK14" s="6"/>
       <c r="AL14" s="6" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="15" spans="1:38" ht="14.5" customHeight="1">
@@ -5464,7 +5470,7 @@
         <v>99</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C15">
         <v>0.95</v>
@@ -5545,7 +5551,7 @@
         <v>100</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C16" s="5">
         <v>0.9</v>
@@ -5621,7 +5627,7 @@
       <c r="AJ16" s="6"/>
       <c r="AK16" s="6"/>
       <c r="AL16" s="6" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="17" spans="1:38" ht="14.5" customHeight="1">
@@ -5629,7 +5635,7 @@
         <v>101</v>
       </c>
       <c r="B17" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C17">
         <v>50</v>
@@ -5694,31 +5700,31 @@
       <c r="Z17" s="7"/>
       <c r="AA17" s="7"/>
       <c r="AB17" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="AC17" s="7" t="s">
         <v>251</v>
-      </c>
-      <c r="AC17" s="7" t="s">
-        <v>252</v>
       </c>
       <c r="AD17" s="7" t="s">
         <v>106</v>
       </c>
       <c r="AE17" s="17" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="AF17" s="7" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AG17" s="7" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AH17" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="AI17" s="7" t="s">
         <v>253</v>
       </c>
-      <c r="AI17" s="7" t="s">
+      <c r="AJ17" s="7" t="s">
         <v>254</v>
-      </c>
-      <c r="AJ17" s="7" t="s">
-        <v>255</v>
       </c>
       <c r="AK17" s="7"/>
       <c r="AL17" s="7"/>
@@ -5728,7 +5734,7 @@
         <v>102</v>
       </c>
       <c r="B18" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C18" s="5">
         <v>25</v>
@@ -5793,32 +5799,32 @@
       <c r="Y18" s="6"/>
       <c r="Z18" s="6"/>
       <c r="AA18" s="19" t="s">
+        <v>255</v>
+      </c>
+      <c r="AB18" s="6" t="s">
         <v>256</v>
       </c>
-      <c r="AB18" s="6" t="s">
+      <c r="AC18" s="19" t="s">
         <v>257</v>
-      </c>
-      <c r="AC18" s="19" t="s">
-        <v>258</v>
       </c>
       <c r="AD18" s="6" t="s">
         <v>106</v>
       </c>
       <c r="AE18" s="17" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="AF18" s="7" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AG18" s="6" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AH18" s="6"/>
       <c r="AI18" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="AJ18" s="6" t="s">
         <v>260</v>
-      </c>
-      <c r="AJ18" s="6" t="s">
-        <v>261</v>
       </c>
       <c r="AK18" s="6"/>
       <c r="AL18" s="6"/>
@@ -5828,7 +5834,7 @@
         <v>103</v>
       </c>
       <c r="B19" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C19">
         <v>20</v>
@@ -5898,22 +5904,22 @@
         <v>106</v>
       </c>
       <c r="AE19" s="17" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="AF19" s="7" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AG19" s="7" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AH19" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="AI19" s="7" t="s">
         <v>262</v>
       </c>
-      <c r="AI19" s="7" t="s">
+      <c r="AJ19" s="1" t="s">
         <v>263</v>
-      </c>
-      <c r="AJ19" s="1" t="s">
-        <v>264</v>
       </c>
       <c r="AK19" s="7"/>
       <c r="AL19" s="7"/>
@@ -5923,7 +5929,7 @@
         <v>104</v>
       </c>
       <c r="B20" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C20" s="5">
         <v>15</v>
@@ -5982,7 +5988,7 @@
       <c r="Y20" s="6"/>
       <c r="Z20" s="6"/>
       <c r="AA20" s="6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="AB20" s="6"/>
       <c r="AC20" s="6"/>
@@ -5990,16 +5996,16 @@
         <v>106</v>
       </c>
       <c r="AE20" s="17" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="AF20" s="7" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AG20" s="6" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AH20" s="6" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="AI20" s="6"/>
       <c r="AJ20" s="6"/>
@@ -6011,7 +6017,7 @@
         <v>105</v>
       </c>
       <c r="B21" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C21">
         <v>15</v>
@@ -6076,28 +6082,28 @@
       <c r="Z21" s="7"/>
       <c r="AA21" s="7"/>
       <c r="AB21" s="7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="AD21" s="7" t="s">
         <v>106</v>
       </c>
       <c r="AE21" s="17" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="AF21" s="7" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AG21" s="7" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AH21" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="AI21" s="7" t="s">
         <v>267</v>
       </c>
-      <c r="AI21" s="7" t="s">
+      <c r="AJ21" s="7" t="s">
         <v>268</v>
-      </c>
-      <c r="AJ21" s="7" t="s">
-        <v>269</v>
       </c>
       <c r="AK21" s="7"/>
       <c r="AL21" s="7"/>
@@ -6107,7 +6113,7 @@
         <v>134</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C22" s="5">
         <v>0.64749999999999996</v>
@@ -6157,28 +6163,28 @@
       </c>
       <c r="W22" s="6"/>
       <c r="X22" s="6" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="Y22" s="6"/>
       <c r="AA22" s="7"/>
       <c r="AB22" s="17" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="AC22" s="5"/>
       <c r="AD22" s="6" t="s">
         <v>175</v>
       </c>
       <c r="AE22" s="17" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="AF22" s="6" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="AG22" s="19" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="AH22" s="6" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="AI22" s="6"/>
       <c r="AJ22" s="6"/>
@@ -6190,7 +6196,7 @@
         <v>135</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C23">
         <v>0.72899999999999998</v>
@@ -6235,28 +6241,28 @@
       </c>
       <c r="W23" s="7"/>
       <c r="X23" s="7" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="Y23" s="7"/>
       <c r="AA23" s="6"/>
       <c r="AB23" s="17" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="AC23" s="7"/>
       <c r="AD23" s="7" t="s">
         <v>175</v>
       </c>
       <c r="AE23" s="17" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="AF23" s="6" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="AG23" s="19" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="AH23" s="6" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="AI23" s="7"/>
       <c r="AJ23" s="7"/>
@@ -6267,7 +6273,7 @@
         <v>136</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C24" s="5">
         <v>0.76690000000000003</v>
@@ -6317,28 +6323,28 @@
       </c>
       <c r="W24" s="6"/>
       <c r="X24" s="6" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="Y24" s="6"/>
       <c r="AA24" s="7"/>
       <c r="AB24" s="17" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="AC24" s="5"/>
       <c r="AD24" s="6" t="s">
         <v>175</v>
       </c>
       <c r="AE24" s="17" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="AF24" s="6" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="AG24" s="19" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="AH24" s="6" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="AI24" s="6"/>
       <c r="AJ24" s="6"/>
@@ -6350,7 +6356,7 @@
         <v>137</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C25">
         <v>0.46850000000000003</v>
@@ -6395,27 +6401,27 @@
       </c>
       <c r="W25" s="7"/>
       <c r="X25" s="7" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="Y25" s="7"/>
       <c r="AA25" s="6"/>
       <c r="AB25" s="17" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="AD25" s="7" t="s">
         <v>175</v>
       </c>
       <c r="AE25" s="17" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="AF25" s="6" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="AG25" s="19" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="AH25" s="6" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="AI25" s="7"/>
       <c r="AJ25" s="7"/>
@@ -6426,7 +6432,7 @@
         <v>138</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C26" s="5">
         <v>0.75</v>
@@ -6476,27 +6482,27 @@
       </c>
       <c r="W26" s="6"/>
       <c r="X26" s="6" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="Y26" s="6"/>
       <c r="AA26" s="7"/>
       <c r="AB26" s="17" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="AD26" s="6" t="s">
         <v>175</v>
       </c>
       <c r="AE26" s="17" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="AF26" s="6" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="AG26" s="19" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="AH26" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="AI26" s="6"/>
       <c r="AJ26" s="6"/>
@@ -6508,7 +6514,7 @@
         <v>70</v>
       </c>
       <c r="B27" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C27">
         <v>0.34250000000000003</v>
@@ -6571,23 +6577,23 @@
       <c r="Y27" s="7"/>
       <c r="Z27" s="7"/>
       <c r="AA27" s="17" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="AB27" s="7"/>
       <c r="AC27" s="17" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="AD27" s="7" t="s">
         <v>77</v>
       </c>
       <c r="AE27" s="7"/>
       <c r="AF27" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="AG27" s="7"/>
       <c r="AH27" s="7"/>
       <c r="AI27" s="7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="AJ27" s="7"/>
       <c r="AK27" s="7"/>
@@ -6598,7 +6604,7 @@
         <v>69</v>
       </c>
       <c r="B28" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C28" s="5">
         <v>0.24399999999999999</v>
@@ -6661,25 +6667,25 @@
       <c r="Y28" s="6"/>
       <c r="Z28" s="6"/>
       <c r="AA28" s="6" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="AB28" s="6"/>
       <c r="AC28" s="19" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="AD28" s="6" t="s">
         <v>77</v>
       </c>
       <c r="AE28" s="6"/>
       <c r="AF28" s="6" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="AG28" s="6" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="AH28" s="6"/>
       <c r="AI28" s="6" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="AJ28" s="6"/>
       <c r="AK28" s="6"/>
@@ -6690,7 +6696,7 @@
         <v>75</v>
       </c>
       <c r="B29" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -6774,7 +6780,7 @@
         <v>74</v>
       </c>
       <c r="B30" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C30" s="5">
         <v>0.57769999999999999</v>
@@ -6835,7 +6841,7 @@
       <c r="Y30" s="6"/>
       <c r="Z30" s="6"/>
       <c r="AA30" s="19" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="AB30" s="6"/>
       <c r="AC30" s="6"/>
@@ -6843,13 +6849,13 @@
         <v>77</v>
       </c>
       <c r="AE30" s="6" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="AF30" s="6"/>
       <c r="AG30" s="6"/>
       <c r="AH30" s="6"/>
       <c r="AI30" s="22" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="AJ30" s="6"/>
       <c r="AK30" s="6"/>
@@ -6860,7 +6866,7 @@
         <v>72</v>
       </c>
       <c r="B31" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C31">
         <v>0</v>
@@ -6916,7 +6922,7 @@
         <v>130</v>
       </c>
       <c r="X31" s="7" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="Y31" s="7"/>
       <c r="Z31" s="7"/>
@@ -6928,7 +6934,7 @@
       </c>
       <c r="AE31" s="7"/>
       <c r="AF31" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="AG31" s="7"/>
       <c r="AH31" s="7"/>
@@ -6942,7 +6948,7 @@
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C32" s="5">
         <v>0</v>
@@ -7000,7 +7006,7 @@
         <v>130</v>
       </c>
       <c r="X32" s="7" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="Y32" s="6"/>
       <c r="Z32" s="6"/>
@@ -7012,12 +7018,12 @@
       </c>
       <c r="AE32" s="6"/>
       <c r="AF32" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="AG32" s="6"/>
       <c r="AH32" s="6"/>
       <c r="AI32" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="AJ32" s="6"/>
       <c r="AK32" s="6"/>
@@ -7028,7 +7034,7 @@
         <v>73</v>
       </c>
       <c r="B33" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C33">
         <v>0</v>
@@ -7088,24 +7094,24 @@
       <c r="AA33" s="7"/>
       <c r="AB33" s="7"/>
       <c r="AC33" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="AD33" s="7" t="s">
         <v>77</v>
       </c>
       <c r="AE33" s="7" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="AF33" s="7"/>
       <c r="AG33" s="7"/>
       <c r="AH33" s="7"/>
       <c r="AI33" s="17" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="AJ33" s="7"/>
       <c r="AK33" s="7"/>
       <c r="AL33" s="7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="34" spans="1:38" ht="14.5" customHeight="1">
@@ -7113,7 +7119,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C34" s="5">
         <v>0</v>
@@ -7178,11 +7184,11 @@
         <v>77</v>
       </c>
       <c r="AE34" s="19" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="AF34" s="6"/>
       <c r="AG34" s="6" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="AH34" s="6"/>
       <c r="AI34" s="6"/>
@@ -7195,11 +7201,10 @@
         <v>76</v>
       </c>
       <c r="B35" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C35">
-        <f>64866+33789</f>
-        <v>98655</v>
+        <v>88603.1</v>
       </c>
       <c r="D35">
         <v>1869000</v>
@@ -7212,25 +7217,26 @@
         <v>108.5</v>
       </c>
       <c r="I35">
-        <v>307</v>
+        <f>I37/(1-I27)</f>
+        <v>321.92849740932644</v>
       </c>
       <c r="J35">
         <v>2.8</v>
       </c>
       <c r="K35">
-        <v>30613</v>
+        <v>30158.48</v>
       </c>
       <c r="L35">
         <v>3461.4</v>
       </c>
       <c r="M35">
-        <v>31968.75</v>
+        <v>28.271999999999998</v>
       </c>
       <c r="N35">
-        <v>18688</v>
+        <v>17267.080000000002</v>
       </c>
       <c r="O35">
-        <v>5920</v>
+        <v>12417.745999999999</v>
       </c>
       <c r="P35">
         <v>260997</v>
@@ -7257,13 +7263,13 @@
       <c r="Y35" s="7"/>
       <c r="Z35" s="7"/>
       <c r="AA35" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="AB35" s="7" t="s">
         <v>283</v>
       </c>
-      <c r="AB35" s="7" t="s">
+      <c r="AC35" s="7" t="s">
         <v>284</v>
-      </c>
-      <c r="AC35" s="7" t="s">
-        <v>285</v>
       </c>
       <c r="AD35" s="7" t="s">
         <v>91</v>
@@ -7271,11 +7277,11 @@
       <c r="AE35" s="7"/>
       <c r="AF35" s="7"/>
       <c r="AG35" s="7" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AH35" s="7"/>
       <c r="AI35" s="7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="AJ35" s="7"/>
       <c r="AK35" s="7"/>
@@ -7283,10 +7289,10 @@
     </row>
     <row r="36" spans="1:38" ht="14.5" customHeight="1">
       <c r="A36" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C36" s="5">
         <v>0.5</v>
@@ -7355,7 +7361,7 @@
       <c r="AG36" s="5"/>
       <c r="AH36" s="5"/>
       <c r="AI36" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AJ36" s="5"/>
       <c r="AK36" s="5"/>
@@ -7366,41 +7372,41 @@
         <v>14</v>
       </c>
       <c r="B37" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C37">
-        <v>64866</v>
+        <v>67223.3764402956</v>
       </c>
       <c r="D37">
-        <v>1351500</v>
+        <v>1159359.712230216</v>
       </c>
       <c r="E37">
-        <v>3.5972</v>
+        <v>3.5962000000000001</v>
       </c>
       <c r="G37" s="8"/>
       <c r="H37" s="15">
         <v>83.8</v>
       </c>
       <c r="I37">
-        <v>296</v>
+        <v>310.661</v>
       </c>
       <c r="J37">
         <v>1.85</v>
       </c>
       <c r="K37">
-        <v>20400</v>
+        <v>20539</v>
       </c>
       <c r="L37">
-        <v>2610</v>
+        <v>2673.57</v>
       </c>
       <c r="M37">
-        <v>26.5</v>
+        <v>23.697381126123137</v>
       </c>
       <c r="N37">
-        <v>12700</v>
+        <v>14240.812392276797</v>
       </c>
       <c r="O37">
-        <v>4720</v>
+        <v>4818.7460000000001</v>
       </c>
       <c r="P37">
         <v>294</v>
@@ -7427,13 +7433,13 @@
       </c>
       <c r="Z37" s="7"/>
       <c r="AA37" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="AB37" s="17" t="s">
         <v>289</v>
       </c>
-      <c r="AB37" s="17" t="s">
-        <v>290</v>
-      </c>
       <c r="AC37" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AD37" s="7"/>
       <c r="AE37" s="7"/>
@@ -7442,7 +7448,7 @@
       <c r="AH37" s="7"/>
       <c r="AI37" s="7"/>
       <c r="AJ37" s="7" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="AK37" s="7"/>
       <c r="AL37" s="7"/>
@@ -7452,7 +7458,7 @@
         <v>15</v>
       </c>
       <c r="B38" s="23" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C38" s="5">
         <f>2353/5.1</f>
@@ -7512,10 +7518,10 @@
       <c r="Y38" s="6"/>
       <c r="Z38" s="6"/>
       <c r="AA38" s="6" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="AB38" s="6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="AC38" s="6"/>
       <c r="AD38" s="6" t="s">
@@ -7547,7 +7553,7 @@
         <v>16</v>
       </c>
       <c r="B39" s="23" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C39">
         <f>0.995^0.5</f>
@@ -7613,10 +7619,10 @@
       <c r="Y39" s="7"/>
       <c r="Z39" s="7"/>
       <c r="AA39" s="6" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="AB39" s="7" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="AC39" s="7"/>
       <c r="AD39" s="7" t="s">
@@ -7648,7 +7654,7 @@
         <v>35</v>
       </c>
       <c r="B40" s="23" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C40" s="5">
         <f>39.886/1.93</f>
@@ -7707,10 +7713,10 @@
       <c r="Y40" s="6"/>
       <c r="Z40" s="6"/>
       <c r="AA40" s="6" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="AB40" s="6" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="AC40" s="6"/>
       <c r="AD40" s="6" t="s">
@@ -7742,7 +7748,7 @@
         <v>36</v>
       </c>
       <c r="B41" s="23" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C41">
         <f>0.1332^0.5</f>
@@ -7793,10 +7799,10 @@
         <v>34</v>
       </c>
       <c r="U41" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="V41" s="7" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="W41" s="7" t="s">
         <v>89</v>
@@ -7807,10 +7813,10 @@
       <c r="Y41" s="7"/>
       <c r="Z41" s="7"/>
       <c r="AA41" s="6" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="AB41" s="6" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="AC41" s="7"/>
       <c r="AD41" s="7" t="s">
@@ -7842,7 +7848,7 @@
         <v>37</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C42" s="5">
         <v>1807.7719999999999</v>
@@ -7906,28 +7912,28 @@
       <c r="Y42" s="6"/>
       <c r="Z42" s="6"/>
       <c r="AA42" s="19" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="AB42" s="6"/>
       <c r="AC42" s="19" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="AD42" s="6" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="AE42" s="6"/>
       <c r="AF42" s="35" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="AG42" s="6"/>
       <c r="AH42" s="19" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="AI42" s="6"/>
       <c r="AJ42" s="6"/>
       <c r="AK42" s="6"/>
       <c r="AL42" s="6" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="43" spans="1:38" ht="14.5" customHeight="1">
@@ -7935,7 +7941,7 @@
         <v>124</v>
       </c>
       <c r="B43" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C43">
         <v>706</v>
@@ -7996,22 +8002,22 @@
         <v>126</v>
       </c>
       <c r="AA43" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="AB43" t="s">
         <v>295</v>
       </c>
-      <c r="AB43" t="s">
+      <c r="AC43" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="AD43" t="s">
         <v>296</v>
       </c>
-      <c r="AC43" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="AD43" t="s">
+      <c r="AE43" t="s">
         <v>297</v>
       </c>
-      <c r="AE43" t="s">
-        <v>298</v>
-      </c>
       <c r="AF43" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="AG43" t="s">
         <v>169</v>
@@ -8032,7 +8038,7 @@
         <v>38</v>
       </c>
       <c r="B44" s="23" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C44" s="5">
         <v>0</v>
@@ -8093,10 +8099,10 @@
       <c r="Y44" s="6"/>
       <c r="Z44" s="6"/>
       <c r="AA44" s="6" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="AB44" s="6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="AC44" s="6"/>
       <c r="AD44" s="6" t="s">
@@ -8130,7 +8136,7 @@
         <v>39</v>
       </c>
       <c r="B45" s="23" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C45">
         <v>1</v>
@@ -8188,7 +8194,7 @@
       <c r="Y45" s="7"/>
       <c r="Z45" s="7"/>
       <c r="AA45" s="7" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="AB45" s="6"/>
       <c r="AC45" s="7"/>
@@ -8223,7 +8229,7 @@
         <v>40</v>
       </c>
       <c r="B46" s="23" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C46" s="5">
         <v>0</v>
@@ -8317,7 +8323,7 @@
         <v>41</v>
       </c>
       <c r="B47" s="23" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C47">
         <v>0</v>
@@ -8407,7 +8413,7 @@
         <v>42</v>
       </c>
       <c r="B48" s="23" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C48" s="5">
         <v>0</v>
@@ -9501,20 +9507,20 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7771608-927F-4E4B-98C0-8BD1C2D780A9}">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D31" sqref="D31:E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5" customWidth="1"/>
-    <col min="27" max="27" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5" customWidth="1"/>
+    <col min="26" max="26" width="9.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="B1" t="s">
         <v>176</v>
       </c>
@@ -9522,27 +9528,33 @@
         <v>180</v>
       </c>
       <c r="D1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+        <v>187</v>
+      </c>
+      <c r="F1" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>173</v>
       </c>
       <c r="B2" t="s">
+        <v>316</v>
+      </c>
+      <c r="D2" t="s">
+        <v>436</v>
+      </c>
+      <c r="E2" t="s">
         <v>317</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="E2" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" s="1" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>1991</v>
       </c>
@@ -9553,7 +9565,7 @@
         <v>3.8069431775500351</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>1992</v>
       </c>
@@ -9564,7 +9576,7 @@
         <v>3.9786446316467243</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>1993</v>
       </c>
@@ -9575,7 +9587,7 @@
         <v>3.9840103020872455</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>1994</v>
       </c>
@@ -9586,51 +9598,63 @@
         <v>4.0779095347963734</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>1995</v>
       </c>
       <c r="B7">
         <v>20.6470998551269</v>
       </c>
+      <c r="D7">
+        <v>13.692828189876151</v>
+      </c>
       <c r="E7">
         <v>4.3703385738047968</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>1996</v>
       </c>
       <c r="B8">
         <v>21.808767505499812</v>
       </c>
+      <c r="D8">
+        <v>15.371121003210868</v>
+      </c>
       <c r="E8">
         <v>4.2496109888930622</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>1997</v>
       </c>
       <c r="B9">
         <v>22.672640446423781</v>
       </c>
+      <c r="D9">
+        <v>15.371121003210868</v>
+      </c>
       <c r="E9">
         <v>4.5420400279014865</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>1998</v>
       </c>
       <c r="B10">
         <v>22.358748725653271</v>
       </c>
+      <c r="D10">
+        <v>15.371121003210868</v>
+      </c>
       <c r="E10">
         <v>5.204163760261844</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>1999</v>
       </c>
@@ -9638,13 +9662,16 @@
         <v>23.802114074153568</v>
       </c>
       <c r="D11">
-        <v>17.020807000000001</v>
+        <v>15.787859252467968</v>
       </c>
       <c r="E11">
         <v>4.8720287599935608</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="F11">
+        <v>17.020807000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12">
         <v>2000</v>
       </c>
@@ -9652,13 +9679,16 @@
         <v>25.38766968932768</v>
       </c>
       <c r="D12">
-        <v>18.202192999999998</v>
+        <v>16.754578592581378</v>
       </c>
       <c r="E12">
         <v>4.8505660782314761</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="F12">
+        <v>18.202192999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13">
         <v>2001</v>
       </c>
@@ -9666,13 +9696,16 @@
         <v>23.772602886730695</v>
       </c>
       <c r="D13">
-        <v>19.002631000000001</v>
+        <v>17.185491612221373</v>
       </c>
       <c r="E13">
         <v>5.0705585662928581</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="F13">
+        <v>19.002631000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14">
         <v>2002</v>
       </c>
@@ -9680,13 +9713,16 @@
         <v>23.35944626281054</v>
       </c>
       <c r="D14">
-        <v>18.904408</v>
+        <v>16.85380198526164</v>
       </c>
       <c r="E14">
         <v>5.2932338895745019</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="F14">
+        <v>18.904408</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15">
         <v>2003</v>
       </c>
@@ -9694,13 +9730,16 @@
         <v>23.871867789880344</v>
       </c>
       <c r="D15">
-        <v>18.82685</v>
+        <v>16.930345745329273</v>
       </c>
       <c r="E15">
         <v>5.2583570317111121</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="F15">
+        <v>18.82685</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16">
         <v>2004</v>
       </c>
@@ -9708,13 +9747,16 @@
         <v>23.67333798358105</v>
       </c>
       <c r="D16">
-        <v>19.891030999999998</v>
+        <v>17.395278213888211</v>
       </c>
       <c r="E16">
         <v>5.3307935826581527</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="F16">
+        <v>19.891030999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17">
         <v>2005</v>
       </c>
@@ -9722,13 +9764,16 @@
         <v>25.623759188710629</v>
       </c>
       <c r="D17">
-        <v>20.752817999999998</v>
+        <v>18.140871136028466</v>
       </c>
       <c r="E17">
         <v>5.4568868380104094</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="F17">
+        <v>20.752817999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18">
         <v>2006</v>
       </c>
@@ -9736,13 +9781,16 @@
         <v>24.843054139614743</v>
       </c>
       <c r="D18">
-        <v>20.207038000000001</v>
+        <v>18.240094528708727</v>
       </c>
       <c r="E18">
         <v>5.5561517411600576</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="F18">
+        <v>20.207038000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19">
         <v>2007</v>
       </c>
@@ -9750,13 +9798,16 @@
         <v>24.494285560980845</v>
       </c>
       <c r="D19">
-        <v>20.918483000000002</v>
+        <v>18.928988369317405</v>
       </c>
       <c r="E19">
         <v>5.4783495197724958</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="F19">
+        <v>20.918483000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20">
         <v>2008</v>
       </c>
@@ -9764,13 +9815,16 @@
         <v>24.547942265386059</v>
       </c>
       <c r="D20">
-        <v>21.436884999999997</v>
+        <v>19.410930562335821</v>
       </c>
       <c r="E20">
         <v>5.4193271449267586</v>
       </c>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="F20">
+        <v>21.436884999999997</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21">
         <v>2009</v>
       </c>
@@ -9778,13 +9832,16 @@
         <v>24.995975747169609</v>
       </c>
       <c r="D21">
-        <v>22.324262999999998</v>
+        <v>20.335125591300542</v>
       </c>
       <c r="E21">
         <v>5.3978644631646722</v>
       </c>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="F21">
+        <v>22.324262999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22">
         <v>2010</v>
       </c>
@@ -9792,13 +9849,16 @@
         <v>28.872672640446424</v>
       </c>
       <c r="D22">
-        <v>23.391197999999999</v>
+        <v>21.347204196639218</v>
       </c>
       <c r="E22">
         <v>6.1383269839566461</v>
       </c>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="F22">
+        <v>23.391197999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23">
         <v>2011</v>
       </c>
@@ -9806,13 +9866,16 @@
         <v>28.046359392606107</v>
       </c>
       <c r="D23">
-        <v>23.379133999999997</v>
+        <v>21.548485936076322</v>
       </c>
       <c r="E23">
         <v>7.0156141009819182</v>
       </c>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="F23">
+        <v>23.379133999999997</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24">
         <v>2012</v>
       </c>
@@ -9820,13 +9883,16 @@
         <v>28.124161613993667</v>
       </c>
       <c r="D24">
-        <v>25.035924999999999</v>
+        <v>22.56339949549157</v>
       </c>
       <c r="E24">
         <v>6.8546439877662708</v>
       </c>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="F24">
+        <v>25.035924999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25">
         <v>2013</v>
       </c>
@@ -9834,13 +9900,16 @@
         <v>28.738530879433384</v>
       </c>
       <c r="D25">
-        <v>25.961294000000002</v>
+        <v>23.963866809321551</v>
       </c>
       <c r="E25">
         <v>5.1698234694425063</v>
       </c>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="F25">
+        <v>25.961294000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26">
         <v>2014</v>
       </c>
@@ -9848,13 +9917,16 @@
         <v>28.486344368728872</v>
       </c>
       <c r="D26">
-        <v>27.434650000000001</v>
+        <v>25.007129909502595</v>
       </c>
       <c r="E26">
         <v>4.6949616354563499</v>
       </c>
-    </row>
-    <row r="27" spans="1:5">
+      <c r="F26">
+        <v>27.434650000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27">
         <v>2015</v>
       </c>
@@ -9862,13 +9934,16 @@
         <v>28.717068197671303</v>
       </c>
       <c r="D27">
-        <v>28.143955999999999</v>
+        <v>25.426703112836272</v>
       </c>
       <c r="E27">
         <v>4.4669206417341849</v>
       </c>
-    </row>
-    <row r="28" spans="1:5">
+      <c r="F27">
+        <v>28.143955999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28">
         <v>2016</v>
       </c>
@@ -9876,13 +9951,16 @@
         <v>27.520523689434992</v>
       </c>
       <c r="D28">
-        <v>28.132810000000003</v>
+        <v>25.514586689210219</v>
       </c>
       <c r="E28">
         <v>4.4132639373289697</v>
       </c>
-    </row>
-    <row r="29" spans="1:5">
+      <c r="F28">
+        <v>28.132810000000003</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29">
         <v>2017</v>
       </c>
@@ -9890,13 +9968,16 @@
         <v>27.702956484412727</v>
       </c>
       <c r="D29">
-        <v>27.218978</v>
+        <v>24.485498359412073</v>
       </c>
       <c r="E29">
         <v>4.5017974995975756</v>
       </c>
-    </row>
-    <row r="30" spans="1:5">
+      <c r="F29">
+        <v>27.218978</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30">
         <v>2018</v>
       </c>
@@ -9904,13 +9985,16 @@
         <v>26.943714117078926</v>
       </c>
       <c r="D30">
-        <v>28.006637999999999</v>
+        <v>24.102779559073923</v>
       </c>
       <c r="E30">
         <v>4.5017974995975756</v>
       </c>
-    </row>
-    <row r="31" spans="1:5">
+      <c r="F30">
+        <v>28.006637999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31">
         <v>2019</v>
       </c>
@@ -9918,13 +10002,16 @@
         <v>26.704941782475718</v>
       </c>
       <c r="D31">
-        <v>28.35378</v>
+        <v>23.697381126123137</v>
       </c>
       <c r="E31">
         <v>4.5742340505446153</v>
       </c>
-    </row>
-    <row r="32" spans="1:5">
+      <c r="F31">
+        <v>28.35378</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32">
         <v>2020</v>
       </c>
@@ -9932,10 +10019,13 @@
         <v>25.846434511992275</v>
       </c>
       <c r="D32">
-        <v>24.563119999999998</v>
+        <v>22.143826292157893</v>
       </c>
       <c r="E32">
         <v>4.885442936094865</v>
+      </c>
+      <c r="F32">
+        <v>24.563119999999998</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -9945,6 +10035,9 @@
       <c r="B33">
         <v>28.142941460535493</v>
       </c>
+      <c r="D33">
+        <v>23.320332233938142</v>
+      </c>
       <c r="E33">
         <v>5.2637227021516342</v>
       </c>
@@ -9955,6 +10048,9 @@
       </c>
       <c r="B34">
         <v>29.55947845683318</v>
+      </c>
+      <c r="D34">
+        <v>23.904332773713399</v>
       </c>
       <c r="E34">
         <v>4.8425175725706922</v>
@@ -9972,7 +10068,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -9985,22 +10081,22 @@
         <v>180</v>
       </c>
       <c r="D1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F1" t="s">
         <v>176</v>
       </c>
       <c r="G1" t="s">
+        <v>428</v>
+      </c>
+      <c r="H1" t="s">
+        <v>427</v>
+      </c>
+      <c r="I1" t="s">
         <v>429</v>
-      </c>
-      <c r="H1" t="s">
-        <v>428</v>
-      </c>
-      <c r="I1" t="s">
-        <v>430</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -10008,25 +10104,25 @@
         <v>173</v>
       </c>
       <c r="B2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D2" t="s">
+        <v>430</v>
+      </c>
+      <c r="E2" t="s">
         <v>431</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>432</v>
       </c>
-      <c r="F2" t="s">
-        <v>433</v>
-      </c>
       <c r="G2" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="H2" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="I2" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="16">
@@ -10607,7 +10703,7 @@
   <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -10623,10 +10719,10 @@
         <v>180</v>
       </c>
       <c r="D1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -10634,22 +10730,22 @@
         <v>173</v>
       </c>
       <c r="B2" t="s">
+        <v>319</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="E2" t="s">
+        <v>322</v>
+      </c>
+      <c r="H2" t="s">
+        <v>321</v>
+      </c>
+      <c r="I2" t="s">
+        <v>182</v>
+      </c>
+      <c r="J2" t="s">
         <v>320</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="E2" t="s">
-        <v>323</v>
-      </c>
-      <c r="H2" t="s">
-        <v>322</v>
-      </c>
-      <c r="I2" t="s">
-        <v>183</v>
-      </c>
-      <c r="J2" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -10821,7 +10917,7 @@
         <v>3649</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:6">
       <c r="A17">
         <v>2004</v>
       </c>
@@ -10835,7 +10931,7 @@
         <v>3746</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:6">
       <c r="A18">
         <v>2005</v>
       </c>
@@ -10849,7 +10945,7 @@
         <v>4316.50818139284</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:6">
       <c r="A19">
         <v>2006</v>
       </c>
@@ -10863,7 +10959,7 @@
         <v>4854.7482013480203</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:6">
       <c r="A20">
         <v>2007</v>
       </c>
@@ -10877,7 +10973,7 @@
         <v>5198.2613767341099</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:6">
       <c r="A21">
         <v>2008</v>
       </c>
@@ -10891,7 +10987,7 @@
         <v>5444.4611366192803</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:6">
       <c r="A22">
         <v>2009</v>
       </c>
@@ -10905,7 +11001,7 @@
         <v>5812.6119620613499</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:6">
       <c r="A23">
         <v>2010</v>
       </c>
@@ -10919,7 +11015,7 @@
         <v>6083.0428684506496</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:6">
       <c r="A24">
         <v>2011</v>
       </c>
@@ -10933,7 +11029,7 @@
         <v>5963.3187353952198</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:6">
       <c r="A25">
         <v>2012</v>
       </c>
@@ -10947,7 +11043,7 @@
         <v>6209.4124508755604</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:6">
       <c r="A26">
         <v>2013</v>
       </c>
@@ -10961,7 +11057,7 @@
         <v>6357.9806620453201</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:6">
       <c r="A27">
         <v>2014</v>
       </c>
@@ -10975,7 +11071,7 @@
         <v>6335.9057517727697</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:6">
       <c r="A28">
         <v>2015</v>
       </c>
@@ -10989,7 +11085,7 @@
         <v>6581.9287709832197</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:6">
       <c r="A29">
         <v>2016</v>
       </c>
@@ -11003,7 +11099,7 @@
         <v>7169.52081815783</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:6">
       <c r="A30">
         <v>2017</v>
       </c>
@@ -11017,7 +11113,7 @@
         <v>7269.2732549698803</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:6">
       <c r="A31">
         <v>2018</v>
       </c>
@@ -11031,7 +11127,7 @@
         <v>7674</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:6">
       <c r="A32">
         <v>2019</v>
       </c>
@@ -11043,6 +11139,10 @@
       </c>
       <c r="E32" s="34">
         <v>7599</v>
+      </c>
+      <c r="F32">
+        <f>SUM(D32:E32)</f>
+        <v>12417.745999999999</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -11093,10 +11193,10 @@
         <v>180</v>
       </c>
       <c r="D1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -11105,7 +11205,7 @@
       </c>
       <c r="B2" s="1"/>
       <c r="D2" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="16">
@@ -11308,10 +11408,10 @@
         <v>180</v>
       </c>
       <c r="D1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -11320,7 +11420,7 @@
       </c>
       <c r="B2" s="1"/>
       <c r="D2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="16">
@@ -11505,7 +11605,7 @@
         <v>180</v>
       </c>
       <c r="E1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -11513,16 +11613,16 @@
         <v>173</v>
       </c>
       <c r="B2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C2" t="s">
         <v>194</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>195</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>196</v>
-      </c>
-      <c r="E2" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -11856,7 +11956,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="D21" activeCellId="1" sqref="F21 D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -11876,13 +11976,13 @@
         <v>180</v>
       </c>
       <c r="D1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E1" t="s">
         <v>177</v>
       </c>
       <c r="F1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -11893,16 +11993,16 @@
         <v>179</v>
       </c>
       <c r="C2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D2" t="s">
-        <v>181</v>
+        <v>434</v>
       </c>
       <c r="E2" t="s">
         <v>178</v>
       </c>
       <c r="F2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="16">
@@ -12335,7 +12435,7 @@
   <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E21"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -12355,16 +12455,16 @@
         <v>180</v>
       </c>
       <c r="D1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F1" t="s">
         <v>182</v>
       </c>
-      <c r="E1" t="s">
-        <v>188</v>
-      </c>
-      <c r="F1" t="s">
-        <v>183</v>
-      </c>
       <c r="G1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="2" spans="1:14">
@@ -12372,19 +12472,19 @@
         <v>173</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="G2" t="s">
         <v>185</v>
-      </c>
-      <c r="C2" t="s">
-        <v>190</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="G2" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="16">
@@ -12924,7 +13024,7 @@
   <dimension ref="A1:Q41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -12941,19 +13041,19 @@
         <v>180</v>
       </c>
       <c r="D1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F1" t="s">
         <v>182</v>
       </c>
-      <c r="E1" t="s">
-        <v>188</v>
-      </c>
-      <c r="F1" t="s">
-        <v>183</v>
-      </c>
       <c r="G1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="L1" t="s">
         <v>180</v>
@@ -12962,7 +13062,7 @@
         <v>180</v>
       </c>
       <c r="Q1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="2" spans="1:17">
@@ -12970,29 +13070,29 @@
         <v>173</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="H2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="L2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="M2" s="32"/>
       <c r="Q2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -13691,19 +13791,19 @@
         <v>180</v>
       </c>
       <c r="D1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="K1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="L1" t="s">
+        <v>413</v>
+      </c>
+      <c r="M1" t="s">
         <v>414</v>
-      </c>
-      <c r="M1" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -13712,7 +13812,7 @@
       </c>
       <c r="B2" s="1"/>
       <c r="D2" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="J2">
         <v>1990</v>
@@ -14299,7 +14399,7 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="D32" sqref="D32:E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -14312,10 +14412,10 @@
         <v>180</v>
       </c>
       <c r="D1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -14323,7 +14423,7 @@
         <v>173</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D2" s="1"/>
     </row>
@@ -14815,10 +14915,10 @@
         <v>180</v>
       </c>
       <c r="D1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -14826,7 +14926,7 @@
         <v>173</v>
       </c>
       <c r="B2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D2" s="1"/>
     </row>
@@ -15248,8 +15348,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A70BBC54-9A6A-4436-A684-DF848EF748EA}">
   <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E71" sqref="D71:E71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -15262,10 +15362,10 @@
         <v>180</v>
       </c>
       <c r="D1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -15273,13 +15373,13 @@
         <v>173</v>
       </c>
       <c r="B2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -16081,7 +16181,7 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -16094,10 +16194,10 @@
         <v>180</v>
       </c>
       <c r="D1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -16105,13 +16205,13 @@
         <v>173</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="16">

</xml_diff>

<commit_message>
Run scenarios from an excel file
- updated functions such that the "Scenario setup.xlsx" excel file can be used to implement nearly any hyperparameter change in nearly any year
- this includes updating the initial operating mine pool and the incentive mine pool, using the load_mine_data hyperparameter, with an example file "load_mine_data.xlsx" included in this commit
- find more details about implementation and usage in the "Scenario setup.xlsx" excel file.
</commit_message>
<xml_diff>
--- a/data/case study data.xlsx
+++ b/data/case study data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnryter/Dropbox (MIT)/John MIT/Research/generalizationOutside/generalization/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CB7EB22-57F3-574B-861B-1AA5EDED6767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74E397BB-CDF7-A34A-B547-53BAF10DB111}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" activeTab="8" xr2:uid="{9C1DBEC5-9C42-494B-AEAA-1D89B674AD0D}"/>
   </bookViews>
@@ -4312,8 +4312,8 @@
   <dimension ref="A1:AN79"/>
   <sheetViews>
     <sheetView zoomScale="114" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S11" sqref="S11"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -15091,7 +15091,7 @@
   <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -18004,7 +18004,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A70BBC54-9A6A-4436-A684-DF848EF748EA}">
   <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E71" sqref="D71:E71"/>
     </sheetView>
   </sheetViews>
@@ -18837,7 +18837,7 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="I10" sqref="I10:I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>

</xml_diff>